<commit_message>
all but one configuration tests pass
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC9A110-EF6F-7F49-949B-5E2E2BDC9F41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD378CCC-D934-8240-A827-3740C9E2341C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="26940" windowHeight="21040" activeTab="4" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="26940" windowHeight="21040" firstSheet="2" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2131" uniqueCount="190">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -348,9 +348,6 @@
     <t>:donor-smokes</t>
   </si>
   <si>
-    <t>:type-d-gp</t>
-  </si>
-  <si>
     <t>:post-transplant</t>
   </si>
   <si>
@@ -613,6 +610,9 @@
   </si>
   <si>
     <t>{:dps 2,  :max 5, :min 0, :type :numeric}</t>
+  </si>
+  <si>
+    <t>unit</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1222,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="1"/>
     </row>
@@ -1262,7 +1262,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9" s="1"/>
     </row>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -1298,19 +1298,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
@@ -1406,104 +1406,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="37" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="37" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" s="37" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D4" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="37" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1535,13 +1535,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1549,32 +1549,32 @@
         <v>80</v>
       </c>
       <c r="B2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" t="s">
         <v>167</v>
-      </c>
-      <c r="C2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" t="s">
         <v>169</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>170</v>
-      </c>
-      <c r="C4" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1586,7 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:J3206"/>
   <sheetViews>
-    <sheetView topLeftCell="A1330" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1360" sqref="J1360"/>
     </sheetView>
   </sheetViews>
@@ -1628,7 +1628,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>9</v>
@@ -31854,8 +31854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA849B77-A729-9F4B-AFFB-4400AE5F1FC9}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -31893,8 +31893,8 @@
       <c r="A4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>148</v>
+      <c r="B4" s="35" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -31942,7 +31942,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -31950,7 +31950,7 @@
         <v>68</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -31962,8 +31962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:F28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -31991,10 +31991,10 @@
         <v>23</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>144</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>145</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>24</v>
@@ -32012,7 +32012,7 @@
         <v>28</v>
       </c>
       <c r="J1" s="39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K1" s="34"/>
     </row>
@@ -32102,7 +32102,7 @@
         <v>0.81245999999999996</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H5" s="14"/>
       <c r="I5" s="11" t="s">
@@ -32130,7 +32130,7 @@
         <v>0.48838999999999999</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -32147,7 +32147,7 @@
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7">
         <v>-0.4007</v>
@@ -32156,7 +32156,7 @@
         <v>1.0520099999999999</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -32182,7 +32182,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -32205,13 +32205,13 @@
         <v>64</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C10" s="63" t="s">
         <v>49</v>
       </c>
       <c r="D10" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -32220,7 +32220,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
@@ -32235,11 +32235,11 @@
         <v>64</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C11" s="63"/>
       <c r="D11" s="53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11">
         <v>-0.11611</v>
@@ -32248,7 +32248,7 @@
         <v>0.21751999999999999</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -32261,11 +32261,11 @@
         <v>64</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E12">
         <v>-3.6799999999999999E-2</v>
@@ -32274,7 +32274,7 @@
         <v>0.46777000000000002</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -32364,7 +32364,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>52</v>
@@ -32394,7 +32394,7 @@
         <v>67</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="51" t="s">
@@ -32420,7 +32420,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="51" t="s">
@@ -32446,7 +32446,7 @@
         <v>67</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="51" t="s">
@@ -32485,7 +32485,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D22" s="51" t="s">
         <v>44</v>
@@ -32658,17 +32658,19 @@
         <v>14</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C30" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="58"/>
+      <c r="D30" s="58" t="s">
+        <v>189</v>
+      </c>
       <c r="G30" s="48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I30" s="33"/>
       <c r="J30" s="33"/>
@@ -32689,7 +32691,7 @@
         <v>-1.0919999999999999E-2</v>
       </c>
       <c r="G31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H31" s="11"/>
       <c r="I31" s="33"/>
@@ -32711,7 +32713,7 @@
         <v>1.24E-3</v>
       </c>
       <c r="G32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H32" s="11"/>
       <c r="I32" s="34"/>
@@ -32735,7 +32737,7 @@
         <v>-4.0000000000000001E-3</v>
       </c>
       <c r="G33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="33"/>
@@ -32782,7 +32784,9 @@
       <c r="C36" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="47"/>
+      <c r="D36" s="58" t="s">
+        <v>189</v>
+      </c>
       <c r="E36" s="59">
         <v>0.14069000000000001</v>
       </c>
@@ -32790,10 +32794,10 @@
         <v>-0.30773</v>
       </c>
       <c r="G36" s="61" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I36" s="11"/>
       <c r="J36" s="40">
@@ -32821,7 +32825,9 @@
       <c r="C38" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D38" s="47"/>
+      <c r="D38" s="58" t="s">
+        <v>189</v>
+      </c>
       <c r="E38" s="22">
         <v>-3.81E-3</v>
       </c>
@@ -32829,10 +32835,10 @@
         <v>-4.5879999999999997E-2</v>
       </c>
       <c r="G38" s="61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I38" s="11"/>
       <c r="J38" s="40">
@@ -32883,7 +32889,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F1" s="7"/>
     </row>
@@ -40709,10 +40715,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBA40B-94B1-B140-8D57-D55E3398F15E}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -40750,7 +40756,7 @@
         <v>64</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -40758,7 +40764,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -40779,7 +40785,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>91</v>
@@ -40803,7 +40809,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="11">
         <v>4.9000000000000004</v>
@@ -40814,23 +40820,15 @@
         <v>2</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="38" t="s">
-        <v>101</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -40842,7 +40840,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -40867,13 +40865,13 @@
         <v>23</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>145</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>26</v>
@@ -40885,7 +40883,7 @@
         <v>28</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J1" s="10" t="s">
         <v>29</v>
@@ -40908,10 +40906,10 @@
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I2" s="41">
         <v>2.2999999999999998</v>
@@ -40966,13 +40964,13 @@
         <v>32</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I5" s="41">
         <v>2.1</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -40993,7 +40991,7 @@
         <v>2.1</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -41010,19 +41008,19 @@
         <v>64</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" s="64" t="s">
         <v>84</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I8" s="41">
         <v>1.4</v>
@@ -41034,11 +41032,11 @@
         <v>64</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="64"/>
       <c r="D9" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9">
         <v>0.28171000000000002</v>
@@ -41053,11 +41051,11 @@
         <v>64</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E10">
         <v>0.48797000000000001</v>
@@ -41081,7 +41079,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>85</v>
@@ -41093,7 +41091,7 @@
         <v>6.3950000000000007E-2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I12" s="41">
         <v>1.6</v>
@@ -41105,7 +41103,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="27"/>
       <c r="D13" s="11" t="s">
@@ -41145,7 +41143,7 @@
         <v>-0.65693000000000001</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G15" s="14"/>
       <c r="I15" s="41">
@@ -41227,24 +41225,26 @@
         <v>14</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="28"/>
+      <c r="D20" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="E20"/>
       <c r="F20" s="48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I20" s="41">
         <v>1.2</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -41259,7 +41259,7 @@
         <v>-5.5210000000000002E-2</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I21" s="41"/>
       <c r="J21" s="9"/>
@@ -41277,7 +41277,7 @@
         <v>1.5100000000000001E-3</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I22" s="41"/>
       <c r="J22" s="9"/>
@@ -41295,7 +41295,7 @@
         <v>-2.82E-3</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I23" s="41"/>
       <c r="J23" s="9"/>
@@ -41311,7 +41311,7 @@
     </row>
     <row r="25" spans="1:10" ht="46" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>77</v>
@@ -41319,12 +41319,14 @@
       <c r="C25" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="29"/>
+      <c r="D25" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="E25">
         <v>9.7850000000000006E-2</v>
       </c>
       <c r="F25" s="48" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I25" s="41">
         <v>2.2000000000000002</v>
@@ -41351,15 +41353,17 @@
       <c r="C27" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="E27">
         <v>-1.966E-2</v>
       </c>
       <c r="F27" s="55" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I27" s="41">
         <v>1.5</v>
@@ -41385,15 +41389,17 @@
       <c r="C29" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="E29">
         <v>1.32E-3</v>
       </c>
       <c r="F29" s="48" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I29" s="41">
         <v>1.1000000000000001</v>
@@ -41411,7 +41417,7 @@
     </row>
     <row r="31" spans="1:10" ht="31" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B31" s="13" t="s">
         <v>77</v>
@@ -41419,15 +41425,17 @@
       <c r="C31" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="29"/>
+      <c r="D31" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="E31">
         <v>-3.5779999999999999E-2</v>
       </c>
       <c r="F31" s="48" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I31" s="41">
         <v>2.4</v>
@@ -41457,7 +41465,7 @@
       <c r="E34" s="30"/>
       <c r="I34" s="41"/>
       <c r="J34" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
First trework after receiving lung R code: calculating S0-outcome...
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2906CFF6-7ED5-EB4C-B7BE-7D7FD31D388F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D7337A-A446-644B-9DD3-318C8F138F6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52840" yWindow="800" windowWidth="26940" windowHeight="21040" activeTab="4" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="52740" yWindow="800" windowWidth="28320" windowHeight="21040" activeTab="4" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="waiting-baseline-cifs" sheetId="6" r:id="rId4"/>
     <sheet name="waiting-baseline-vars" sheetId="4" r:id="rId5"/>
     <sheet name="waiting-inputs" sheetId="5" r:id="rId6"/>
-    <sheet name="post-transplant-baseline-cifs" sheetId="9" r:id="rId7"/>
-    <sheet name="post-transplant-baseline-vars" sheetId="10" r:id="rId8"/>
-    <sheet name="post-transplant-inputs" sheetId="11" r:id="rId9"/>
-    <sheet name="Average donor values by centre" sheetId="17" r:id="rId10"/>
+    <sheet name="waiting-results" sheetId="20" r:id="rId7"/>
+    <sheet name="post-transplant-baseline-cifs" sheetId="9" r:id="rId8"/>
+    <sheet name="post-transplant-baseline-vars" sheetId="10" r:id="rId9"/>
+    <sheet name="post-transplant-inputs" sheetId="11" r:id="rId10"/>
+    <sheet name="Average donor values by centre" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="196">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -590,6 +591,48 @@
   <si>
     <t>unit</t>
   </si>
+  <si>
+    <t>:chart</t>
+  </si>
+  <si>
+    <t>:area</t>
+  </si>
+  <si>
+    <t>:icons</t>
+  </si>
+  <si>
+    <t>:table</t>
+  </si>
+  <si>
+    <t>:text</t>
+  </si>
+  <si>
+    <t>:transplant</t>
+  </si>
+  <si>
+    <t>:death</t>
+  </si>
+  <si>
+    <t>Died</t>
+  </si>
+  <si>
+    <t>Still waiting</t>
+  </si>
+  <si>
+    <t>Transplanted</t>
+  </si>
+  <si>
+    <t>:tab-key</t>
+  </si>
+  <si>
+    <t>:bar-label</t>
+  </si>
+  <si>
+    <t>:bar-ciff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[:+  (get cifs :transplant) (get cifs :death)) </t>
+  </si>
 </sst>
 </file>
 
@@ -710,7 +753,7 @@
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -861,6 +904,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1254,6 +1300,730 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
+  <dimension ref="A1:J55"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
+    <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="10" max="10" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="40">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3">
+        <v>0.28404000000000001</v>
+      </c>
+      <c r="I3" s="40">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="10"/>
+      <c r="E4"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="8"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I5" s="40">
+        <v>2.1</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>0.23224</v>
+      </c>
+      <c r="I6" s="40">
+        <v>2.1</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="10"/>
+      <c r="E7"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="8"/>
+    </row>
+    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I8" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="62"/>
+      <c r="D9" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9">
+        <v>0.28171000000000002</v>
+      </c>
+      <c r="I9" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E10">
+        <v>0.48797000000000001</v>
+      </c>
+      <c r="I10" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="10"/>
+      <c r="E11"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12">
+        <v>6.3950000000000007E-2</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I12" s="40">
+        <v>1.6</v>
+      </c>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" s="26"/>
+      <c r="D13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="40">
+        <v>1.6</v>
+      </c>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="10"/>
+      <c r="E14"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15">
+        <v>-0.65693000000000001</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="I15" s="40">
+        <v>1.7</v>
+      </c>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="26"/>
+      <c r="D16" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>0.17297000000000001</v>
+      </c>
+      <c r="G16" s="10"/>
+      <c r="I16" s="40">
+        <v>1.7</v>
+      </c>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17">
+        <v>-1.486E-2</v>
+      </c>
+      <c r="G17" s="10"/>
+      <c r="I17" s="40">
+        <v>1.7</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10"/>
+      <c r="I18" s="40">
+        <v>1.7</v>
+      </c>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="10"/>
+      <c r="E19"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="76" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20" s="40">
+        <v>1.2</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="27"/>
+      <c r="E21">
+        <v>-5.5210000000000002E-2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I21" s="40"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="31"/>
+      <c r="D22" s="27"/>
+      <c r="E22">
+        <v>1.5100000000000001E-3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="40"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="27"/>
+      <c r="E23">
+        <v>-2.82E-3</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" s="40"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="46" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25">
+        <v>9.7850000000000006E-2</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="I25" s="40">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="11"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="28"/>
+      <c r="E26"/>
+      <c r="F26" s="47"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="46" x14ac:dyDescent="0.2">
+      <c r="A27" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E27">
+        <v>-1.966E-2</v>
+      </c>
+      <c r="F27" s="53" t="s">
+        <v>176</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I27" s="40">
+        <v>1.5</v>
+      </c>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="10"/>
+      <c r="E28"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" ht="46" x14ac:dyDescent="0.2">
+      <c r="A29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E29">
+        <v>1.32E-3</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I29" s="40">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="10"/>
+      <c r="E30"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="8"/>
+    </row>
+    <row r="31" spans="1:10" ht="31" x14ac:dyDescent="0.2">
+      <c r="A31" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31">
+        <v>-3.5779999999999999E-2</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I31" s="40">
+        <v>2.4</v>
+      </c>
+      <c r="J31" s="8"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="E32" s="29"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="29"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="8"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="62"/>
+      <c r="E34" s="29"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="62"/>
+      <c r="E35" s="29"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="8"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="E36" s="30"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="8"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="E37" s="30"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+      <c r="E38" s="30"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
+      <c r="E39" s="30"/>
+      <c r="I39" s="40"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="E40" s="30"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="E41" s="30"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="8"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="E43" s="10"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="E47" s="27"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E49" s="10"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E50" s="10"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E51" s="27"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E55" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C34:C35"/>
+  </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C3A71E-E042-8B43-861F-B74ED9AFD679}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -1492,20 +2262,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="113" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>113</v>
       </c>
@@ -1515,8 +2285,26 @@
       <c r="C1" s="24" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>75</v>
       </c>
@@ -1526,8 +2314,9 @@
       <c r="C2" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="63"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>96</v>
       </c>
@@ -1538,7 +2327,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>163</v>
       </c>
@@ -1558,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:D3206"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:J1048576"/>
+    <sheetView topLeftCell="A1340" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -26409,7 +27198,7 @@
         <v>63</v>
       </c>
       <c r="B11" s="14">
-        <v>23.022400000000001</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -26422,7 +27211,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -27308,6 +28097,66 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA7EBA2-FAD6-B44A-8567-0E4410E5B4BD}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView zoomScale="99" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>191</v>
+      </c>
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FE1BB-1AC5-6D40-AB0F-F4D73062F511}">
   <dimension ref="A1:N1015"/>
   <sheetViews>
@@ -35165,7 +36014,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBA40B-94B1-B140-8D57-D55E3398F15E}">
   <dimension ref="A1:B19"/>
   <sheetViews>
@@ -35285,728 +36134,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:J55"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
-    <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="41" t="s">
-        <v>111</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I2" s="40">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3">
-        <v>0.28404000000000001</v>
-      </c>
-      <c r="I3" s="40">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="10"/>
-      <c r="E4"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="40">
-        <v>2.1</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6">
-        <v>0.23224</v>
-      </c>
-      <c r="I6" s="40">
-        <v>2.1</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="10"/>
-      <c r="E7"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C8" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I8" s="40">
-        <v>1.4</v>
-      </c>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9">
-        <v>0.28171000000000002</v>
-      </c>
-      <c r="I9" s="40">
-        <v>1.4</v>
-      </c>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="E10">
-        <v>0.48797000000000001</v>
-      </c>
-      <c r="I10" s="40">
-        <v>1.4</v>
-      </c>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="10"/>
-      <c r="E11"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E12">
-        <v>6.3950000000000007E-2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I12" s="40">
-        <v>1.6</v>
-      </c>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="40">
-        <v>1.6</v>
-      </c>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="10"/>
-      <c r="E14"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15">
-        <v>-0.65693000000000001</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="I15" s="40">
-        <v>1.7</v>
-      </c>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16">
-        <v>0.17297000000000001</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="I16" s="40">
-        <v>1.7</v>
-      </c>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17">
-        <v>-1.486E-2</v>
-      </c>
-      <c r="G17" s="10"/>
-      <c r="I17" s="40">
-        <v>1.7</v>
-      </c>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10"/>
-      <c r="I18" s="40">
-        <v>1.7</v>
-      </c>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="10"/>
-      <c r="E19"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" ht="76" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E20"/>
-      <c r="F20" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I20" s="40">
-        <v>1.2</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="27"/>
-      <c r="E21">
-        <v>-5.5210000000000002E-2</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I21" s="40"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="27"/>
-      <c r="E22">
-        <v>1.5100000000000001E-3</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I22" s="40"/>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="27"/>
-      <c r="E23">
-        <v>-2.82E-3</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I23" s="40"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
-      <c r="E24"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" ht="46" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E25">
-        <v>9.7850000000000006E-2</v>
-      </c>
-      <c r="F25" s="47" t="s">
-        <v>177</v>
-      </c>
-      <c r="I25" s="40">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="28"/>
-      <c r="E26"/>
-      <c r="F26" s="47"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:10" ht="46" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E27">
-        <v>-1.966E-2</v>
-      </c>
-      <c r="F27" s="53" t="s">
-        <v>176</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="I27" s="40">
-        <v>1.5</v>
-      </c>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="10"/>
-      <c r="E28"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" ht="46" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E29">
-        <v>1.32E-3</v>
-      </c>
-      <c r="F29" s="47" t="s">
-        <v>176</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="I29" s="40">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="10"/>
-      <c r="E30"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="1:10" ht="31" x14ac:dyDescent="0.2">
-      <c r="A31" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E31">
-        <v>-3.5779999999999999E-2</v>
-      </c>
-      <c r="F31" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I31" s="40">
-        <v>2.4</v>
-      </c>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="E32" s="29"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="29"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="62"/>
-      <c r="E34" s="29"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="62"/>
-      <c r="E35" s="29"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="E36" s="30"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="E37" s="30"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="E38" s="30"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="E39" s="30"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="E40" s="30"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="E41" s="30"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E43" s="10"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E47" s="27"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E51" s="27"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E53" s="10"/>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E55" s="27"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C34:C35"/>
-  </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Working on text and vis configurations
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8606DD97-8CB9-6B4F-BD9D-B75EE7C5898E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACB3E72-AE9D-DC44-84B4-0397E42A9CF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52740" yWindow="4180" windowWidth="28320" windowHeight="21040" activeTab="3" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="57760" yWindow="4180" windowWidth="28320" windowHeight="21040" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -18,13 +18,12 @@
     <sheet name="tools" sheetId="16" r:id="rId3"/>
     <sheet name="waiting-baseline-cifs" sheetId="6" r:id="rId4"/>
     <sheet name="waiting-baseline-vars" sheetId="4" r:id="rId5"/>
-    <sheet name="waiting-meta" sheetId="21" r:id="rId6"/>
-    <sheet name="waiting-inputs" sheetId="5" r:id="rId7"/>
-    <sheet name="waiting-results" sheetId="20" r:id="rId8"/>
-    <sheet name="post-transplant-baseline-cifs" sheetId="9" r:id="rId9"/>
-    <sheet name="post-transplant-baseline-vars" sheetId="10" r:id="rId10"/>
-    <sheet name="post-transplant-inputs" sheetId="11" r:id="rId11"/>
-    <sheet name="Average donor values by centre" sheetId="17" r:id="rId12"/>
+    <sheet name="waiting-inputs" sheetId="5" r:id="rId6"/>
+    <sheet name="waiting-results" sheetId="20" r:id="rId7"/>
+    <sheet name="post-transplant-baseline-cifs" sheetId="9" r:id="rId8"/>
+    <sheet name="post-transplant-baseline-vars" sheetId="10" r:id="rId9"/>
+    <sheet name="post-transplant-inputs" sheetId="11" r:id="rId10"/>
+    <sheet name="Average donor values by centre" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="189">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -587,21 +586,6 @@
     <t>unit</t>
   </si>
   <si>
-    <t>:chart</t>
-  </si>
-  <si>
-    <t>:area</t>
-  </si>
-  <si>
-    <t>:icons</t>
-  </si>
-  <si>
-    <t>:table</t>
-  </si>
-  <si>
-    <t>:text</t>
-  </si>
-  <si>
     <t>:transplant</t>
   </si>
   <si>
@@ -627,18 +611,6 @@
   </si>
   <si>
     <t xml:space="preserve">[:+  (get cifs :transplant) (get cifs :death)) </t>
-  </si>
-  <si>
-    <t>:vis</t>
-  </si>
-  <si>
-    <t>bars</t>
-  </si>
-  <si>
-    <t>labels</t>
-  </si>
-  <si>
-    <t>:meta-key</t>
   </si>
 </sst>
 </file>
@@ -1307,128 +1279,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBA40B-94B1-B140-8D57-D55E3398F15E}">
-  <dimension ref="A1:B19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="10">
-        <v>2.0499999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="37" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="10">
-        <v>4.9000000000000004</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-      <c r="B19" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:J55"/>
   <sheetViews>
@@ -2152,7 +2002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C3A71E-E042-8B43-861F-B74ED9AFD679}">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2391,10 +2241,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2404,7 +2254,7 @@
     <col min="3" max="3" width="47.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>111</v>
       </c>
@@ -2414,26 +2264,8 @@
       <c r="C1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>73</v>
       </c>
@@ -2445,7 +2277,7 @@
       </c>
       <c r="D2" s="61"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>94</v>
       </c>
@@ -2456,7 +2288,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>161</v>
       </c>
@@ -2476,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:D3206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2497,10 +2329,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -27336,40 +27168,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35818A6-BD30-394E-9378-0FA508C9E15F}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M37"/>
   <sheetViews>
@@ -28259,7 +28057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA7EBA2-FAD6-B44A-8567-0E4410E5B4BD}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -28274,44 +28072,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C1" t="s">
         <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -28319,7 +28117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FE1BB-1AC5-6D40-AB0F-F4D73062F511}">
   <dimension ref="A1:N1015"/>
   <sheetViews>
@@ -36175,4 +35973,126 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBA40B-94B1-B140-8D57-D55E3398F15E}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fills and legends created from metadata
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACB3E72-AE9D-DC44-84B4-0397E42A9CF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8A1C38-0AE1-A048-B2BF-FADED1058A80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57760" yWindow="4180" windowWidth="28320" windowHeight="21040" activeTab="2" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="57760" yWindow="4180" windowWidth="28320" windowHeight="21040" firstSheet="1" activeTab="3" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="191">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -611,6 +611,12 @@
   </si>
   <si>
     <t xml:space="preserve">[:+  (get cifs :transplant) (get cifs :death)) </t>
+  </si>
+  <si>
+    <t>:cif-transplant</t>
+  </si>
+  <si>
+    <t>:cif-death</t>
   </si>
 </sst>
 </file>
@@ -2243,7 +2249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0769D7-2771-0847-A535-A41EFB32FC0A}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -2308,7 +2314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:D3206"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -2329,10 +2335,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
and now with correct categorical SPT baselines
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780AC7FE-66C3-774B-9DDF-E6ADB0B39773}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2B7CFA-3F61-174E-9939-16E5EC1E0E6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61280" yWindow="4180" windowWidth="28320" windowHeight="21040" firstSheet="1" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="61280" yWindow="4180" windowWidth="28320" windowHeight="21040" firstSheet="1" activeTab="7" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -992,18 +992,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1571,7 +1571,7 @@
       <c r="B8" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="66" t="s">
         <v>77</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -1595,7 +1595,7 @@
       <c r="B9" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="17" t="s">
         <v>208</v>
       </c>
@@ -1791,7 +1791,7 @@
       <c r="C20" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="63" t="s">
         <v>186</v>
       </c>
       <c r="E20">
@@ -1817,7 +1817,7 @@
       <c r="B21" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="D21" s="65" t="s">
+      <c r="D21" s="63" t="s">
         <v>187</v>
       </c>
       <c r="E21">
@@ -1834,7 +1834,7 @@
         <v>193</v>
       </c>
       <c r="C22" s="31"/>
-      <c r="D22" s="65" t="s">
+      <c r="D22" s="63" t="s">
         <v>188</v>
       </c>
       <c r="E22">
@@ -1851,7 +1851,7 @@
         <v>194</v>
       </c>
       <c r="C23" s="31"/>
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="63" t="s">
         <v>189</v>
       </c>
       <c r="E23">
@@ -1868,7 +1868,7 @@
         <v>195</v>
       </c>
       <c r="C24" s="61"/>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="63" t="s">
         <v>190</v>
       </c>
       <c r="E24">
@@ -1896,7 +1896,7 @@
       <c r="C26" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="64" t="s">
+      <c r="D26" s="62" t="s">
         <v>213</v>
       </c>
       <c r="E26">
@@ -1918,7 +1918,7 @@
         <v>211</v>
       </c>
       <c r="C27" s="26"/>
-      <c r="D27" s="64" t="s">
+      <c r="D27" s="62" t="s">
         <v>215</v>
       </c>
       <c r="E27">
@@ -1936,7 +1936,7 @@
         <v>212</v>
       </c>
       <c r="C28" s="26"/>
-      <c r="D28" s="64" t="s">
+      <c r="D28" s="62" t="s">
         <v>214</v>
       </c>
       <c r="E28">
@@ -2057,7 +2057,7 @@
       <c r="C36" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="66" t="s">
+      <c r="D36" s="64" t="s">
         <v>204</v>
       </c>
       <c r="E36">
@@ -2079,7 +2079,7 @@
         <v>197</v>
       </c>
       <c r="C37" s="26"/>
-      <c r="D37" s="66" t="s">
+      <c r="D37" s="64" t="s">
         <v>205</v>
       </c>
       <c r="E37">
@@ -2097,7 +2097,7 @@
         <v>198</v>
       </c>
       <c r="C38" s="26"/>
-      <c r="D38" s="66" t="s">
+      <c r="D38" s="64" t="s">
         <v>206</v>
       </c>
       <c r="E38">
@@ -2115,7 +2115,7 @@
         <v>199</v>
       </c>
       <c r="C39" s="26"/>
-      <c r="D39" s="66" t="s">
+      <c r="D39" s="64" t="s">
         <v>207</v>
       </c>
       <c r="E39">
@@ -2200,7 +2200,7 @@
       <c r="B44" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C44" s="63"/>
+      <c r="C44" s="66"/>
       <c r="D44" s="3" t="s">
         <v>203</v>
       </c>
@@ -2216,7 +2216,7 @@
     <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
-      <c r="C45" s="63"/>
+      <c r="C45" s="66"/>
       <c r="E45" s="29"/>
       <c r="I45" s="40"/>
       <c r="J45" s="8"/>
@@ -27473,7 +27473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -27718,7 +27718,7 @@
       <c r="B10" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="65" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="49" t="s">
@@ -27748,7 +27748,7 @@
       <c r="B11" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="51" t="s">
         <v>158</v>
       </c>
@@ -28423,8 +28423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FE1BB-1AC5-6D40-AB0F-F4D73062F511}">
   <dimension ref="A1:N1015"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E313" sqref="E313"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C400"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -28488,7 +28488,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.98988639040000004</v>
+        <v>0.9905913207</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -28506,7 +28506,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>0.97964942180000003</v>
+        <v>0.9810283045</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -28522,7 +28522,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>0.9744918025</v>
+        <v>0.97621457899999997</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -28538,7 +28538,7 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>0.96932938430000004</v>
+        <v>0.97140577260000005</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -28554,7 +28554,7 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>0.95902617570000004</v>
+        <v>0.96179730730000002</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -28570,7 +28570,7 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>0.95375841559999996</v>
+        <v>0.95692094130000005</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -28586,7 +28586,7 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>0.943205776</v>
+        <v>0.94715603059999998</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -28602,7 +28602,7 @@
         <v>25</v>
       </c>
       <c r="C10">
-        <v>0.93783379860000005</v>
+        <v>0.94220261329999999</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -28618,7 +28618,7 @@
         <v>26</v>
       </c>
       <c r="C11">
-        <v>0.93238212750000005</v>
+        <v>0.93716899279999999</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -28634,12 +28634,12 @@
         <v>42</v>
       </c>
       <c r="C12">
-        <v>0.92693259979999998</v>
+        <v>0.93212459039999995</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="63"/>
+      <c r="F12" s="66"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28650,12 +28650,12 @@
         <v>56</v>
       </c>
       <c r="C13">
-        <v>0.92143891099999997</v>
+        <v>0.92701903009999997</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="63"/>
+      <c r="F13" s="66"/>
     </row>
     <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -28665,7 +28665,7 @@
         <v>57</v>
       </c>
       <c r="C14">
-        <v>0.91588139189999995</v>
+        <v>0.92185905420000003</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -28679,7 +28679,7 @@
         <v>69</v>
       </c>
       <c r="C15">
-        <v>0.91032272489999999</v>
+        <v>0.91669159889999996</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -28693,7 +28693,7 @@
         <v>70</v>
       </c>
       <c r="C16">
-        <v>0.89908917479999995</v>
+        <v>0.90626014580000003</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -28707,7 +28707,7 @@
         <v>80</v>
       </c>
       <c r="C17">
-        <v>0.89337731669999998</v>
+        <v>0.90096447430000004</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -28721,7 +28721,7 @@
         <v>96</v>
       </c>
       <c r="C18">
-        <v>0.88756588150000004</v>
+        <v>0.89558997780000005</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -28735,7 +28735,7 @@
         <v>100</v>
       </c>
       <c r="C19">
-        <v>0.88160790020000002</v>
+        <v>0.89006224199999995</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -28749,7 +28749,7 @@
         <v>105</v>
       </c>
       <c r="C20">
-        <v>0.87563951770000004</v>
+        <v>0.88451604949999996</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -28763,7 +28763,7 @@
         <v>114</v>
       </c>
       <c r="C21">
-        <v>0.86966359439999996</v>
+        <v>0.87895389970000004</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -28777,7 +28777,7 @@
         <v>121</v>
       </c>
       <c r="C22">
-        <v>0.86358447419999995</v>
+        <v>0.87328199549999996</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -28791,7 +28791,7 @@
         <v>122</v>
       </c>
       <c r="C23">
-        <v>0.85745943120000001</v>
+        <v>0.86756776719999995</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -28805,7 +28805,7 @@
         <v>138</v>
       </c>
       <c r="C24">
-        <v>0.8513031069</v>
+        <v>0.86180697979999998</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -28819,7 +28819,7 @@
         <v>157</v>
       </c>
       <c r="C25">
-        <v>0.84510913320000003</v>
+        <v>0.85601025529999997</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -28833,7 +28833,7 @@
         <v>173</v>
       </c>
       <c r="C26">
-        <v>0.83257950400000003</v>
+        <v>0.84427747249999996</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -28847,7 +28847,7 @@
         <v>177</v>
       </c>
       <c r="C27">
-        <v>0.82618863190000003</v>
+        <v>0.83826440479999997</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
@@ -28861,7 +28861,7 @@
         <v>193</v>
       </c>
       <c r="C28">
-        <v>0.81977990270000001</v>
+        <v>0.83223046919999999</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
@@ -28875,7 +28875,7 @@
         <v>237</v>
       </c>
       <c r="C29">
-        <v>0.81334877120000004</v>
+        <v>0.82619825830000004</v>
       </c>
       <c r="E29" s="3">
         <v>1</v>
@@ -28889,7 +28889,7 @@
         <v>276</v>
       </c>
       <c r="C30">
-        <v>0.80687687829999999</v>
+        <v>0.82012119610000001</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
@@ -28903,7 +28903,7 @@
         <v>289</v>
       </c>
       <c r="C31">
-        <v>0.80037924120000004</v>
+        <v>0.81401348419999997</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
@@ -28917,7 +28917,7 @@
         <v>292</v>
       </c>
       <c r="C32">
-        <v>0.7938250107</v>
+        <v>0.80781451179999997</v>
       </c>
       <c r="E32" s="3">
         <v>1</v>
@@ -28931,7 +28931,7 @@
         <v>297</v>
       </c>
       <c r="C33">
-        <v>0.78724549830000001</v>
+        <v>0.80158932569999997</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
@@ -28945,7 +28945,7 @@
         <v>303</v>
       </c>
       <c r="C34">
-        <v>0.78062644690000005</v>
+        <v>0.79533016229999998</v>
       </c>
       <c r="E34" s="3">
         <v>1</v>
@@ -28959,7 +28959,7 @@
         <v>310</v>
       </c>
       <c r="C35">
-        <v>0.77394366790000002</v>
+        <v>0.78899315820000004</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
@@ -28973,7 +28973,7 @@
         <v>328</v>
       </c>
       <c r="C36">
-        <v>0.7672300568</v>
+        <v>0.78261299610000001</v>
       </c>
       <c r="E36" s="3">
         <v>1</v>
@@ -28987,7 +28987,7 @@
         <v>403</v>
       </c>
       <c r="C37">
-        <v>0.75989236189999998</v>
+        <v>0.77553552889999999</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -29001,7 +29001,7 @@
         <v>439</v>
       </c>
       <c r="C38">
-        <v>0.7524912372</v>
+        <v>0.76840616559999997</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -29015,7 +29015,7 @@
         <v>517</v>
       </c>
       <c r="C39">
-        <v>0.73774568519999995</v>
+        <v>0.754205864</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
@@ -29029,7 +29029,7 @@
         <v>553</v>
       </c>
       <c r="C40">
-        <v>0.73025162210000005</v>
+        <v>0.74696827929999998</v>
       </c>
       <c r="E40" s="3">
         <v>1</v>
@@ -29043,7 +29043,7 @@
         <v>558</v>
       </c>
       <c r="C41">
-        <v>0.7226664049</v>
+        <v>0.73960507750000004</v>
       </c>
       <c r="E41" s="3">
         <v>1</v>
@@ -29057,7 +29057,7 @@
         <v>723</v>
       </c>
       <c r="C42">
-        <v>0.71430290839999999</v>
+        <v>0.73144059459999999</v>
       </c>
       <c r="E42" s="3">
         <v>1</v>
@@ -29071,7 +29071,7 @@
         <v>732</v>
       </c>
       <c r="C43">
-        <v>0.70567078439999997</v>
+        <v>0.72292952749999995</v>
       </c>
       <c r="E43" s="3">
         <v>1</v>
@@ -29085,7 +29085,7 @@
         <v>827</v>
       </c>
       <c r="C44">
-        <v>0.69617308079999995</v>
+        <v>0.71339093990000002</v>
       </c>
       <c r="E44" s="3">
         <v>1</v>
@@ -29099,7 +29099,7 @@
         <v>1258</v>
       </c>
       <c r="C45">
-        <v>0.68558160489999997</v>
+        <v>0.70309116009999995</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
@@ -29113,7 +29113,7 @@
         <v>1572</v>
       </c>
       <c r="C46">
-        <v>0.67094507920000002</v>
+        <v>0.6886668091</v>
       </c>
       <c r="E46" s="3">
         <v>1</v>
@@ -29127,7 +29127,7 @@
         <v>1582</v>
       </c>
       <c r="C47">
-        <v>0.6560978985</v>
+        <v>0.67395089279999998</v>
       </c>
       <c r="E47" s="3">
         <v>1</v>
@@ -29141,7 +29141,7 @@
         <v>1826</v>
       </c>
       <c r="C48">
-        <v>0.6560978985</v>
+        <v>0.67395089279999998</v>
       </c>
       <c r="E48" s="3">
         <v>47</v>
@@ -29169,7 +29169,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0.99570164520000004</v>
+        <v>0.99595214759999995</v>
       </c>
       <c r="E50" s="3">
         <f>E49+1</f>
@@ -29184,7 +29184,7 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>0.99139595209999998</v>
+        <v>0.99189401850000003</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" ref="E51:E114" si="0">E50+1</f>
@@ -29199,7 +29199,7 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>0.98707759250000005</v>
+        <v>0.98781764490000001</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" si="0"/>
@@ -29214,7 +29214,7 @@
         <v>4</v>
       </c>
       <c r="C53">
-        <v>0.98491666720000004</v>
+        <v>0.98577652729999998</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" si="0"/>
@@ -29229,7 +29229,7 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>0.98058919239999998</v>
+        <v>0.98169148279999996</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" si="0"/>
@@ -29244,7 +29244,7 @@
         <v>7</v>
       </c>
       <c r="C55">
-        <v>0.97841728090000002</v>
+        <v>0.97964204499999996</v>
       </c>
       <c r="E55" s="3">
         <f t="shared" si="0"/>
@@ -29259,7 +29259,7 @@
         <v>8</v>
       </c>
       <c r="C56">
-        <v>0.97624091820000003</v>
+        <v>0.97758839230000005</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" si="0"/>
@@ -29274,7 +29274,7 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>0.97405935659999998</v>
+        <v>0.97552817140000003</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" si="0"/>
@@ -29289,7 +29289,7 @@
         <v>10</v>
       </c>
       <c r="C58">
-        <v>0.97187186790000002</v>
+        <v>0.97346472070000001</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" si="0"/>
@@ -29304,7 +29304,7 @@
         <v>11</v>
       </c>
       <c r="C59">
-        <v>0.96967788539999999</v>
+        <v>0.97139814680000003</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" si="0"/>
@@ -29319,7 +29319,7 @@
         <v>13</v>
       </c>
       <c r="C60">
-        <v>0.9674799624</v>
+        <v>0.96932595109999997</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" si="0"/>
@@ -29334,7 +29334,7 @@
         <v>15</v>
       </c>
       <c r="C61">
-        <v>0.96527981699999998</v>
+        <v>0.96724892839999999</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" si="0"/>
@@ -29349,7 +29349,7 @@
         <v>16</v>
       </c>
       <c r="C62">
-        <v>0.96307391669999998</v>
+        <v>0.96516623589999995</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" si="0"/>
@@ -29364,7 +29364,7 @@
         <v>19</v>
       </c>
       <c r="C63">
-        <v>0.95866271189999996</v>
+        <v>0.96100342569999997</v>
       </c>
       <c r="E63" s="3">
         <f t="shared" si="0"/>
@@ -29379,7 +29379,7 @@
         <v>25</v>
       </c>
       <c r="C64">
-        <v>0.95645112430000001</v>
+        <v>0.95891491549999996</v>
       </c>
       <c r="E64" s="3">
         <f t="shared" si="0"/>
@@ -29394,7 +29394,7 @@
         <v>29</v>
       </c>
       <c r="C65">
-        <v>0.95423432969999999</v>
+        <v>0.95682276369999997</v>
       </c>
       <c r="E65" s="3">
         <f t="shared" si="0"/>
@@ -29409,7 +29409,7 @@
         <v>38</v>
       </c>
       <c r="C66">
-        <v>0.95201968420000005</v>
+        <v>0.95473155620000005</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" si="0"/>
@@ -29424,7 +29424,7 @@
         <v>41</v>
       </c>
       <c r="C67">
-        <v>0.94980323730000005</v>
+        <v>0.95263867310000006</v>
       </c>
       <c r="E67" s="3">
         <f t="shared" si="0"/>
@@ -29439,7 +29439,7 @@
         <v>42</v>
       </c>
       <c r="C68">
-        <v>0.94536884359999995</v>
+        <v>0.94845026649999997</v>
       </c>
       <c r="E68" s="3">
         <f t="shared" si="0"/>
@@ -29454,7 +29454,7 @@
         <v>44</v>
       </c>
       <c r="C69">
-        <v>0.9431467563</v>
+        <v>0.94634940290000003</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="0"/>
@@ -29469,7 +29469,7 @@
         <v>49</v>
       </c>
       <c r="C70">
-        <v>0.94092109229999998</v>
+        <v>0.94424345210000005</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="0"/>
@@ -29484,7 +29484,7 @@
         <v>52</v>
       </c>
       <c r="C71">
-        <v>0.93647285270000002</v>
+        <v>0.94003248589999999</v>
       </c>
       <c r="E71" s="3">
         <f t="shared" si="0"/>
@@ -29499,7 +29499,7 @@
         <v>64</v>
       </c>
       <c r="C72">
-        <v>0.93423977859999996</v>
+        <v>0.93791963919999999</v>
       </c>
       <c r="E72" s="3">
         <f t="shared" si="0"/>
@@ -29514,7 +29514,7 @@
         <v>72</v>
       </c>
       <c r="C73">
-        <v>0.93200206569999999</v>
+        <v>0.93579956720000002</v>
       </c>
       <c r="E73" s="3">
         <f t="shared" si="0"/>
@@ -29529,7 +29529,7 @@
         <v>115</v>
       </c>
       <c r="C74">
-        <v>0.92970446839999998</v>
+        <v>0.93362172710000002</v>
       </c>
       <c r="E74" s="3">
         <f t="shared" si="0"/>
@@ -29544,7 +29544,7 @@
         <v>118</v>
       </c>
       <c r="C75">
-        <v>0.92740746070000002</v>
+        <v>0.93144532710000005</v>
       </c>
       <c r="E75" s="3">
         <f t="shared" si="0"/>
@@ -29559,7 +29559,7 @@
         <v>121</v>
       </c>
       <c r="C76">
-        <v>0.92510739210000004</v>
+        <v>0.92926759120000002</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" si="0"/>
@@ -29574,7 +29574,7 @@
         <v>123</v>
       </c>
       <c r="C77">
-        <v>0.92280684639999999</v>
+        <v>0.92708813199999995</v>
       </c>
       <c r="E77" s="3">
         <f t="shared" si="0"/>
@@ -29589,7 +29589,7 @@
         <v>127</v>
       </c>
       <c r="C78">
-        <v>0.92050723700000003</v>
+        <v>0.92490771780000003</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="0"/>
@@ -29604,7 +29604,7 @@
         <v>141</v>
       </c>
       <c r="C79">
-        <v>0.91820525139999998</v>
+        <v>0.92272432510000002</v>
       </c>
       <c r="E79" s="3">
         <f t="shared" si="0"/>
@@ -29619,7 +29619,7 @@
         <v>144</v>
       </c>
       <c r="C80">
-        <v>0.91590321100000005</v>
+        <v>0.92054093250000002</v>
       </c>
       <c r="E80" s="3">
         <f t="shared" si="0"/>
@@ -29634,7 +29634,7 @@
         <v>163</v>
       </c>
       <c r="C81">
-        <v>0.9135981634</v>
+        <v>0.91835374910000001</v>
       </c>
       <c r="E81" s="3">
         <f t="shared" si="0"/>
@@ -29649,7 +29649,7 @@
         <v>164</v>
       </c>
       <c r="C82">
-        <v>0.91129295060000004</v>
+        <v>0.91616604189999995</v>
       </c>
       <c r="E82" s="3">
         <f t="shared" si="0"/>
@@ -29664,7 +29664,7 @@
         <v>166</v>
       </c>
       <c r="C83">
-        <v>0.90897704739999996</v>
+        <v>0.91396695539999995</v>
       </c>
       <c r="E83" s="3">
         <f t="shared" si="0"/>
@@ -29679,7 +29679,7 @@
         <v>190</v>
       </c>
       <c r="C84">
-        <v>0.9066596938</v>
+        <v>0.91176486069999996</v>
       </c>
       <c r="E84" s="3">
         <f t="shared" si="0"/>
@@ -29694,7 +29694,7 @@
         <v>191</v>
       </c>
       <c r="C85">
-        <v>0.90433818539999999</v>
+        <v>0.90955653569999995</v>
       </c>
       <c r="E85" s="3">
         <f t="shared" si="0"/>
@@ -29709,7 +29709,7 @@
         <v>198</v>
       </c>
       <c r="C86">
-        <v>0.90201299629999998</v>
+        <v>0.90734337430000001</v>
       </c>
       <c r="E86" s="3">
         <f t="shared" si="0"/>
@@ -29724,7 +29724,7 @@
         <v>203</v>
       </c>
       <c r="C87">
-        <v>0.89968581039999995</v>
+        <v>0.90512700540000002</v>
       </c>
       <c r="E87" s="3">
         <f t="shared" si="0"/>
@@ -29739,7 +29739,7 @@
         <v>213</v>
       </c>
       <c r="C88">
-        <v>0.89735967319999999</v>
+        <v>0.90291124060000005</v>
       </c>
       <c r="E88" s="3">
         <f t="shared" si="0"/>
@@ -29754,7 +29754,7 @@
         <v>215</v>
       </c>
       <c r="C89">
-        <v>0.89503499620000004</v>
+        <v>0.90069523269999996</v>
       </c>
       <c r="E89" s="3">
         <f t="shared" si="0"/>
@@ -29769,7 +29769,7 @@
         <v>216</v>
       </c>
       <c r="C90">
-        <v>0.89270844940000005</v>
+        <v>0.89847549230000001</v>
       </c>
       <c r="E90" s="3">
         <f t="shared" si="0"/>
@@ -29784,7 +29784,7 @@
         <v>269</v>
       </c>
       <c r="C91">
-        <v>0.89038139179999998</v>
+        <v>0.89625520039999995</v>
       </c>
       <c r="E91" s="3">
         <f t="shared" si="0"/>
@@ -29799,7 +29799,7 @@
         <v>298</v>
       </c>
       <c r="C92">
-        <v>0.88804456759999995</v>
+        <v>0.89402620430000002</v>
       </c>
       <c r="E92" s="3">
         <f t="shared" si="0"/>
@@ -29814,7 +29814,7 @@
         <v>303</v>
       </c>
       <c r="C93">
-        <v>0.88570644040000002</v>
+        <v>0.89179575600000005</v>
       </c>
       <c r="E93" s="3">
         <f t="shared" si="0"/>
@@ -29829,7 +29829,7 @@
         <v>348</v>
       </c>
       <c r="C94">
-        <v>0.88332952460000003</v>
+        <v>0.88953363760000004</v>
       </c>
       <c r="E94" s="3">
         <f t="shared" si="0"/>
@@ -29844,7 +29844,7 @@
         <v>351</v>
       </c>
       <c r="C95">
-        <v>0.88094692409999997</v>
+        <v>0.88726569070000005</v>
       </c>
       <c r="E95" s="3">
         <f t="shared" si="0"/>
@@ -29859,7 +29859,7 @@
         <v>361</v>
       </c>
       <c r="C96">
-        <v>0.87854140800000002</v>
+        <v>0.88497506370000001</v>
       </c>
       <c r="E96" s="3">
         <f t="shared" si="0"/>
@@ -29874,7 +29874,7 @@
         <v>375</v>
       </c>
       <c r="C97">
-        <v>0.87612665940000001</v>
+        <v>0.88267546659999996</v>
       </c>
       <c r="E97" s="3">
         <f t="shared" si="0"/>
@@ -29889,7 +29889,7 @@
         <v>398</v>
       </c>
       <c r="C98">
-        <v>0.87365627479999997</v>
+        <v>0.88031540949999998</v>
       </c>
       <c r="E98" s="3">
         <f t="shared" si="0"/>
@@ -29904,7 +29904,7 @@
         <v>412</v>
       </c>
       <c r="C99">
-        <v>0.87115427310000004</v>
+        <v>0.87793052439999997</v>
       </c>
       <c r="E99" s="3">
         <f t="shared" si="0"/>
@@ -29919,7 +29919,7 @@
         <v>415</v>
       </c>
       <c r="C100">
-        <v>0.8686517104</v>
+        <v>0.87554539539999998</v>
       </c>
       <c r="E100" s="3">
         <f t="shared" si="0"/>
@@ -29934,7 +29934,7 @@
         <v>436</v>
       </c>
       <c r="C101">
-        <v>0.86613317349999996</v>
+        <v>0.87314483890000005</v>
       </c>
       <c r="E101" s="3">
         <f t="shared" si="0"/>
@@ -29949,7 +29949,7 @@
         <v>441</v>
       </c>
       <c r="C102">
-        <v>0.86361112409999996</v>
+        <v>0.87073922439999996</v>
       </c>
       <c r="E102" s="3">
         <f t="shared" si="0"/>
@@ -29964,7 +29964,7 @@
         <v>463</v>
       </c>
       <c r="C103">
-        <v>0.86107878329999998</v>
+        <v>0.86832145260000004</v>
       </c>
       <c r="E103" s="3">
         <f t="shared" si="0"/>
@@ -29979,7 +29979,7 @@
         <v>505</v>
       </c>
       <c r="C104">
-        <v>0.85854190829999999</v>
+        <v>0.86589610900000002</v>
       </c>
       <c r="E104" s="3">
         <f t="shared" si="0"/>
@@ -29994,7 +29994,7 @@
         <v>548</v>
       </c>
       <c r="C105">
-        <v>0.85346708609999999</v>
+        <v>0.86104089039999998</v>
       </c>
       <c r="E105" s="3">
         <f t="shared" si="0"/>
@@ -30009,7 +30009,7 @@
         <v>552</v>
       </c>
       <c r="C106">
-        <v>0.85091610529999995</v>
+        <v>0.8586034561</v>
       </c>
       <c r="E106" s="3">
         <f t="shared" si="0"/>
@@ -30024,7 +30024,7 @@
         <v>575</v>
       </c>
       <c r="C107">
-        <v>0.84836350780000003</v>
+        <v>0.85616503909999997</v>
       </c>
       <c r="E107" s="3">
         <f t="shared" si="0"/>
@@ -30039,7 +30039,7 @@
         <v>644</v>
       </c>
       <c r="C108">
-        <v>0.84580760759999996</v>
+        <v>0.8537199446</v>
       </c>
       <c r="E108" s="3">
         <f t="shared" si="0"/>
@@ -30054,7 +30054,7 @@
         <v>652</v>
       </c>
       <c r="C109">
-        <v>0.84322247400000006</v>
+        <v>0.85124728650000003</v>
       </c>
       <c r="E109" s="3">
         <f t="shared" si="0"/>
@@ -30069,7 +30069,7 @@
         <v>660</v>
       </c>
       <c r="C110">
-        <v>0.84062153750000002</v>
+        <v>0.84875995309999996</v>
       </c>
       <c r="E110" s="3">
         <f t="shared" si="0"/>
@@ -30084,7 +30084,7 @@
         <v>661</v>
       </c>
       <c r="C111">
-        <v>0.83802028230000003</v>
+        <v>0.84626992670000001</v>
       </c>
       <c r="E111" s="3">
         <f t="shared" si="0"/>
@@ -30099,7 +30099,7 @@
         <v>697</v>
       </c>
       <c r="C112">
-        <v>0.8353577875</v>
+        <v>0.84371941910000003</v>
       </c>
       <c r="E112" s="3">
         <f t="shared" si="0"/>
@@ -30114,7 +30114,7 @@
         <v>739</v>
       </c>
       <c r="C113">
-        <v>0.83248132640000005</v>
+        <v>0.84096157920000003</v>
       </c>
       <c r="E113" s="3">
         <f t="shared" si="0"/>
@@ -30129,7 +30129,7 @@
         <v>740</v>
       </c>
       <c r="C114">
-        <v>0.82960026320000002</v>
+        <v>0.83820055459999998</v>
       </c>
       <c r="E114" s="3">
         <f t="shared" si="0"/>
@@ -30144,7 +30144,7 @@
         <v>753</v>
       </c>
       <c r="C115">
-        <v>0.82666542929999998</v>
+        <v>0.83538700789999998</v>
       </c>
       <c r="E115" s="3">
         <f t="shared" ref="E115:E142" si="1">E114+1</f>
@@ -30159,7 +30159,7 @@
         <v>755</v>
       </c>
       <c r="C116">
-        <v>0.82371188360000003</v>
+        <v>0.83255572990000004</v>
       </c>
       <c r="E116" s="3">
         <f t="shared" si="1"/>
@@ -30174,7 +30174,7 @@
         <v>811</v>
       </c>
       <c r="C117">
-        <v>0.82050746090000004</v>
+        <v>0.82948640090000003</v>
       </c>
       <c r="E117" s="3">
         <f t="shared" si="1"/>
@@ -30189,7 +30189,7 @@
         <v>826</v>
       </c>
       <c r="C118">
-        <v>0.81727838539999997</v>
+        <v>0.82639208180000001</v>
       </c>
       <c r="E118" s="3">
         <f t="shared" si="1"/>
@@ -30204,7 +30204,7 @@
         <v>836</v>
       </c>
       <c r="C119">
-        <v>0.81404589900000002</v>
+        <v>0.82329505130000002</v>
       </c>
       <c r="E119" s="3">
         <f t="shared" si="1"/>
@@ -30219,7 +30219,7 @@
         <v>838</v>
       </c>
       <c r="C120">
-        <v>0.81080728520000001</v>
+        <v>0.8201905625</v>
       </c>
       <c r="E120" s="3">
         <f t="shared" si="1"/>
@@ -30234,7 +30234,7 @@
         <v>907</v>
       </c>
       <c r="C121">
-        <v>0.80756236719999996</v>
+        <v>0.81708320290000003</v>
       </c>
       <c r="E121" s="3">
         <f t="shared" si="1"/>
@@ -30249,7 +30249,7 @@
         <v>938</v>
       </c>
       <c r="C122">
-        <v>0.80430873179999995</v>
+        <v>0.81396899649999999</v>
       </c>
       <c r="E122" s="3">
         <f t="shared" si="1"/>
@@ -30264,7 +30264,7 @@
         <v>954</v>
       </c>
       <c r="C123">
-        <v>0.80104948009999999</v>
+        <v>0.81084977120000001</v>
       </c>
       <c r="E123" s="3">
         <f t="shared" si="1"/>
@@ -30279,7 +30279,7 @@
         <v>987</v>
       </c>
       <c r="C124">
-        <v>0.79776741009999996</v>
+        <v>0.80771277850000001</v>
       </c>
       <c r="E124" s="3">
         <f t="shared" si="1"/>
@@ -30294,7 +30294,7 @@
         <v>1008</v>
       </c>
       <c r="C125">
-        <v>0.79444994000000002</v>
+        <v>0.80454621790000003</v>
       </c>
       <c r="E125" s="3">
         <f t="shared" si="1"/>
@@ -30309,7 +30309,7 @@
         <v>1059</v>
       </c>
       <c r="C126">
-        <v>0.79109199620000004</v>
+        <v>0.80133932959999998</v>
       </c>
       <c r="E126" s="3">
         <f t="shared" si="1"/>
@@ -30324,7 +30324,7 @@
         <v>1066</v>
       </c>
       <c r="C127">
-        <v>0.78770501469999998</v>
+        <v>0.79810030580000002</v>
       </c>
       <c r="E127" s="3">
         <f t="shared" si="1"/>
@@ -30339,7 +30339,7 @@
         <v>1136</v>
       </c>
       <c r="C128">
-        <v>0.78375779560000003</v>
+        <v>0.79436713049999996</v>
       </c>
       <c r="E128" s="3">
         <f t="shared" si="1"/>
@@ -30354,7 +30354,7 @@
         <v>1148</v>
       </c>
       <c r="C129">
-        <v>0.77974218449999999</v>
+        <v>0.79056284430000001</v>
       </c>
       <c r="E129" s="3">
         <f t="shared" si="1"/>
@@ -30369,7 +30369,7 @@
         <v>1191</v>
       </c>
       <c r="C130">
-        <v>0.77559343030000005</v>
+        <v>0.78662663460000004</v>
       </c>
       <c r="E130" s="3">
         <f t="shared" si="1"/>
@@ -30384,7 +30384,7 @@
         <v>1317</v>
       </c>
       <c r="C131">
-        <v>0.77140654340000003</v>
+        <v>0.78264898810000005</v>
       </c>
       <c r="E131" s="3">
         <f t="shared" si="1"/>
@@ -30399,7 +30399,7 @@
         <v>1343</v>
       </c>
       <c r="C132">
-        <v>0.76718970779999995</v>
+        <v>0.77863818549999997</v>
       </c>
       <c r="E132" s="3">
         <f t="shared" si="1"/>
@@ -30414,7 +30414,7 @@
         <v>1351</v>
       </c>
       <c r="C133">
-        <v>0.76290146339999998</v>
+        <v>0.77457579980000002</v>
       </c>
       <c r="E133" s="3">
         <f t="shared" si="1"/>
@@ -30429,7 +30429,7 @@
         <v>1557</v>
       </c>
       <c r="C134">
-        <v>0.75670921339999997</v>
+        <v>0.76878888460000006</v>
       </c>
       <c r="E134" s="3">
         <f t="shared" si="1"/>
@@ -30444,7 +30444,7 @@
         <v>1563</v>
       </c>
       <c r="C135">
-        <v>0.75051636880000006</v>
+        <v>0.76299650279999998</v>
       </c>
       <c r="E135" s="3">
         <f t="shared" si="1"/>
@@ -30459,7 +30459,7 @@
         <v>1645</v>
       </c>
       <c r="C136">
-        <v>0.7442344367</v>
+        <v>0.75706410280000003</v>
       </c>
       <c r="E136" s="3">
         <f t="shared" si="1"/>
@@ -30474,7 +30474,7 @@
         <v>1733</v>
       </c>
       <c r="C137">
-        <v>0.73792569289999999</v>
+        <v>0.75110615550000004</v>
       </c>
       <c r="E137" s="3">
         <f t="shared" si="1"/>
@@ -30489,7 +30489,7 @@
         <v>1745</v>
       </c>
       <c r="C138">
-        <v>0.73158817089999995</v>
+        <v>0.74512972570000002</v>
       </c>
       <c r="E138" s="3">
         <f t="shared" si="1"/>
@@ -30504,7 +30504,7 @@
         <v>1762</v>
       </c>
       <c r="C139">
-        <v>0.72504099050000004</v>
+        <v>0.73899710169999999</v>
       </c>
       <c r="E139" s="3">
         <f t="shared" si="1"/>
@@ -30519,7 +30519,7 @@
         <v>1783</v>
       </c>
       <c r="C140">
-        <v>0.7182215555</v>
+        <v>0.73258415750000005</v>
       </c>
       <c r="E140" s="3">
         <f t="shared" si="1"/>
@@ -30534,7 +30534,7 @@
         <v>1784</v>
       </c>
       <c r="C141">
-        <v>0.71136034439999996</v>
+        <v>0.72614927100000004</v>
       </c>
       <c r="E141" s="3">
         <f t="shared" si="1"/>
@@ -30549,7 +30549,7 @@
         <v>1826</v>
       </c>
       <c r="C142">
-        <v>0.71136034439999996</v>
+        <v>0.72614927100000004</v>
       </c>
       <c r="E142" s="3">
         <f t="shared" si="1"/>
@@ -30578,7 +30578,7 @@
         <v>0</v>
       </c>
       <c r="C144">
-        <v>0.99696451070000003</v>
+        <v>0.99709106359999999</v>
       </c>
       <c r="E144" s="3">
         <f t="shared" ref="E144:E207" si="2">E143+1</f>
@@ -30593,7 +30593,7 @@
         <v>1</v>
       </c>
       <c r="C145">
-        <v>0.99392696619999998</v>
+        <v>0.99417908700000002</v>
       </c>
       <c r="E145" s="3">
         <f t="shared" si="2"/>
@@ -30608,7 +30608,7 @@
         <v>2</v>
       </c>
       <c r="C146">
-        <v>0.99088240169999997</v>
+        <v>0.99126163570000003</v>
       </c>
       <c r="E146" s="3">
         <f t="shared" si="2"/>
@@ -30623,7 +30623,7 @@
         <v>5</v>
       </c>
       <c r="C147">
-        <v>0.98783299059999996</v>
+        <v>0.98833676820000005</v>
       </c>
       <c r="E147" s="3">
         <f t="shared" si="2"/>
@@ -30638,7 +30638,7 @@
         <v>10</v>
       </c>
       <c r="C148">
-        <v>0.98475915319999996</v>
+        <v>0.98539286039999996</v>
       </c>
       <c r="E148" s="3">
         <f t="shared" si="2"/>
@@ -30653,7 +30653,7 @@
         <v>28</v>
       </c>
       <c r="C149">
-        <v>0.98165919040000005</v>
+        <v>0.98242341860000004</v>
       </c>
       <c r="E149" s="3">
         <f t="shared" si="2"/>
@@ -30668,7 +30668,7 @@
         <v>51</v>
       </c>
       <c r="C150">
-        <v>0.97855213019999998</v>
+        <v>0.97944666960000004</v>
       </c>
       <c r="E150" s="3">
         <f t="shared" si="2"/>
@@ -30683,7 +30683,7 @@
         <v>52</v>
       </c>
       <c r="C151">
-        <v>0.97543553110000003</v>
+        <v>0.97646330930000003</v>
       </c>
       <c r="E151" s="3">
         <f t="shared" si="2"/>
@@ -30698,7 +30698,7 @@
         <v>53</v>
       </c>
       <c r="C152">
-        <v>0.97232297359999997</v>
+        <v>0.97348155930000002</v>
       </c>
       <c r="E152" s="3">
         <f t="shared" si="2"/>
@@ -30713,7 +30713,7 @@
         <v>58</v>
       </c>
       <c r="C153">
-        <v>0.96917576689999996</v>
+        <v>0.97048518340000001</v>
       </c>
       <c r="E153" s="3">
         <f t="shared" si="2"/>
@@ -30728,7 +30728,7 @@
         <v>82</v>
       </c>
       <c r="C154">
-        <v>0.96600012749999997</v>
+        <v>0.96745803919999995</v>
       </c>
       <c r="E154" s="3">
         <f t="shared" si="2"/>
@@ -30743,7 +30743,7 @@
         <v>88</v>
       </c>
       <c r="C155">
-        <v>0.96281723740000003</v>
+        <v>0.9644238141</v>
       </c>
       <c r="E155" s="3">
         <f t="shared" si="2"/>
@@ -30758,7 +30758,7 @@
         <v>91</v>
       </c>
       <c r="C156">
-        <v>0.95963595810000002</v>
+        <v>0.96138915059999996</v>
       </c>
       <c r="E156" s="3">
         <f t="shared" si="2"/>
@@ -30773,7 +30773,7 @@
         <v>103</v>
       </c>
       <c r="C157">
-        <v>0.95641274330000003</v>
+        <v>0.95831493540000001</v>
       </c>
       <c r="E157" s="3">
         <f t="shared" si="2"/>
@@ -30788,7 +30788,7 @@
         <v>112</v>
       </c>
       <c r="C158">
-        <v>0.95316250790000001</v>
+        <v>0.95521207060000002</v>
       </c>
       <c r="E158" s="3">
         <f t="shared" si="2"/>
@@ -30803,7 +30803,7 @@
         <v>119</v>
       </c>
       <c r="C159">
-        <v>0.94990967609999999</v>
+        <v>0.95210651180000005</v>
       </c>
       <c r="E159" s="3">
         <f t="shared" si="2"/>
@@ -30818,7 +30818,7 @@
         <v>154</v>
       </c>
       <c r="C160">
-        <v>0.94340382089999997</v>
+        <v>0.94590151509999998</v>
       </c>
       <c r="E160" s="3">
         <f t="shared" si="2"/>
@@ -30833,7 +30833,7 @@
         <v>188</v>
       </c>
       <c r="C161">
-        <v>0.94013462290000005</v>
+        <v>0.94277780389999999</v>
       </c>
       <c r="E161" s="3">
         <f t="shared" si="2"/>
@@ -30848,7 +30848,7 @@
         <v>198</v>
       </c>
       <c r="C162">
-        <v>0.93684406779999996</v>
+        <v>0.93963041000000003</v>
       </c>
       <c r="E162" s="3">
         <f t="shared" si="2"/>
@@ -30863,7 +30863,7 @@
         <v>208</v>
       </c>
       <c r="C163">
-        <v>0.93354884490000001</v>
+        <v>0.93647499810000001</v>
       </c>
       <c r="E163" s="3">
         <f t="shared" si="2"/>
@@ -30878,7 +30878,7 @@
         <v>246</v>
       </c>
       <c r="C164">
-        <v>0.93024062740000002</v>
+        <v>0.93330510739999994</v>
       </c>
       <c r="E164" s="3">
         <f t="shared" si="2"/>
@@ -30893,7 +30893,7 @@
         <v>262</v>
       </c>
       <c r="C165">
-        <v>0.9269210417</v>
+        <v>0.93012490329999997</v>
       </c>
       <c r="E165" s="3">
         <f t="shared" si="2"/>
@@ -30908,7 +30908,7 @@
         <v>267</v>
       </c>
       <c r="C166">
-        <v>0.92360206170000003</v>
+        <v>0.92694525049999998</v>
       </c>
       <c r="E166" s="3">
         <f t="shared" si="2"/>
@@ -30923,7 +30923,7 @@
         <v>268</v>
       </c>
       <c r="C167">
-        <v>0.92027500839999998</v>
+        <v>0.92375646730000005</v>
       </c>
       <c r="E167" s="3">
         <f t="shared" si="2"/>
@@ -30938,7 +30938,7 @@
         <v>274</v>
       </c>
       <c r="C168">
-        <v>0.91692873100000005</v>
+        <v>0.9205493937</v>
       </c>
       <c r="E168" s="3">
         <f t="shared" si="2"/>
@@ -30953,7 +30953,7 @@
         <v>301</v>
       </c>
       <c r="C169">
-        <v>0.91356891910000004</v>
+        <v>0.91732764460000005</v>
       </c>
       <c r="E169" s="3">
         <f t="shared" si="2"/>
@@ -30968,7 +30968,7 @@
         <v>312</v>
       </c>
       <c r="C170">
-        <v>0.91018840069999996</v>
+        <v>0.91409033490000002</v>
       </c>
       <c r="E170" s="3">
         <f t="shared" si="2"/>
@@ -30983,7 +30983,7 @@
         <v>318</v>
       </c>
       <c r="C171">
-        <v>0.90679604790000001</v>
+        <v>0.91083740840000005</v>
       </c>
       <c r="E171" s="3">
         <f t="shared" si="2"/>
@@ -30998,7 +30998,7 @@
         <v>327</v>
       </c>
       <c r="C172">
-        <v>0.90337366320000001</v>
+        <v>0.90755319369999998</v>
       </c>
       <c r="E172" s="3">
         <f t="shared" si="2"/>
@@ -31013,7 +31013,7 @@
         <v>330</v>
       </c>
       <c r="C173">
-        <v>0.89994604779999998</v>
+        <v>0.90426033780000004</v>
       </c>
       <c r="E173" s="3">
         <f t="shared" si="2"/>
@@ -31028,7 +31028,7 @@
         <v>331</v>
       </c>
       <c r="C174">
-        <v>0.89308460889999997</v>
+        <v>0.8976743948</v>
       </c>
       <c r="E174" s="3">
         <f t="shared" si="2"/>
@@ -31043,7 +31043,7 @@
         <v>344</v>
       </c>
       <c r="C175">
-        <v>0.88605335149999997</v>
+        <v>0.89092815709999995</v>
       </c>
       <c r="E175" s="3">
         <f t="shared" si="2"/>
@@ -31058,7 +31058,7 @@
         <v>373</v>
       </c>
       <c r="C176">
-        <v>0.88236709830000004</v>
+        <v>0.88739951409999995</v>
       </c>
       <c r="E176" s="3">
         <f t="shared" si="2"/>
@@ -31073,7 +31073,7 @@
         <v>374</v>
       </c>
       <c r="C177">
-        <v>0.87865800530000004</v>
+        <v>0.88384901849999997</v>
       </c>
       <c r="E177" s="3">
         <f t="shared" si="2"/>
@@ -31088,7 +31088,7 @@
         <v>394</v>
       </c>
       <c r="C178">
-        <v>0.87493067550000003</v>
+        <v>0.88028088950000005</v>
       </c>
       <c r="E178" s="3">
         <f t="shared" si="2"/>
@@ -31103,7 +31103,7 @@
         <v>415</v>
       </c>
       <c r="C179">
-        <v>0.8711963291</v>
+        <v>0.87670175480000001</v>
       </c>
       <c r="E179" s="3">
         <f t="shared" si="2"/>
@@ -31118,7 +31118,7 @@
         <v>439</v>
       </c>
       <c r="C180">
-        <v>0.86744060509999998</v>
+        <v>0.87309248809999995</v>
       </c>
       <c r="E180" s="3">
         <f t="shared" si="2"/>
@@ -31133,7 +31133,7 @@
         <v>449</v>
       </c>
       <c r="C181">
-        <v>0.86368154590000001</v>
+        <v>0.86947705529999997</v>
       </c>
       <c r="E181" s="3">
         <f t="shared" si="2"/>
@@ -31148,7 +31148,7 @@
         <v>450</v>
       </c>
       <c r="C182">
-        <v>0.85992241979999995</v>
+        <v>0.86586011060000001</v>
       </c>
       <c r="E182" s="3">
         <f t="shared" si="2"/>
@@ -31163,7 +31163,7 @@
         <v>452</v>
       </c>
       <c r="C183">
-        <v>0.85613425409999999</v>
+        <v>0.8622248964</v>
       </c>
       <c r="E183" s="3">
         <f t="shared" si="2"/>
@@ -31178,7 +31178,7 @@
         <v>472</v>
       </c>
       <c r="C184">
-        <v>0.85233336410000005</v>
+        <v>0.8585799798</v>
       </c>
       <c r="E184" s="3">
         <f t="shared" si="2"/>
@@ -31193,7 +31193,7 @@
         <v>480</v>
       </c>
       <c r="C185">
-        <v>0.84850153719999999</v>
+        <v>0.85490774270000003</v>
       </c>
       <c r="E185" s="3">
         <f t="shared" si="2"/>
@@ -31208,7 +31208,7 @@
         <v>507</v>
       </c>
       <c r="C186">
-        <v>0.84464299180000002</v>
+        <v>0.85121169799999996</v>
       </c>
       <c r="E186" s="3">
         <f t="shared" si="2"/>
@@ -31223,7 +31223,7 @@
         <v>511</v>
       </c>
       <c r="C187">
-        <v>0.84078145390000003</v>
+        <v>0.84751451730000005</v>
       </c>
       <c r="E187" s="3">
         <f t="shared" si="2"/>
@@ -31238,7 +31238,7 @@
         <v>568</v>
       </c>
       <c r="C188">
-        <v>0.83688938930000001</v>
+        <v>0.84379798289999997</v>
       </c>
       <c r="E188" s="3">
         <f t="shared" si="2"/>
@@ -31253,7 +31253,7 @@
         <v>593</v>
       </c>
       <c r="C189">
-        <v>0.83298296380000003</v>
+        <v>0.84005665190000001</v>
       </c>
       <c r="E189" s="3">
         <f t="shared" si="2"/>
@@ -31268,7 +31268,7 @@
         <v>595</v>
       </c>
       <c r="C190">
-        <v>0.82906958710000001</v>
+        <v>0.83630768150000001</v>
       </c>
       <c r="E190" s="3">
         <f t="shared" si="2"/>
@@ -31283,7 +31283,7 @@
         <v>604</v>
       </c>
       <c r="C191">
-        <v>0.82511610160000004</v>
+        <v>0.83253725609999996</v>
       </c>
       <c r="E191" s="3">
         <f t="shared" si="2"/>
@@ -31298,7 +31298,7 @@
         <v>620</v>
       </c>
       <c r="C192">
-        <v>0.82114294430000001</v>
+        <v>0.82874480890000002</v>
       </c>
       <c r="E192" s="3">
         <f t="shared" si="2"/>
@@ -31313,7 +31313,7 @@
         <v>625</v>
       </c>
       <c r="C193">
-        <v>0.81715414109999995</v>
+        <v>0.82493477979999996</v>
       </c>
       <c r="E193" s="3">
         <f t="shared" si="2"/>
@@ -31328,7 +31328,7 @@
         <v>665</v>
       </c>
       <c r="C194">
-        <v>0.8130697657</v>
+        <v>0.82101773430000002</v>
       </c>
       <c r="E194" s="3">
         <f t="shared" si="2"/>
@@ -31343,7 +31343,7 @@
         <v>703</v>
       </c>
       <c r="C195">
-        <v>0.8087248024</v>
+        <v>0.81686419750000006</v>
       </c>
       <c r="E195" s="3">
         <f t="shared" si="2"/>
@@ -31358,7 +31358,7 @@
         <v>704</v>
       </c>
       <c r="C196">
-        <v>0.80436505110000001</v>
+        <v>0.81269338710000005</v>
       </c>
       <c r="E196" s="3">
         <f t="shared" si="2"/>
@@ -31373,7 +31373,7 @@
         <v>756</v>
       </c>
       <c r="C197">
-        <v>0.79964392650000005</v>
+        <v>0.80814806650000004</v>
       </c>
       <c r="E197" s="3">
         <f t="shared" si="2"/>
@@ -31388,7 +31388,7 @@
         <v>772</v>
       </c>
       <c r="C198">
-        <v>0.79487185979999997</v>
+        <v>0.8035584536</v>
       </c>
       <c r="E198" s="3">
         <f t="shared" si="2"/>
@@ -31403,7 +31403,7 @@
         <v>776</v>
       </c>
       <c r="C199">
-        <v>0.79004964300000002</v>
+        <v>0.79892511879999994</v>
       </c>
       <c r="E199" s="3">
         <f t="shared" si="2"/>
@@ -31418,7 +31418,7 @@
         <v>869</v>
       </c>
       <c r="C200">
-        <v>0.78515565629999995</v>
+        <v>0.7941874699</v>
       </c>
       <c r="E200" s="3">
         <f t="shared" si="2"/>
@@ -31433,7 +31433,7 @@
         <v>876</v>
       </c>
       <c r="C201">
-        <v>0.78024869659999996</v>
+        <v>0.78944069179999998</v>
       </c>
       <c r="E201" s="3">
         <f t="shared" si="2"/>
@@ -31448,7 +31448,7 @@
         <v>923</v>
       </c>
       <c r="C202">
-        <v>0.77531966100000005</v>
+        <v>0.78467348459999997</v>
       </c>
       <c r="E202" s="3">
         <f t="shared" si="2"/>
@@ -31463,7 +31463,7 @@
         <v>1002</v>
       </c>
       <c r="C203">
-        <v>0.77031197470000001</v>
+        <v>0.77985952199999997</v>
       </c>
       <c r="E203" s="3">
         <f t="shared" si="2"/>
@@ -31478,7 +31478,7 @@
         <v>1007</v>
       </c>
       <c r="C204">
-        <v>0.76530880999999995</v>
+        <v>0.77504419459999996</v>
       </c>
       <c r="E204" s="3">
         <f t="shared" si="2"/>
@@ -31493,7 +31493,7 @@
         <v>1030</v>
       </c>
       <c r="C205">
-        <v>0.76027579729999994</v>
+        <v>0.77020665290000001</v>
       </c>
       <c r="E205" s="3">
         <f t="shared" si="2"/>
@@ -31508,7 +31508,7 @@
         <v>1045</v>
       </c>
       <c r="C206">
-        <v>0.75516120779999996</v>
+        <v>0.76527930690000001</v>
       </c>
       <c r="E206" s="3">
         <f t="shared" si="2"/>
@@ -31523,7 +31523,7 @@
         <v>1082</v>
       </c>
       <c r="C207">
-        <v>0.7496731941</v>
+        <v>0.76001342640000003</v>
       </c>
       <c r="E207" s="3">
         <f t="shared" si="2"/>
@@ -31538,7 +31538,7 @@
         <v>1110</v>
       </c>
       <c r="C208">
-        <v>0.74396087420000001</v>
+        <v>0.75450965000000003</v>
       </c>
       <c r="E208" s="3">
         <f t="shared" ref="E208:E271" si="3">E207+1</f>
@@ -31553,7 +31553,7 @@
         <v>1147</v>
       </c>
       <c r="C209">
-        <v>0.73800877389999997</v>
+        <v>0.74875934759999996</v>
       </c>
       <c r="E209" s="3">
         <f t="shared" si="3"/>
@@ -31568,7 +31568,7 @@
         <v>1151</v>
       </c>
       <c r="C210">
-        <v>0.73204191959999998</v>
+        <v>0.74299742499999999</v>
       </c>
       <c r="E210" s="3">
         <f t="shared" si="3"/>
@@ -31583,7 +31583,7 @@
         <v>1171</v>
       </c>
       <c r="C211">
-        <v>0.72598789600000002</v>
+        <v>0.73711789029999997</v>
       </c>
       <c r="E211" s="3">
         <f t="shared" si="3"/>
@@ -31598,7 +31598,7 @@
         <v>1186</v>
       </c>
       <c r="C212">
-        <v>0.71982571309999999</v>
+        <v>0.73115367060000003</v>
       </c>
       <c r="E212" s="3">
         <f t="shared" si="3"/>
@@ -31613,7 +31613,7 @@
         <v>1224</v>
       </c>
       <c r="C213">
-        <v>0.71368232649999996</v>
+        <v>0.72519142640000001</v>
       </c>
       <c r="E213" s="3">
         <f t="shared" si="3"/>
@@ -31628,7 +31628,7 @@
         <v>1225</v>
       </c>
       <c r="C214">
-        <v>0.70744190959999997</v>
+        <v>0.71913837579999995</v>
       </c>
       <c r="E214" s="3">
         <f t="shared" si="3"/>
@@ -31643,7 +31643,7 @@
         <v>1293</v>
       </c>
       <c r="C215">
-        <v>0.70111442570000004</v>
+        <v>0.71301023249999995</v>
       </c>
       <c r="E215" s="3">
         <f t="shared" si="3"/>
@@ -31658,7 +31658,7 @@
         <v>1445</v>
       </c>
       <c r="C216">
-        <v>0.69437678110000001</v>
+        <v>0.70646509759999998</v>
       </c>
       <c r="E216" s="3">
         <f t="shared" si="3"/>
@@ -31673,7 +31673,7 @@
         <v>1582</v>
       </c>
       <c r="C217">
-        <v>0.68677771089999995</v>
+        <v>0.69910233519999998</v>
       </c>
       <c r="E217" s="3">
         <f t="shared" si="3"/>
@@ -31688,7 +31688,7 @@
         <v>1588</v>
       </c>
       <c r="C218">
-        <v>0.67916112920000005</v>
+        <v>0.69169601479999998</v>
       </c>
       <c r="E218" s="3">
         <f t="shared" si="3"/>
@@ -31703,7 +31703,7 @@
         <v>1662</v>
       </c>
       <c r="C219">
-        <v>0.6714740656</v>
+        <v>0.68423449589999996</v>
       </c>
       <c r="E219" s="3">
         <f t="shared" si="3"/>
@@ -31718,7 +31718,7 @@
         <v>1773</v>
       </c>
       <c r="C220">
-        <v>0.66362689929999996</v>
+        <v>0.67663608259999997</v>
       </c>
       <c r="E220" s="3">
         <f t="shared" si="3"/>
@@ -31733,7 +31733,7 @@
         <v>1806</v>
       </c>
       <c r="C221">
-        <v>0.65531951259999999</v>
+        <v>0.66859595449999998</v>
       </c>
       <c r="E221" s="3">
         <f t="shared" si="3"/>
@@ -31748,7 +31748,7 @@
         <v>1826</v>
       </c>
       <c r="C222">
-        <v>0.65531951259999999</v>
+        <v>0.66859595449999998</v>
       </c>
       <c r="E222" s="3">
         <f t="shared" si="3"/>
@@ -31777,7 +31777,7 @@
         <v>1</v>
       </c>
       <c r="C224">
-        <v>0.99807483990000001</v>
+        <v>0.99822328449999997</v>
       </c>
       <c r="E224" s="3">
         <f t="shared" si="3"/>
@@ -31792,7 +31792,7 @@
         <v>3</v>
       </c>
       <c r="C225">
-        <v>0.99614463779999995</v>
+        <v>0.99643769900000001</v>
       </c>
       <c r="E225" s="3">
         <f t="shared" si="3"/>
@@ -31807,7 +31807,7 @@
         <v>5</v>
       </c>
       <c r="C226">
-        <v>0.99421265400000003</v>
+        <v>0.99465019799999999</v>
       </c>
       <c r="E226" s="3">
         <f t="shared" si="3"/>
@@ -31822,7 +31822,7 @@
         <v>6</v>
       </c>
       <c r="C227">
-        <v>0.9922800651</v>
+        <v>0.9928608847</v>
       </c>
       <c r="E227" s="3">
         <f t="shared" si="3"/>
@@ -31837,7 +31837,7 @@
         <v>8</v>
       </c>
       <c r="C228">
-        <v>0.9903424448</v>
+        <v>0.99106883830000003</v>
       </c>
       <c r="E228" s="3">
         <f t="shared" si="3"/>
@@ -31852,7 +31852,7 @@
         <v>10</v>
       </c>
       <c r="C229">
-        <v>0.98840216609999998</v>
+        <v>0.98927371080000004</v>
       </c>
       <c r="E229" s="3">
         <f t="shared" si="3"/>
@@ -31867,7 +31867,7 @@
         <v>11</v>
       </c>
       <c r="C230">
-        <v>0.98645983410000004</v>
+        <v>0.98747507599999995</v>
       </c>
       <c r="E230" s="3">
         <f t="shared" si="3"/>
@@ -31882,7 +31882,7 @@
         <v>12</v>
       </c>
       <c r="C231">
-        <v>0.98450955429999998</v>
+        <v>0.98566890910000005</v>
       </c>
       <c r="E231" s="3">
         <f t="shared" si="3"/>
@@ -31897,7 +31897,7 @@
         <v>14</v>
       </c>
       <c r="C232">
-        <v>0.98059756149999999</v>
+        <v>0.98204815729999995</v>
       </c>
       <c r="E232" s="3">
         <f t="shared" si="3"/>
@@ -31912,7 +31912,7 @@
         <v>17</v>
       </c>
       <c r="C233">
-        <v>0.97665901450000003</v>
+        <v>0.97840048180000005</v>
       </c>
       <c r="E233" s="3">
         <f t="shared" si="3"/>
@@ -31927,7 +31927,7 @@
         <v>18</v>
       </c>
       <c r="C234">
-        <v>0.97270610329999996</v>
+        <v>0.97474568390000005</v>
       </c>
       <c r="E234" s="3">
         <f t="shared" si="3"/>
@@ -31942,7 +31942,7 @@
         <v>19</v>
       </c>
       <c r="C235">
-        <v>0.96677402960000003</v>
+        <v>0.96925919920000003</v>
       </c>
       <c r="E235" s="3">
         <f t="shared" si="3"/>
@@ -31957,7 +31957,7 @@
         <v>21</v>
       </c>
       <c r="C236">
-        <v>0.96477659829999995</v>
+        <v>0.96741790270000005</v>
       </c>
       <c r="E236" s="3">
         <f t="shared" si="3"/>
@@ -31972,7 +31972,7 @@
         <v>24</v>
       </c>
       <c r="C237">
-        <v>0.96077926179999995</v>
+        <v>0.96373202670000002</v>
       </c>
       <c r="E237" s="3">
         <f t="shared" si="3"/>
@@ -31987,7 +31987,7 @@
         <v>26</v>
       </c>
       <c r="C238">
-        <v>0.95877480169999996</v>
+        <v>0.96188435839999997</v>
       </c>
       <c r="E238" s="3">
         <f t="shared" si="3"/>
@@ -32002,7 +32002,7 @@
         <v>31</v>
       </c>
       <c r="C239">
-        <v>0.95675520889999999</v>
+        <v>0.96002263480000005</v>
       </c>
       <c r="E239" s="3">
         <f t="shared" si="3"/>
@@ -32017,7 +32017,7 @@
         <v>32</v>
       </c>
       <c r="C240">
-        <v>0.95271682089999998</v>
+        <v>0.95629910809999996</v>
       </c>
       <c r="E240" s="3">
         <f t="shared" si="3"/>
@@ -32032,7 +32032,7 @@
         <v>34</v>
       </c>
       <c r="C241">
-        <v>0.95069132980000004</v>
+        <v>0.95442967970000003</v>
       </c>
       <c r="E241" s="3">
         <f t="shared" si="3"/>
@@ -32047,7 +32047,7 @@
         <v>43</v>
       </c>
       <c r="C242">
-        <v>0.94864577589999999</v>
+        <v>0.95254054369999996</v>
       </c>
       <c r="E242" s="3">
         <f t="shared" si="3"/>
@@ -32062,7 +32062,7 @@
         <v>45</v>
       </c>
       <c r="C243">
-        <v>0.94659897059999998</v>
+        <v>0.95064929009999999</v>
       </c>
       <c r="E243" s="3">
         <f t="shared" si="3"/>
@@ -32077,7 +32077,7 @@
         <v>46</v>
       </c>
       <c r="C244">
-        <v>0.94455059590000001</v>
+        <v>0.94875756580000004</v>
       </c>
       <c r="E244" s="3">
         <f t="shared" si="3"/>
@@ -32092,7 +32092,7 @@
         <v>49</v>
       </c>
       <c r="C245">
-        <v>0.94044871819999998</v>
+        <v>0.94496553139999995</v>
       </c>
       <c r="E245" s="3">
         <f t="shared" si="3"/>
@@ -32107,7 +32107,7 @@
         <v>55</v>
       </c>
       <c r="C246">
-        <v>0.93838883559999997</v>
+        <v>0.94305899810000005</v>
       </c>
       <c r="E246" s="3">
         <f t="shared" si="3"/>
@@ -32122,7 +32122,7 @@
         <v>61</v>
       </c>
       <c r="C247">
-        <v>0.93632997159999998</v>
+        <v>0.94115235159999999</v>
       </c>
       <c r="E247" s="3">
         <f t="shared" si="3"/>
@@ -32137,7 +32137,7 @@
         <v>62</v>
       </c>
       <c r="C248">
-        <v>0.9342685557</v>
+        <v>0.93924318090000003</v>
       </c>
       <c r="E248" s="3">
         <f t="shared" si="3"/>
@@ -32152,7 +32152,7 @@
         <v>84</v>
       </c>
       <c r="C249">
-        <v>0.93219609790000002</v>
+        <v>0.93732315749999995</v>
       </c>
       <c r="E249" s="3">
         <f t="shared" si="3"/>
@@ -32167,7 +32167,7 @@
         <v>90</v>
       </c>
       <c r="C250">
-        <v>0.9300984981</v>
+        <v>0.93537604679999997</v>
       </c>
       <c r="E250" s="3">
         <f t="shared" si="3"/>
@@ -32182,7 +32182,7 @@
         <v>102</v>
       </c>
       <c r="C251">
-        <v>0.92794805400000002</v>
+        <v>0.93337817840000004</v>
       </c>
       <c r="E251" s="3">
         <f t="shared" si="3"/>
@@ -32197,7 +32197,7 @@
         <v>109</v>
       </c>
       <c r="C252">
-        <v>0.92579294339999996</v>
+        <v>0.93137676550000004</v>
       </c>
       <c r="E252" s="3">
         <f t="shared" si="3"/>
@@ -32212,7 +32212,7 @@
         <v>118</v>
       </c>
       <c r="C253">
-        <v>0.92362931749999999</v>
+        <v>0.92936628290000001</v>
       </c>
       <c r="E253" s="3">
         <f t="shared" si="3"/>
@@ -32227,7 +32227,7 @@
         <v>127</v>
       </c>
       <c r="C254">
-        <v>0.92146664109999998</v>
+        <v>0.92735618040000001</v>
       </c>
       <c r="E254" s="3">
         <f t="shared" si="3"/>
@@ -32242,7 +32242,7 @@
         <v>132</v>
       </c>
       <c r="C255">
-        <v>0.91930337399999995</v>
+        <v>0.92534422650000003</v>
       </c>
       <c r="E255" s="3">
         <f t="shared" si="3"/>
@@ -32257,7 +32257,7 @@
         <v>149</v>
       </c>
       <c r="C256">
-        <v>0.91713079770000006</v>
+        <v>0.92332069780000003</v>
       </c>
       <c r="E256" s="3">
         <f t="shared" si="3"/>
@@ -32272,7 +32272,7 @@
         <v>163</v>
       </c>
       <c r="C257">
-        <v>0.91494612809999998</v>
+        <v>0.92128873730000005</v>
       </c>
       <c r="E257" s="3">
         <f t="shared" si="3"/>
@@ -32287,7 +32287,7 @@
         <v>166</v>
       </c>
       <c r="C258">
-        <v>0.91056934730000005</v>
+        <v>0.9172157742</v>
       </c>
       <c r="E258" s="3">
         <f t="shared" si="3"/>
@@ -32302,7 +32302,7 @@
         <v>176</v>
       </c>
       <c r="C259">
-        <v>0.90836208409999997</v>
+        <v>0.91515791499999999</v>
       </c>
       <c r="E259" s="3">
         <f t="shared" si="3"/>
@@ -32317,7 +32317,7 @@
         <v>177</v>
       </c>
       <c r="C260">
-        <v>0.90614774210000004</v>
+        <v>0.91309391159999997</v>
       </c>
       <c r="E260" s="3">
         <f t="shared" si="3"/>
@@ -32332,7 +32332,7 @@
         <v>180</v>
       </c>
       <c r="C261">
-        <v>0.90392552879999999</v>
+        <v>0.91102387080000002</v>
       </c>
       <c r="E261" s="3">
         <f t="shared" si="3"/>
@@ -32347,7 +32347,7 @@
         <v>182</v>
       </c>
       <c r="C262">
-        <v>0.9016959202</v>
+        <v>0.90894871980000003</v>
       </c>
       <c r="E262" s="3">
         <f t="shared" si="3"/>
@@ -32362,7 +32362,7 @@
         <v>185</v>
       </c>
       <c r="C263">
-        <v>0.89946096610000004</v>
+        <v>0.90686712660000002</v>
       </c>
       <c r="E263" s="3">
         <f t="shared" si="3"/>
@@ -32377,7 +32377,7 @@
         <v>189</v>
       </c>
       <c r="C264">
-        <v>0.89722306269999996</v>
+        <v>0.90478227180000004</v>
       </c>
       <c r="E264" s="3">
         <f t="shared" si="3"/>
@@ -32392,7 +32392,7 @@
         <v>191</v>
       </c>
       <c r="C265">
-        <v>0.89498583480000005</v>
+        <v>0.90269619369999998</v>
       </c>
       <c r="E265" s="3">
         <f t="shared" si="3"/>
@@ -32407,7 +32407,7 @@
         <v>227</v>
       </c>
       <c r="C266">
-        <v>0.89274579080000005</v>
+        <v>0.90060766410000004</v>
       </c>
       <c r="E266" s="3">
         <f t="shared" si="3"/>
@@ -32422,7 +32422,7 @@
         <v>231</v>
       </c>
       <c r="C267">
-        <v>0.89048485570000002</v>
+        <v>0.89850252620000004</v>
       </c>
       <c r="E267" s="3">
         <f t="shared" si="3"/>
@@ -32437,7 +32437,7 @@
         <v>252</v>
       </c>
       <c r="C268">
-        <v>0.88821720729999998</v>
+        <v>0.89639285319999995</v>
       </c>
       <c r="E268" s="3">
         <f t="shared" si="3"/>
@@ -32452,7 +32452,7 @@
         <v>256</v>
       </c>
       <c r="C269">
-        <v>0.88594111860000002</v>
+        <v>0.89427591849999999</v>
       </c>
       <c r="E269" s="3">
         <f t="shared" si="3"/>
@@ -32467,7 +32467,7 @@
         <v>271</v>
       </c>
       <c r="C270">
-        <v>0.88366167709999999</v>
+        <v>0.89215725430000004</v>
       </c>
       <c r="E270" s="3">
         <f t="shared" si="3"/>
@@ -32482,7 +32482,7 @@
         <v>300</v>
       </c>
       <c r="C271">
-        <v>0.88137777809999995</v>
+        <v>0.89003385950000002</v>
       </c>
       <c r="E271" s="3">
         <f t="shared" si="3"/>
@@ -32497,7 +32497,7 @@
         <v>301</v>
       </c>
       <c r="C272">
-        <v>0.87908455559999998</v>
+        <v>0.88790398290000005</v>
       </c>
       <c r="E272" s="3">
         <f t="shared" ref="E272:E335" si="4">E271+1</f>
@@ -32512,7 +32512,7 @@
         <v>316</v>
       </c>
       <c r="C273">
-        <v>0.87677582949999999</v>
+        <v>0.88575710240000005</v>
       </c>
       <c r="E273" s="3">
         <f t="shared" si="4"/>
@@ -32527,7 +32527,7 @@
         <v>349</v>
       </c>
       <c r="C274">
-        <v>0.87445279539999998</v>
+        <v>0.88359839480000002</v>
       </c>
       <c r="E274" s="3">
         <f t="shared" si="4"/>
@@ -32542,7 +32542,7 @@
         <v>373</v>
       </c>
       <c r="C275">
-        <v>0.87198058249999999</v>
+        <v>0.8813143175</v>
       </c>
       <c r="E275" s="3">
         <f t="shared" si="4"/>
@@ -32557,7 +32557,7 @@
         <v>375</v>
       </c>
       <c r="C276">
-        <v>0.8694946657</v>
+        <v>0.87901920109999998</v>
       </c>
       <c r="E276" s="3">
         <f t="shared" si="4"/>
@@ -32572,7 +32572,7 @@
         <v>421</v>
       </c>
       <c r="C277">
-        <v>0.86693028989999998</v>
+        <v>0.87665212589999997</v>
       </c>
       <c r="E277" s="3">
         <f t="shared" si="4"/>
@@ -32587,7 +32587,7 @@
         <v>444</v>
       </c>
       <c r="C278">
-        <v>0.86435512680000004</v>
+        <v>0.87427690319999996</v>
       </c>
       <c r="E278" s="3">
         <f t="shared" si="4"/>
@@ -32602,7 +32602,7 @@
         <v>463</v>
       </c>
       <c r="C279">
-        <v>0.86178036420000004</v>
+        <v>0.87190112210000004</v>
       </c>
       <c r="E279" s="3">
         <f t="shared" si="4"/>
@@ -32617,7 +32617,7 @@
         <v>465</v>
       </c>
       <c r="C280">
-        <v>0.85918596250000001</v>
+        <v>0.8695009575</v>
       </c>
       <c r="E280" s="3">
         <f t="shared" si="4"/>
@@ -32632,7 +32632,7 @@
         <v>471</v>
       </c>
       <c r="C281">
-        <v>0.85657020530000005</v>
+        <v>0.86707915680000003</v>
       </c>
       <c r="E281" s="3">
         <f t="shared" si="4"/>
@@ -32647,7 +32647,7 @@
         <v>490</v>
       </c>
       <c r="C282">
-        <v>0.85394320759999998</v>
+        <v>0.86464920359999997</v>
       </c>
       <c r="E282" s="3">
         <f t="shared" si="4"/>
@@ -32662,7 +32662,7 @@
         <v>492</v>
       </c>
       <c r="C283">
-        <v>0.85130735769999999</v>
+        <v>0.86221332669999995</v>
       </c>
       <c r="E283" s="3">
         <f t="shared" si="4"/>
@@ -32677,7 +32677,7 @@
         <v>528</v>
       </c>
       <c r="C284">
-        <v>0.8486646095</v>
+        <v>0.85977017320000004</v>
       </c>
       <c r="E284" s="3">
         <f t="shared" si="4"/>
@@ -32692,7 +32692,7 @@
         <v>534</v>
       </c>
       <c r="C285">
-        <v>0.84601081440000003</v>
+        <v>0.8573142748</v>
       </c>
       <c r="E285" s="3">
         <f t="shared" si="4"/>
@@ -32707,7 +32707,7 @@
         <v>588</v>
       </c>
       <c r="C286">
-        <v>0.84335273129999999</v>
+        <v>0.85485448399999997</v>
       </c>
       <c r="E286" s="3">
         <f t="shared" si="4"/>
@@ -32722,7 +32722,7 @@
         <v>925</v>
       </c>
       <c r="C287">
-        <v>0.84000201649999995</v>
+        <v>0.85177727000000003</v>
       </c>
       <c r="E287" s="3">
         <f t="shared" si="4"/>
@@ -32737,7 +32737,7 @@
         <v>969</v>
       </c>
       <c r="C288">
-        <v>0.83661101569999996</v>
+        <v>0.84867178070000004</v>
       </c>
       <c r="E288" s="3">
         <f t="shared" si="4"/>
@@ -32752,7 +32752,7 @@
         <v>999</v>
       </c>
       <c r="C289">
-        <v>0.83310580209999996</v>
+        <v>0.84547471640000005</v>
       </c>
       <c r="E289" s="3">
         <f t="shared" si="4"/>
@@ -32767,7 +32767,7 @@
         <v>1032</v>
       </c>
       <c r="C290">
-        <v>0.8294747871</v>
+        <v>0.84216958850000001</v>
       </c>
       <c r="E290" s="3">
         <f t="shared" si="4"/>
@@ -32782,7 +32782,7 @@
         <v>1038</v>
       </c>
       <c r="C291">
-        <v>0.82579837339999995</v>
+        <v>0.8388198617</v>
       </c>
       <c r="E291" s="3">
         <f t="shared" si="4"/>
@@ -32797,7 +32797,7 @@
         <v>1049</v>
       </c>
       <c r="C292">
-        <v>0.82210554920000001</v>
+        <v>0.83544807430000001</v>
       </c>
       <c r="E292" s="3">
         <f t="shared" si="4"/>
@@ -32812,7 +32812,7 @@
         <v>1066</v>
       </c>
       <c r="C293">
-        <v>0.81836935219999996</v>
+        <v>0.83204344149999998</v>
       </c>
       <c r="E293" s="3">
         <f t="shared" si="4"/>
@@ -32827,7 +32827,7 @@
         <v>1087</v>
       </c>
       <c r="C294">
-        <v>0.8146078726</v>
+        <v>0.82861138020000003</v>
       </c>
       <c r="E294" s="3">
         <f t="shared" si="4"/>
@@ -32842,7 +32842,7 @@
         <v>1090</v>
       </c>
       <c r="C295">
-        <v>0.810813267</v>
+        <v>0.82514730960000005</v>
       </c>
       <c r="E295" s="3">
         <f t="shared" si="4"/>
@@ -32857,7 +32857,7 @@
         <v>1100</v>
       </c>
       <c r="C296">
-        <v>0.80700584230000005</v>
+        <v>0.82167182719999998</v>
       </c>
       <c r="E296" s="3">
         <f t="shared" si="4"/>
@@ -32872,7 +32872,7 @@
         <v>1107</v>
       </c>
       <c r="C297">
-        <v>0.8031437146</v>
+        <v>0.81814095249999996</v>
       </c>
       <c r="E297" s="3">
         <f t="shared" si="4"/>
@@ -32887,7 +32887,7 @@
         <v>1117</v>
       </c>
       <c r="C298">
-        <v>0.79925590420000003</v>
+        <v>0.81458832069999998</v>
       </c>
       <c r="E298" s="3">
         <f t="shared" si="4"/>
@@ -32902,7 +32902,7 @@
         <v>1191</v>
       </c>
       <c r="C299">
-        <v>0.79520018240000001</v>
+        <v>0.81090810120000001</v>
       </c>
       <c r="E299" s="3">
         <f t="shared" si="4"/>
@@ -32917,7 +32917,7 @@
         <v>1246</v>
       </c>
       <c r="C300">
-        <v>0.79112150349999999</v>
+        <v>0.80721030100000002</v>
       </c>
       <c r="E300" s="3">
         <f t="shared" si="4"/>
@@ -32932,7 +32932,7 @@
         <v>1410</v>
       </c>
       <c r="C301">
-        <v>0.78693607939999999</v>
+        <v>0.803405072</v>
       </c>
       <c r="E301" s="3">
         <f t="shared" si="4"/>
@@ -32947,7 +32947,7 @@
         <v>1440</v>
       </c>
       <c r="C302">
-        <v>0.78255506880000003</v>
+        <v>0.79942335129999997</v>
       </c>
       <c r="E302" s="3">
         <f t="shared" si="4"/>
@@ -32962,7 +32962,7 @@
         <v>1571</v>
       </c>
       <c r="C303">
-        <v>0.77788905659999996</v>
+        <v>0.79521596530000005</v>
       </c>
       <c r="E303" s="3">
         <f t="shared" si="4"/>
@@ -32977,7 +32977,7 @@
         <v>1606</v>
       </c>
       <c r="C304">
-        <v>0.77319790639999997</v>
+        <v>0.79099583029999998</v>
       </c>
       <c r="E304" s="3">
         <f t="shared" si="4"/>
@@ -32992,7 +32992,7 @@
         <v>1618</v>
       </c>
       <c r="C305">
-        <v>0.76850065089999997</v>
+        <v>0.78676793779999998</v>
       </c>
       <c r="E305" s="3">
         <f t="shared" si="4"/>
@@ -33007,7 +33007,7 @@
         <v>1678</v>
       </c>
       <c r="C306">
-        <v>0.76379160229999998</v>
+        <v>0.78253370460000005</v>
       </c>
       <c r="E306" s="3">
         <f t="shared" si="4"/>
@@ -33022,7 +33022,7 @@
         <v>1700</v>
       </c>
       <c r="C307">
-        <v>0.75904667000000003</v>
+        <v>0.7782642582</v>
       </c>
       <c r="E307" s="3">
         <f t="shared" si="4"/>
@@ -33037,7 +33037,7 @@
         <v>1796</v>
       </c>
       <c r="C308">
-        <v>0.7540464791</v>
+        <v>0.77378174690000001</v>
       </c>
       <c r="E308" s="3">
         <f t="shared" si="4"/>
@@ -33052,7 +33052,7 @@
         <v>1807</v>
       </c>
       <c r="C309">
-        <v>0.74904086989999996</v>
+        <v>0.76928884220000004</v>
       </c>
       <c r="E309" s="3">
         <f t="shared" si="4"/>
@@ -33067,7 +33067,7 @@
         <v>1808</v>
       </c>
       <c r="C310">
-        <v>0.74397319740000001</v>
+        <v>0.76472526620000003</v>
       </c>
       <c r="E310" s="3">
         <f t="shared" si="4"/>
@@ -33082,7 +33082,7 @@
         <v>1826</v>
       </c>
       <c r="C311">
-        <v>0.74397319740000001</v>
+        <v>0.76472526620000003</v>
       </c>
       <c r="E311" s="3">
         <f t="shared" si="4"/>
@@ -33111,7 +33111,7 @@
         <v>0</v>
       </c>
       <c r="C313">
-        <v>0.98943296199999997</v>
+        <v>0.99022890070000003</v>
       </c>
       <c r="E313" s="3">
         <f t="shared" si="4"/>
@@ -33126,7 +33126,7 @@
         <v>3</v>
       </c>
       <c r="C314">
-        <v>0.98672631349999995</v>
+        <v>0.98773943109999995</v>
       </c>
       <c r="E314" s="3">
         <f t="shared" si="4"/>
@@ -33141,7 +33141,7 @@
         <v>6</v>
       </c>
       <c r="C315">
-        <v>0.98400964759999998</v>
+        <v>0.98524048190000002</v>
       </c>
       <c r="E315" s="3">
         <f t="shared" si="4"/>
@@ -33156,7 +33156,7 @@
         <v>12</v>
       </c>
       <c r="C316">
-        <v>0.98128420910000003</v>
+        <v>0.98273183490000005</v>
       </c>
       <c r="E316" s="3">
         <f t="shared" si="4"/>
@@ -33171,7 +33171,7 @@
         <v>16</v>
       </c>
       <c r="C317">
-        <v>0.97583883940000005</v>
+        <v>0.97771445450000005</v>
       </c>
       <c r="E317" s="3">
         <f t="shared" si="4"/>
@@ -33186,7 +33186,7 @@
         <v>19</v>
       </c>
       <c r="C318">
-        <v>0.97309428710000001</v>
+        <v>0.97519127549999995</v>
       </c>
       <c r="E318" s="3">
         <f t="shared" si="4"/>
@@ -33201,7 +33201,7 @@
         <v>25</v>
       </c>
       <c r="C319">
-        <v>0.97034545329999999</v>
+        <v>0.97266268280000001</v>
       </c>
       <c r="E319" s="3">
         <f t="shared" si="4"/>
@@ -33216,7 +33216,7 @@
         <v>33</v>
       </c>
       <c r="C320">
-        <v>0.96759356969999999</v>
+        <v>0.97013074450000003</v>
       </c>
       <c r="E320" s="3">
         <f t="shared" si="4"/>
@@ -33231,7 +33231,7 @@
         <v>47</v>
       </c>
       <c r="C321">
-        <v>0.96483392909999999</v>
+        <v>0.96759424429999996</v>
       </c>
       <c r="E321" s="3">
         <f t="shared" si="4"/>
@@ -33246,7 +33246,7 @@
         <v>48</v>
       </c>
       <c r="C322">
-        <v>0.96206254570000005</v>
+        <v>0.96504996340000004</v>
       </c>
       <c r="E322" s="3">
         <f t="shared" si="4"/>
@@ -33261,7 +33261,7 @@
         <v>66</v>
       </c>
       <c r="C323">
-        <v>0.95928305339999997</v>
+        <v>0.96249545830000005</v>
       </c>
       <c r="E323" s="3">
         <f t="shared" si="4"/>
@@ -33276,7 +33276,7 @@
         <v>81</v>
       </c>
       <c r="C324">
-        <v>0.95650065429999998</v>
+        <v>0.95993792909999998</v>
       </c>
       <c r="E324" s="3">
         <f t="shared" si="4"/>
@@ -33291,7 +33291,7 @@
         <v>82</v>
       </c>
       <c r="C325">
-        <v>0.95370618279999997</v>
+        <v>0.95736761420000005</v>
       </c>
       <c r="E325" s="3">
         <f t="shared" si="4"/>
@@ -33306,7 +33306,7 @@
         <v>87</v>
       </c>
       <c r="C326">
-        <v>0.95091070200000005</v>
+        <v>0.95479496890000004</v>
       </c>
       <c r="E326" s="3">
         <f t="shared" si="4"/>
@@ -33321,7 +33321,7 @@
         <v>91</v>
       </c>
       <c r="C327">
-        <v>0.94811503809999997</v>
+        <v>0.95222055839999997</v>
       </c>
       <c r="E327" s="3">
         <f t="shared" si="4"/>
@@ -33336,7 +33336,7 @@
         <v>94</v>
       </c>
       <c r="C328">
-        <v>0.94531149290000005</v>
+        <v>0.94963708690000004</v>
       </c>
       <c r="E328" s="3">
         <f t="shared" si="4"/>
@@ -33351,7 +33351,7 @@
         <v>95</v>
       </c>
       <c r="C329">
-        <v>0.94250315770000004</v>
+        <v>0.94704827270000003</v>
       </c>
       <c r="E329" s="3">
         <f t="shared" si="4"/>
@@ -33366,7 +33366,7 @@
         <v>99</v>
       </c>
       <c r="C330">
-        <v>0.93687696440000001</v>
+        <v>0.94186336130000003</v>
       </c>
       <c r="E330" s="3">
         <f t="shared" si="4"/>
@@ -33381,7 +33381,7 @@
         <v>104</v>
       </c>
       <c r="C331">
-        <v>0.93404134630000002</v>
+        <v>0.93924749829999998</v>
       </c>
       <c r="E331" s="3">
         <f t="shared" si="4"/>
@@ -33396,7 +33396,7 @@
         <v>119</v>
       </c>
       <c r="C332">
-        <v>0.93120341230000003</v>
+        <v>0.93662890200000004</v>
       </c>
       <c r="E332" s="3">
         <f t="shared" si="4"/>
@@ -33411,7 +33411,7 @@
         <v>128</v>
       </c>
       <c r="C333">
-        <v>0.92834474629999997</v>
+        <v>0.93399187439999998</v>
       </c>
       <c r="E333" s="3">
         <f t="shared" si="4"/>
@@ -33426,7 +33426,7 @@
         <v>137</v>
       </c>
       <c r="C334">
-        <v>0.92547921129999999</v>
+        <v>0.93134824199999999</v>
       </c>
       <c r="E334" s="3">
         <f t="shared" si="4"/>
@@ -33441,7 +33441,7 @@
         <v>140</v>
       </c>
       <c r="C335">
-        <v>0.92260480899999997</v>
+        <v>0.92869571149999997</v>
       </c>
       <c r="E335" s="3">
         <f t="shared" si="4"/>
@@ -33456,7 +33456,7 @@
         <v>145</v>
       </c>
       <c r="C336">
-        <v>0.91972684159999996</v>
+        <v>0.92603334289999994</v>
       </c>
       <c r="E336" s="3">
         <f t="shared" ref="E336:E399" si="5">E335+1</f>
@@ -33471,7 +33471,7 @@
         <v>150</v>
       </c>
       <c r="C337">
-        <v>0.91684388080000001</v>
+        <v>0.92336640599999997</v>
       </c>
       <c r="E337" s="3">
         <f t="shared" si="5"/>
@@ -33486,7 +33486,7 @@
         <v>184</v>
       </c>
       <c r="C338">
-        <v>0.91395834450000002</v>
+        <v>0.92069476729999999</v>
       </c>
       <c r="E338" s="3">
         <f t="shared" si="5"/>
@@ -33501,7 +33501,7 @@
         <v>189</v>
       </c>
       <c r="C339">
-        <v>0.91107430379999998</v>
+        <v>0.91802462659999995</v>
       </c>
       <c r="E339" s="3">
         <f t="shared" si="5"/>
@@ -33516,7 +33516,7 @@
         <v>196</v>
       </c>
       <c r="C340">
-        <v>0.90818642940000005</v>
+        <v>0.9153488783</v>
       </c>
       <c r="E340" s="3">
         <f t="shared" si="5"/>
@@ -33531,7 +33531,7 @@
         <v>198</v>
       </c>
       <c r="C341">
-        <v>0.90527723640000002</v>
+        <v>0.91265288119999999</v>
       </c>
       <c r="E341" s="3">
         <f t="shared" si="5"/>
@@ -33546,7 +33546,7 @@
         <v>208</v>
       </c>
       <c r="C342">
-        <v>0.9023679081</v>
+        <v>0.90995381269999998</v>
       </c>
       <c r="E342" s="3">
         <f t="shared" si="5"/>
@@ -33561,7 +33561,7 @@
         <v>238</v>
       </c>
       <c r="C343">
-        <v>0.89945280800000005</v>
+        <v>0.9072503864</v>
       </c>
       <c r="E343" s="3">
         <f t="shared" si="5"/>
@@ -33576,7 +33576,7 @@
         <v>240</v>
       </c>
       <c r="C344">
-        <v>0.89652608690000002</v>
+        <v>0.90453807909999995</v>
       </c>
       <c r="E344" s="3">
         <f t="shared" si="5"/>
@@ -33591,7 +33591,7 @@
         <v>244</v>
       </c>
       <c r="C345">
-        <v>0.89359429739999996</v>
+        <v>0.90181552539999998</v>
       </c>
       <c r="E345" s="3">
         <f t="shared" si="5"/>
@@ -33606,7 +33606,7 @@
         <v>256</v>
       </c>
       <c r="C346">
-        <v>0.89066077290000001</v>
+        <v>0.89909226760000005</v>
       </c>
       <c r="E346" s="3">
         <f t="shared" si="5"/>
@@ -33621,7 +33621,7 @@
         <v>268</v>
       </c>
       <c r="C347">
-        <v>0.88771888080000005</v>
+        <v>0.89635411789999997</v>
       </c>
       <c r="E347" s="3">
         <f t="shared" si="5"/>
@@ -33636,7 +33636,7 @@
         <v>307</v>
       </c>
       <c r="C348">
-        <v>0.88477289020000005</v>
+        <v>0.89361145399999997</v>
       </c>
       <c r="E348" s="3">
         <f t="shared" si="5"/>
@@ -33651,7 +33651,7 @@
         <v>323</v>
       </c>
       <c r="C349">
-        <v>0.88180952280000002</v>
+        <v>0.89086674320000003</v>
       </c>
       <c r="E349" s="3">
         <f t="shared" si="5"/>
@@ -33666,7 +33666,7 @@
         <v>324</v>
       </c>
       <c r="C350">
-        <v>0.87883420239999999</v>
+        <v>0.88810333379999995</v>
       </c>
       <c r="E350" s="3">
         <f t="shared" si="5"/>
@@ -33681,7 +33681,7 @@
         <v>343</v>
       </c>
       <c r="C351">
-        <v>0.8758402488</v>
+        <v>0.88531409809999995</v>
       </c>
       <c r="E351" s="3">
         <f t="shared" si="5"/>
@@ -33696,7 +33696,7 @@
         <v>349</v>
       </c>
       <c r="C352">
-        <v>0.87284762930000004</v>
+        <v>0.88252656029999998</v>
       </c>
       <c r="E352" s="3">
         <f t="shared" si="5"/>
@@ -33711,7 +33711,7 @@
         <v>350</v>
       </c>
       <c r="C353">
-        <v>0.86686468000000005</v>
+        <v>0.87694961370000002</v>
       </c>
       <c r="E353" s="3">
         <f t="shared" si="5"/>
@@ -33726,7 +33726,7 @@
         <v>373</v>
       </c>
       <c r="C354">
-        <v>0.86383028989999999</v>
+        <v>0.87412092360000004</v>
       </c>
       <c r="E354" s="3">
         <f t="shared" si="5"/>
@@ -33741,7 +33741,7 @@
         <v>385</v>
       </c>
       <c r="C355">
-        <v>0.86073009489999996</v>
+        <v>0.87123842070000002</v>
       </c>
       <c r="E355" s="3">
         <f t="shared" si="5"/>
@@ -33756,7 +33756,7 @@
         <v>448</v>
       </c>
       <c r="C356">
-        <v>0.85758750039999998</v>
+        <v>0.86831415980000004</v>
       </c>
       <c r="E356" s="3">
         <f t="shared" si="5"/>
@@ -33771,7 +33771,7 @@
         <v>458</v>
       </c>
       <c r="C357">
-        <v>0.85443986910000003</v>
+        <v>0.86538318359999999</v>
       </c>
       <c r="E357" s="3">
         <f t="shared" si="5"/>
@@ -33786,7 +33786,7 @@
         <v>473</v>
       </c>
       <c r="C358">
-        <v>0.85128537969999996</v>
+        <v>0.86244597840000004</v>
       </c>
       <c r="E358" s="3">
         <f t="shared" si="5"/>
@@ -33801,7 +33801,7 @@
         <v>478</v>
       </c>
       <c r="C359">
-        <v>0.848119179</v>
+        <v>0.859489014</v>
       </c>
       <c r="E359" s="3">
         <f t="shared" si="5"/>
@@ -33816,7 +33816,7 @@
         <v>482</v>
       </c>
       <c r="C360">
-        <v>0.84493276969999997</v>
+        <v>0.85651108679999999</v>
       </c>
       <c r="E360" s="3">
         <f t="shared" si="5"/>
@@ -33831,7 +33831,7 @@
         <v>487</v>
       </c>
       <c r="C361">
-        <v>0.84174107419999999</v>
+        <v>0.85352748310000004</v>
       </c>
       <c r="E361" s="3">
         <f t="shared" si="5"/>
@@ -33846,7 +33846,7 @@
         <v>491</v>
       </c>
       <c r="C362">
-        <v>0.83854794050000003</v>
+        <v>0.85054011910000005</v>
       </c>
       <c r="E362" s="3">
         <f t="shared" si="5"/>
@@ -33861,7 +33861,7 @@
         <v>507</v>
       </c>
       <c r="C363">
-        <v>0.83535590589999997</v>
+        <v>0.84755215539999995</v>
       </c>
       <c r="E363" s="3">
         <f t="shared" si="5"/>
@@ -33876,7 +33876,7 @@
         <v>524</v>
       </c>
       <c r="C364">
-        <v>0.82895314019999999</v>
+        <v>0.84155982979999999</v>
       </c>
       <c r="E364" s="3">
         <f t="shared" si="5"/>
@@ -33891,7 +33891,7 @@
         <v>535</v>
       </c>
       <c r="C365">
-        <v>0.82572515120000001</v>
+        <v>0.83853677140000005</v>
       </c>
       <c r="E365" s="3">
         <f t="shared" si="5"/>
@@ -33906,7 +33906,7 @@
         <v>543</v>
       </c>
       <c r="C366">
-        <v>0.82249086859999998</v>
+        <v>0.83550792460000001</v>
       </c>
       <c r="E366" s="3">
         <f t="shared" si="5"/>
@@ -33921,7 +33921,7 @@
         <v>579</v>
       </c>
       <c r="C367">
-        <v>0.81924852719999997</v>
+        <v>0.83246744039999998</v>
       </c>
       <c r="E367" s="3">
         <f t="shared" si="5"/>
@@ -33936,7 +33936,7 @@
         <v>603</v>
       </c>
       <c r="C368">
-        <v>0.81600485010000001</v>
+        <v>0.82942695619999995</v>
       </c>
       <c r="E368" s="3">
         <f t="shared" si="5"/>
@@ -33951,7 +33951,7 @@
         <v>613</v>
       </c>
       <c r="C369">
-        <v>0.81275541350000002</v>
+        <v>0.82637887050000003</v>
       </c>
       <c r="E369" s="3">
         <f t="shared" si="5"/>
@@ -33966,7 +33966,7 @@
         <v>621</v>
       </c>
       <c r="C370">
-        <v>0.80947892330000004</v>
+        <v>0.82330777420000001</v>
       </c>
       <c r="E370" s="3">
         <f t="shared" si="5"/>
@@ -33981,7 +33981,7 @@
         <v>654</v>
       </c>
       <c r="C371">
-        <v>0.80617306060000005</v>
+        <v>0.82020171980000001</v>
       </c>
       <c r="E371" s="3">
         <f t="shared" si="5"/>
@@ -33996,7 +33996,7 @@
         <v>667</v>
       </c>
       <c r="C372">
-        <v>0.80285194780000002</v>
+        <v>0.81707217600000004</v>
       </c>
       <c r="E372" s="3">
         <f t="shared" si="5"/>
@@ -34011,7 +34011,7 @@
         <v>685</v>
       </c>
       <c r="C373">
-        <v>0.79945583730000003</v>
+        <v>0.81388394070000003</v>
       </c>
       <c r="E373" s="3">
         <f t="shared" si="5"/>
@@ -34026,7 +34026,7 @@
         <v>721</v>
       </c>
       <c r="C374">
-        <v>0.7924297897</v>
+        <v>0.80731364790000004</v>
       </c>
       <c r="E374" s="3">
         <f t="shared" si="5"/>
@@ -34041,7 +34041,7 @@
         <v>789</v>
       </c>
       <c r="C375">
-        <v>0.78872848090000003</v>
+        <v>0.80385707679999996</v>
       </c>
       <c r="E375" s="3">
         <f t="shared" si="5"/>
@@ -34056,7 +34056,7 @@
         <v>821</v>
       </c>
       <c r="C376">
-        <v>0.78496136459999999</v>
+        <v>0.80033978130000005</v>
       </c>
       <c r="E376" s="3">
         <f t="shared" si="5"/>
@@ -34071,7 +34071,7 @@
         <v>849</v>
       </c>
       <c r="C377">
-        <v>0.78114866169999997</v>
+        <v>0.79678670709999999</v>
       </c>
       <c r="E377" s="3">
         <f t="shared" si="5"/>
@@ -34086,7 +34086,7 @@
         <v>859</v>
       </c>
       <c r="C378">
-        <v>0.77733234699999998</v>
+        <v>0.79322726870000004</v>
       </c>
       <c r="E378" s="3">
         <f t="shared" si="5"/>
@@ -34101,7 +34101,7 @@
         <v>861</v>
       </c>
       <c r="C379">
-        <v>0.77349066700000002</v>
+        <v>0.78962781900000001</v>
       </c>
       <c r="E379" s="3">
         <f t="shared" si="5"/>
@@ -34116,7 +34116,7 @@
         <v>880</v>
       </c>
       <c r="C380">
-        <v>0.7696446509</v>
+        <v>0.78602025939999998</v>
       </c>
       <c r="E380" s="3">
         <f t="shared" si="5"/>
@@ -34131,7 +34131,7 @@
         <v>899</v>
       </c>
       <c r="C381">
-        <v>0.76578001620000002</v>
+        <v>0.78238555939999999</v>
       </c>
       <c r="E381" s="3">
         <f t="shared" si="5"/>
@@ -34146,7 +34146,7 @@
         <v>923</v>
       </c>
       <c r="C382">
-        <v>0.76187479709999995</v>
+        <v>0.77871336729999996</v>
       </c>
       <c r="E382" s="3">
         <f t="shared" si="5"/>
@@ -34161,7 +34161,7 @@
         <v>944</v>
       </c>
       <c r="C383">
-        <v>0.757960678</v>
+        <v>0.77503139359999995</v>
       </c>
       <c r="E383" s="3">
         <f t="shared" si="5"/>
@@ -34176,7 +34176,7 @@
         <v>1027</v>
       </c>
       <c r="C384">
-        <v>0.75402285920000001</v>
+        <v>0.77132617660000002</v>
       </c>
       <c r="E384" s="3">
         <f t="shared" si="5"/>
@@ -34191,7 +34191,7 @@
         <v>1126</v>
       </c>
       <c r="C385">
-        <v>0.74941173979999998</v>
+        <v>0.76702642470000004</v>
       </c>
       <c r="E385" s="3">
         <f t="shared" si="5"/>
@@ -34206,7 +34206,7 @@
         <v>1127</v>
       </c>
       <c r="C386">
-        <v>0.74478197960000003</v>
+        <v>0.76270204190000002</v>
       </c>
       <c r="E386" s="3">
         <f t="shared" si="5"/>
@@ -34221,7 +34221,7 @@
         <v>1289</v>
       </c>
       <c r="C387">
-        <v>0.74006926179999999</v>
+        <v>0.75830302979999997</v>
       </c>
       <c r="E387" s="3">
         <f t="shared" si="5"/>
@@ -34236,7 +34236,7 @@
         <v>1335</v>
       </c>
       <c r="C388">
-        <v>0.73530327090000003</v>
+        <v>0.75385839939999999</v>
       </c>
       <c r="E388" s="3">
         <f t="shared" si="5"/>
@@ -34251,7 +34251,7 @@
         <v>1353</v>
       </c>
       <c r="C389">
-        <v>0.73049251869999998</v>
+        <v>0.74939363520000002</v>
       </c>
       <c r="E389" s="3">
         <f t="shared" si="5"/>
@@ -34266,7 +34266,7 @@
         <v>1361</v>
       </c>
       <c r="C390">
-        <v>0.72565997189999998</v>
+        <v>0.74489552370000001</v>
       </c>
       <c r="E390" s="3">
         <f t="shared" si="5"/>
@@ -34281,7 +34281,7 @@
         <v>1408</v>
       </c>
       <c r="C391">
-        <v>0.72081000090000003</v>
+        <v>0.74036438459999998</v>
       </c>
       <c r="E391" s="3">
         <f t="shared" si="5"/>
@@ -34296,7 +34296,7 @@
         <v>1418</v>
       </c>
       <c r="C392">
-        <v>0.71593626659999998</v>
+        <v>0.73579445399999999</v>
       </c>
       <c r="E392" s="3">
         <f t="shared" si="5"/>
@@ -34311,7 +34311,7 @@
         <v>1468</v>
       </c>
       <c r="C393">
-        <v>0.71051999030000002</v>
+        <v>0.73066556920000003</v>
       </c>
       <c r="E393" s="3">
         <f t="shared" si="5"/>
@@ -34326,7 +34326,7 @@
         <v>1512</v>
       </c>
       <c r="C394">
-        <v>0.70472944429999995</v>
+        <v>0.72516744119999998</v>
       </c>
       <c r="E394" s="3">
         <f t="shared" si="5"/>
@@ -34341,7 +34341,7 @@
         <v>1554</v>
       </c>
       <c r="C395">
-        <v>0.69840503470000004</v>
+        <v>0.71913538399999999</v>
       </c>
       <c r="E395" s="3">
         <f t="shared" si="5"/>
@@ -34356,7 +34356,7 @@
         <v>1562</v>
       </c>
       <c r="C396">
-        <v>0.69206540380000003</v>
+        <v>0.71308995350000004</v>
       </c>
       <c r="E396" s="3">
         <f t="shared" si="5"/>
@@ -34371,7 +34371,7 @@
         <v>1624</v>
       </c>
       <c r="C397">
-        <v>0.68568955070000004</v>
+        <v>0.70700655290000003</v>
       </c>
       <c r="E397" s="3">
         <f t="shared" si="5"/>
@@ -34386,7 +34386,7 @@
         <v>1790</v>
       </c>
       <c r="C398">
-        <v>0.67910143560000003</v>
+        <v>0.70066076509999997</v>
       </c>
       <c r="E398" s="3">
         <f t="shared" si="5"/>
@@ -34401,7 +34401,7 @@
         <v>1815</v>
       </c>
       <c r="C399">
-        <v>0.67239715440000003</v>
+        <v>0.69415153549999997</v>
       </c>
       <c r="E399" s="3">
         <f t="shared" si="5"/>
@@ -34416,7 +34416,7 @@
         <v>1826</v>
       </c>
       <c r="C400">
-        <v>0.67239715440000003</v>
+        <v>0.69415153549999997</v>
       </c>
       <c r="E400" s="3">
         <f t="shared" ref="E400" si="6">E399+1</f>

</xml_diff>

<commit_message>
lung xslx++, simple all-required counting fix
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{098A13B2-24D6-BF44-AA10-E0FFA4503AE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C889ADE-2118-EF4C-A724-96C07D5B3C06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="65900" yWindow="4180" windowWidth="23700" windowHeight="21040" firstSheet="4" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="61180" yWindow="4180" windowWidth="27700" windowHeight="21040" firstSheet="5" activeTab="8" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2211" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="233">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -754,7 +754,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -785,12 +785,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -866,10 +860,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -968,8 +962,8 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1001,7 +995,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1018,16 +1011,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1421,13 +1414,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:J65"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="E2" sqref="E2:E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" style="3" customWidth="1"/>
@@ -1437,11 +1430,12 @@
     <col min="6" max="6" width="17.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
     <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.83203125" style="3"/>
+    <col min="10" max="10" width="15" style="32" customWidth="1"/>
+    <col min="11" max="11" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1469,11 +1463,14 @@
       <c r="I1" s="41" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>84</v>
       </c>
@@ -1498,9 +1495,12 @@
       <c r="I2" s="40">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>84</v>
       </c>
@@ -1512,23 +1512,26 @@
         <v>71</v>
       </c>
       <c r="E3">
-        <v>0.28404000000000001</v>
+        <v>0.29226000000000002</v>
       </c>
       <c r="I3" s="40">
         <v>2.2999999999999998</v>
       </c>
-      <c r="J3" s="8"/>
-    </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="26"/>
       <c r="D4" s="10"/>
       <c r="E4"/>
       <c r="I4" s="40"/>
-      <c r="J4" s="8"/>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>87</v>
       </c>
@@ -1553,11 +1556,14 @@
       <c r="I5" s="40">
         <v>2.1</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>87</v>
       </c>
@@ -1569,32 +1575,35 @@
         <v>36</v>
       </c>
       <c r="E6">
-        <v>0.23224</v>
+        <v>0.24582000000000001</v>
       </c>
       <c r="I6" s="40">
         <v>2.1</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="26"/>
       <c r="D7" s="10"/>
       <c r="E7"/>
       <c r="I7" s="40"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="64" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="14" t="s">
@@ -1609,28 +1618,34 @@
       <c r="I8" s="40">
         <v>1.4</v>
       </c>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="63"/>
+      <c r="C9" s="64"/>
       <c r="D9" s="17" t="s">
         <v>198</v>
       </c>
       <c r="E9">
-        <v>0.28171000000000002</v>
+        <v>0.27340999999999999</v>
       </c>
       <c r="I9" s="40">
         <v>1.4</v>
       </c>
-      <c r="J9" s="8"/>
-    </row>
-    <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J9" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>57</v>
       </c>
@@ -1642,23 +1657,26 @@
         <v>199</v>
       </c>
       <c r="E10">
-        <v>0.48797000000000001</v>
+        <v>0.48875999999999997</v>
       </c>
       <c r="I10" s="40">
         <v>1.4</v>
       </c>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J10" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="26"/>
       <c r="D11" s="10"/>
       <c r="E11"/>
       <c r="I11" s="40"/>
-      <c r="J11" s="8"/>
-    </row>
-    <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
@@ -1672,7 +1690,7 @@
         <v>83</v>
       </c>
       <c r="E12">
-        <v>6.3950000000000007E-2</v>
+        <v>4.9770000000000002E-2</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>141</v>
@@ -1680,9 +1698,12 @@
       <c r="I12" s="40">
         <v>1.6</v>
       </c>
-      <c r="J12" s="8"/>
-    </row>
-    <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J12" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
@@ -1699,18 +1720,21 @@
       <c r="I13" s="40">
         <v>1.6</v>
       </c>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="26"/>
       <c r="D14" s="10"/>
       <c r="E14"/>
       <c r="I14" s="40"/>
-      <c r="J14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>66</v>
       </c>
@@ -1724,7 +1748,7 @@
         <v>62</v>
       </c>
       <c r="E15">
-        <v>-0.65693000000000001</v>
+        <v>-0.40421000000000001</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>141</v>
@@ -1733,9 +1757,12 @@
       <c r="I15" s="40">
         <v>1.7</v>
       </c>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J15" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
         <v>66</v>
       </c>
@@ -1747,15 +1774,18 @@
         <v>48</v>
       </c>
       <c r="E16">
-        <v>0.17297000000000001</v>
+        <v>0.20102</v>
       </c>
       <c r="G16" s="10"/>
       <c r="I16" s="40">
         <v>1.7</v>
       </c>
-      <c r="J16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>66</v>
       </c>
@@ -1767,15 +1797,18 @@
         <v>63</v>
       </c>
       <c r="E17">
-        <v>-1.486E-2</v>
+        <v>4.8410000000000002E-2</v>
       </c>
       <c r="G17" s="10"/>
       <c r="I17" s="40">
         <v>1.7</v>
       </c>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>66</v>
       </c>
@@ -1793,18 +1826,21 @@
       <c r="I18" s="40">
         <v>1.7</v>
       </c>
-      <c r="J18" s="8"/>
-    </row>
-    <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J18" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="26"/>
       <c r="D19" s="10"/>
       <c r="E19"/>
       <c r="I19" s="40"/>
-      <c r="J19" s="8"/>
-    </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>214</v>
       </c>
@@ -1814,7 +1850,7 @@
       <c r="C20" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="58" t="s">
         <v>176</v>
       </c>
       <c r="E20">
@@ -1829,27 +1865,33 @@
       <c r="I20" s="40">
         <v>1.2</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K20" s="8" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>214</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="58" t="s">
         <v>177</v>
       </c>
       <c r="E21">
         <v>-5.6439999999999997E-2</v>
       </c>
       <c r="I21" s="40"/>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J21" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>214</v>
       </c>
@@ -1857,16 +1899,19 @@
         <v>183</v>
       </c>
       <c r="C22" s="31"/>
-      <c r="D22" s="59" t="s">
+      <c r="D22" s="58" t="s">
         <v>178</v>
       </c>
       <c r="E22">
         <v>-5.0889999999999998E-2</v>
       </c>
       <c r="I22" s="40"/>
-      <c r="J22" s="8"/>
-    </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J22" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>214</v>
       </c>
@@ -1874,42 +1919,48 @@
         <v>184</v>
       </c>
       <c r="C23" s="31"/>
-      <c r="D23" s="59" t="s">
+      <c r="D23" s="58" t="s">
         <v>179</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="I23" s="40"/>
-      <c r="J23" s="8"/>
-    </row>
-    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J23" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>214</v>
       </c>
       <c r="B24" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="59" t="s">
+      <c r="C24" s="56"/>
+      <c r="D24" s="58" t="s">
         <v>180</v>
       </c>
       <c r="E24">
         <v>0.22292000000000001</v>
       </c>
       <c r="I24" s="40"/>
-      <c r="J24" s="8"/>
-    </row>
-    <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J24" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="26"/>
       <c r="D25" s="27"/>
       <c r="E25"/>
       <c r="I25" s="40"/>
-      <c r="J25" s="8"/>
-    </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>89</v>
       </c>
@@ -1919,7 +1970,7 @@
       <c r="C26" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="58" t="s">
+      <c r="D26" s="57" t="s">
         <v>203</v>
       </c>
       <c r="E26">
@@ -1931,9 +1982,12 @@
       <c r="I26" s="40">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J26" s="8"/>
-    </row>
-    <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J26" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>89</v>
       </c>
@@ -1941,7 +1995,7 @@
         <v>201</v>
       </c>
       <c r="C27" s="26"/>
-      <c r="D27" s="58" t="s">
+      <c r="D27" s="57" t="s">
         <v>205</v>
       </c>
       <c r="E27">
@@ -1949,9 +2003,12 @@
       </c>
       <c r="F27" s="47"/>
       <c r="I27" s="40"/>
-      <c r="J27" s="8"/>
-    </row>
-    <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J27" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>89</v>
       </c>
@@ -1959,7 +2016,7 @@
         <v>202</v>
       </c>
       <c r="C28" s="26"/>
-      <c r="D28" s="58" t="s">
+      <c r="D28" s="57" t="s">
         <v>204</v>
       </c>
       <c r="E28">
@@ -1967,9 +2024,12 @@
       </c>
       <c r="F28" s="47"/>
       <c r="I28" s="40"/>
-      <c r="J28" s="8"/>
-    </row>
-    <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J28" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="26"/>
@@ -1977,9 +2037,9 @@
       <c r="E29"/>
       <c r="F29" s="47"/>
       <c r="I29" s="40"/>
-      <c r="J29" s="8"/>
-    </row>
-    <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>52</v>
       </c>
@@ -2004,9 +2064,12 @@
       <c r="I30" s="40">
         <v>1.5</v>
       </c>
-      <c r="J30" s="8"/>
-    </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J30" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>52</v>
       </c>
@@ -2020,9 +2083,12 @@
         <v>-1.281E-2</v>
       </c>
       <c r="I31" s="40"/>
-      <c r="J31" s="8"/>
-    </row>
-    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J31" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>52</v>
       </c>
@@ -2036,9 +2102,12 @@
         <v>0</v>
       </c>
       <c r="I32" s="40"/>
-      <c r="J32" s="8"/>
-    </row>
-    <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J32" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" s="8"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>52</v>
       </c>
@@ -2052,276 +2121,301 @@
         <v>-0.26149</v>
       </c>
       <c r="I33" s="40"/>
-      <c r="J33" s="8"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="J33" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
-      <c r="E34" s="30"/>
+      <c r="E34"/>
       <c r="I34" s="40"/>
-      <c r="J34" s="8"/>
-    </row>
-    <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="10"/>
-      <c r="E35"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="8"/>
-    </row>
-    <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35">
+        <v>0.10959000000000001</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I35" s="40">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J35" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="8"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D36" s="60" t="s">
-        <v>194</v>
+        <v>187</v>
+      </c>
+      <c r="C36" s="26"/>
+      <c r="D36" s="59" t="s">
+        <v>195</v>
       </c>
       <c r="E36">
-        <v>0.10959000000000001</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I36" s="40">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J36" s="8"/>
-    </row>
-    <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="47"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C37" s="26"/>
-      <c r="D37" s="60" t="s">
-        <v>195</v>
+      <c r="D37" s="59" t="s">
+        <v>196</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>9.579E-2</v>
       </c>
       <c r="F37" s="47"/>
       <c r="I37" s="40"/>
-      <c r="J37" s="8"/>
-    </row>
-    <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J37" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C38" s="26"/>
-      <c r="D38" s="60" t="s">
-        <v>196</v>
+      <c r="D38" s="59" t="s">
+        <v>197</v>
       </c>
       <c r="E38">
-        <v>9.579E-2</v>
+        <v>0.20563999999999999</v>
       </c>
       <c r="F38" s="47"/>
       <c r="I38" s="40"/>
-      <c r="J38" s="8"/>
-    </row>
-    <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>189</v>
-      </c>
+      <c r="J38" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" s="8"/>
+    </row>
+    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
-        <v>197</v>
-      </c>
-      <c r="E39">
-        <v>0.20563999999999999</v>
-      </c>
-      <c r="F39" s="47"/>
+      <c r="D39" s="10"/>
+      <c r="E39"/>
       <c r="I39" s="40"/>
-      <c r="J39" s="8"/>
-    </row>
-    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="10"/>
-      <c r="E40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="8"/>
-    </row>
-    <row r="41" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E40">
+        <v>0.13420000000000001</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I40" s="40">
+        <v>2.4</v>
+      </c>
+      <c r="J40" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K40" s="8"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>90</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>190</v>
+        <v>173</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>191</v>
       </c>
       <c r="E41">
-        <v>0.13420000000000001</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I41" s="40">
-        <v>2.4</v>
-      </c>
-      <c r="J41" s="8"/>
-    </row>
-    <row r="42" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="F41" s="47"/>
+      <c r="I41" s="40"/>
+      <c r="J41" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="8"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>90</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>191</v>
+        <v>174</v>
+      </c>
+      <c r="C42" s="26"/>
+      <c r="D42" s="27" t="s">
+        <v>192</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>0.13092999999999999</v>
       </c>
       <c r="F42" s="47"/>
       <c r="I42" s="40"/>
-      <c r="J42" s="8"/>
-    </row>
-    <row r="43" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="J42" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K42" s="8"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>90</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="27" t="s">
-        <v>192</v>
+        <v>175</v>
+      </c>
+      <c r="C43" s="64"/>
+      <c r="D43" s="3" t="s">
+        <v>193</v>
       </c>
       <c r="E43">
-        <v>0.13092999999999999</v>
+        <v>-0.56130000000000002</v>
       </c>
       <c r="F43" s="47"/>
       <c r="I43" s="40"/>
-      <c r="J43" s="8"/>
-    </row>
-    <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="C44" s="63"/>
-      <c r="D44" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="E44">
-        <v>-0.56130000000000002</v>
-      </c>
-      <c r="F44" s="47"/>
+      <c r="K43" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="64"/>
+      <c r="E44" s="29"/>
       <c r="I44" s="40"/>
-      <c r="J44" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K44" s="8"/>
+    </row>
+    <row r="45" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
-      <c r="C45" s="63"/>
-      <c r="E45" s="29"/>
+      <c r="E45" s="30"/>
       <c r="I45" s="40"/>
-      <c r="J45" s="8"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="E46" s="30"/>
       <c r="I46" s="40"/>
-      <c r="J46" s="8"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K46" s="8"/>
+    </row>
+    <row r="47" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="E47" s="30"/>
       <c r="I47" s="40"/>
-      <c r="J47" s="8"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K47" s="8"/>
+    </row>
+    <row r="48" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="E48" s="30"/>
       <c r="I48" s="40"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K48" s="8"/>
+    </row>
+    <row r="49" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="E49" s="30"/>
       <c r="I49" s="40"/>
-      <c r="J49" s="8"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="E50" s="30"/>
       <c r="I50" s="40"/>
-      <c r="J50" s="8"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="E51" s="30"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="8"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E53" s="10"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E57" s="27"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="K50" s="8"/>
+    </row>
+    <row r="51" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="52" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="54" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="55" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="56" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="E56" s="27"/>
+    </row>
+    <row r="57" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="E57" s="10"/>
+    </row>
+    <row r="58" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E60" s="10"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E61" s="27"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="E60" s="27"/>
+    </row>
+    <row r="61" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="E63" s="10"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E64" s="10"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E65" s="27"/>
-    </row>
+    <row r="64" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+      <c r="E64" s="27"/>
+    </row>
+    <row r="65" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="14" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="14" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C43:C44"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
@@ -2600,7 +2694,7 @@
       <c r="C2" t="s">
         <v>148</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="55"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -27496,8 +27590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -27509,10 +27603,10 @@
     <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34.5" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="10.5" style="39" customWidth="1"/>
-    <col min="11" max="11" width="60.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" style="32" customWidth="1"/>
     <col min="12" max="12" width="4.33203125" style="32" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="3"/>
   </cols>
@@ -27548,7 +27642,9 @@
       <c r="J1" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="33"/>
+      <c r="K1" s="33" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
@@ -27578,6 +27674,9 @@
       </c>
       <c r="J2" s="39">
         <v>1.08</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -27604,6 +27703,9 @@
       <c r="I3" s="10"/>
       <c r="J3" s="39">
         <v>1.08</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -27645,6 +27747,9 @@
       <c r="J5" s="39">
         <v>1.0900000000000001</v>
       </c>
+      <c r="K5" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
@@ -27671,6 +27776,9 @@
       <c r="J6" s="39">
         <v>1.0900000000000001</v>
       </c>
+      <c r="K6" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
@@ -27697,6 +27805,9 @@
       <c r="J7" s="39">
         <v>1.0900000000000001</v>
       </c>
+      <c r="K7" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
@@ -27722,6 +27833,9 @@
       <c r="I8" s="10"/>
       <c r="J8" s="39">
         <v>1.0900000000000001</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -27741,7 +27855,7 @@
       <c r="B10" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="63" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="48" t="s">
@@ -27763,6 +27877,9 @@
       <c r="J10" s="39">
         <v>1.03</v>
       </c>
+      <c r="K10" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
@@ -27771,7 +27888,7 @@
       <c r="B11" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="62"/>
+      <c r="C11" s="63"/>
       <c r="D11" s="50" t="s">
         <v>152</v>
       </c>
@@ -27789,6 +27906,9 @@
       <c r="J11" s="39">
         <v>1.03</v>
       </c>
+      <c r="K11" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
@@ -27814,6 +27934,9 @@
       <c r="I12" s="10"/>
       <c r="J12" s="39">
         <v>1.03</v>
+      </c>
+      <c r="K12" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -27856,6 +27979,9 @@
       <c r="J14" s="39">
         <v>1.07</v>
       </c>
+      <c r="K14" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
@@ -27881,6 +28007,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="39">
         <v>1.07</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -27922,6 +28051,9 @@
       <c r="J17" s="39">
         <v>1.05</v>
       </c>
+      <c r="K17" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
@@ -27948,6 +28080,9 @@
       <c r="J18" s="39">
         <v>1.05</v>
       </c>
+      <c r="K18" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
@@ -27974,6 +28109,9 @@
       <c r="J19" s="39">
         <v>1.05</v>
       </c>
+      <c r="K19" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
@@ -27999,6 +28137,9 @@
       <c r="I20" s="10"/>
       <c r="J20" s="39">
         <v>1.05</v>
+      </c>
+      <c r="K20" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28038,7 +28179,9 @@
       <c r="J22" s="39">
         <v>1.1399999999999999</v>
       </c>
-      <c r="K22" s="32"/>
+      <c r="K22" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="L22" s="32"/>
       <c r="M22" s="3"/>
     </row>
@@ -28065,7 +28208,9 @@
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="39"/>
-      <c r="K23" s="32"/>
+      <c r="K23" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="L23" s="32"/>
       <c r="M23" s="3"/>
     </row>
@@ -28104,6 +28249,9 @@
       <c r="J25" s="39">
         <v>1.1000000000000001</v>
       </c>
+      <c r="K25" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
@@ -28128,7 +28276,9 @@
       <c r="J26" s="39">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K26" s="55"/>
+      <c r="K26" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
@@ -28153,7 +28303,9 @@
       <c r="J27" s="39">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K27" s="55"/>
+      <c r="K27" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
@@ -28177,6 +28329,9 @@
       </c>
       <c r="J28" s="39">
         <v>1.1000000000000001</v>
+      </c>
+      <c r="K28" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28197,7 +28352,7 @@
       <c r="C30" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D30" s="64" t="s">
+      <c r="D30" s="61" t="s">
         <v>176</v>
       </c>
       <c r="E30">
@@ -28216,6 +28371,9 @@
       <c r="J30" s="32">
         <v>1.02</v>
       </c>
+      <c r="K30" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
@@ -28225,7 +28383,7 @@
         <v>217</v>
       </c>
       <c r="C31" s="52"/>
-      <c r="D31" s="58" t="s">
+      <c r="D31" s="57" t="s">
         <v>177</v>
       </c>
       <c r="E31">
@@ -28242,6 +28400,9 @@
       <c r="J31" s="32">
         <v>1.02</v>
       </c>
+      <c r="K31" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="32" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
@@ -28251,7 +28412,7 @@
         <v>218</v>
       </c>
       <c r="C32" s="52"/>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="57" t="s">
         <v>178</v>
       </c>
       <c r="E32">
@@ -28268,7 +28429,9 @@
       <c r="J32" s="32">
         <v>1.02</v>
       </c>
-      <c r="K32" s="32"/>
+      <c r="K32" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="L32" s="32"/>
     </row>
     <row r="33" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -28279,7 +28442,7 @@
         <v>219</v>
       </c>
       <c r="C33" s="52"/>
-      <c r="D33" s="65" t="s">
+      <c r="D33" s="62" t="s">
         <v>179</v>
       </c>
       <c r="E33">
@@ -28296,7 +28459,9 @@
       <c r="J33" s="32">
         <v>1.02</v>
       </c>
-      <c r="K33" s="32"/>
+      <c r="K33" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="L33" s="32"/>
     </row>
     <row r="34" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -28307,7 +28472,7 @@
         <v>220</v>
       </c>
       <c r="C34" s="52"/>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="57" t="s">
         <v>180</v>
       </c>
       <c r="E34">
@@ -28322,14 +28487,16 @@
       <c r="H34" s="3"/>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
+      <c r="K34" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="L34" s="32"/>
     </row>
     <row r="35" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="58"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="57"/>
       <c r="E35"/>
       <c r="F35"/>
       <c r="G35"/>
@@ -28368,6 +28535,9 @@
       <c r="J36" s="39">
         <v>1.06</v>
       </c>
+      <c r="K36" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
@@ -28376,7 +28546,7 @@
       <c r="B37" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="C37" s="61"/>
+      <c r="C37" s="60"/>
       <c r="D37" s="54" t="s">
         <v>226</v>
       </c>
@@ -28391,6 +28561,9 @@
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
+      <c r="K37" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
@@ -28399,7 +28572,7 @@
       <c r="B38" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="C38" s="61"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="54" t="s">
         <v>208</v>
       </c>
@@ -28414,6 +28587,9 @@
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
+      <c r="K38" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
@@ -28422,7 +28598,7 @@
       <c r="B39" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="C39" s="61"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="54" t="s">
         <v>209</v>
       </c>
@@ -28437,6 +28613,9 @@
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
+      <c r="K39" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="40" spans="1:12" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
@@ -28478,7 +28657,9 @@
       <c r="J41" s="39">
         <v>1.1200000000000001</v>
       </c>
-      <c r="K41" s="55"/>
+      <c r="K41" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
@@ -28499,6 +28680,9 @@
       <c r="G42" s="10" t="s">
         <v>141</v>
       </c>
+      <c r="K42" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
@@ -28518,6 +28702,9 @@
       </c>
       <c r="G43" s="10" t="s">
         <v>141</v>
+      </c>
+      <c r="K43" s="32" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -28605,7 +28792,7 @@
   <mergeCells count="1">
     <mergeCell ref="C10:C11"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -28641,7 +28828,7 @@
       <c r="A2" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="55" t="s">
         <v>165</v>
       </c>
       <c r="C2" t="s">
@@ -28890,7 +29077,7 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="63"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28906,7 +29093,7 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="63"/>
+      <c r="F13" s="64"/>
     </row>
     <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -36532,8 +36719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBA40B-94B1-B140-8D57-D55E3398F15E}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36660,7 +36847,7 @@
         <v>173</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix BMI 2 or more
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C889ADE-2118-EF4C-A724-96C07D5B3C06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC1EBB2-9C06-3745-9CE7-5F04B6FD4CCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61180" yWindow="4180" windowWidth="27700" windowHeight="21040" firstSheet="5" activeTab="8" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="320" yWindow="460" windowWidth="27700" windowHeight="21040" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -742,7 +742,7 @@
     <t>under 25</t>
   </si>
   <si>
-    <t>2 or more</t>
+    <t>25 or more</t>
   </si>
 </sst>
 </file>
@@ -1414,13 +1414,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" style="3" customWidth="1"/>
@@ -1435,7 +1435,7 @@
     <col min="12" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>84</v>
       </c>
@@ -1563,7 +1563,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>87</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
       <c r="C7" s="26"/>
@@ -1596,7 +1596,7 @@
       <c r="I7" s="40"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>57</v>
       </c>
@@ -1623,7 +1623,7 @@
       </c>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>57</v>
       </c>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="26"/>
@@ -1676,7 +1676,7 @@
       <c r="I11" s="40"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="26"/>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="26"/>
@@ -1840,7 +1840,7 @@
       <c r="I19" s="40"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>214</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="12" t="s">
         <v>214</v>
       </c>
@@ -1891,7 +1891,7 @@
       </c>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>214</v>
       </c>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>214</v>
       </c>
@@ -1931,7 +1931,7 @@
       </c>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>214</v>
       </c>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="26"/>
@@ -1960,7 +1960,7 @@
       <c r="I25" s="40"/>
       <c r="K25" s="8"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>89</v>
       </c>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="K26" s="8"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>89</v>
       </c>
@@ -2008,7 +2008,7 @@
       </c>
       <c r="K27" s="8"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>89</v>
       </c>
@@ -2029,7 +2029,7 @@
       </c>
       <c r="K28" s="8"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="26"/>
@@ -2039,7 +2039,7 @@
       <c r="I29" s="40"/>
       <c r="K29" s="8"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>52</v>
       </c>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="K30" s="8"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>52</v>
       </c>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="K31" s="8"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>52</v>
       </c>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="K32" s="8"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>52</v>
       </c>
@@ -2126,14 +2126,14 @@
       </c>
       <c r="K33" s="8"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="E34"/>
       <c r="I34" s="40"/>
       <c r="K34" s="8"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>68</v>
       </c>
@@ -2160,7 +2160,7 @@
       </c>
       <c r="K35" s="8"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>68</v>
       </c>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="K36" s="8"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>68</v>
       </c>
@@ -2202,7 +2202,7 @@
       </c>
       <c r="K37" s="8"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>68</v>
       </c>
@@ -2232,7 +2232,7 @@
       <c r="I39" s="40"/>
       <c r="K39" s="8"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>90</v>
       </c>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>90</v>
       </c>
@@ -2279,7 +2279,7 @@
       </c>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>90</v>
       </c>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="K42" s="8"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>90</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="64"/>
@@ -2328,88 +2328,78 @@
       <c r="I44" s="40"/>
       <c r="K44" s="8"/>
     </row>
-    <row r="45" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A45" s="12"/>
       <c r="B45" s="12"/>
       <c r="E45" s="30"/>
       <c r="I45" s="40"/>
       <c r="K45" s="8"/>
     </row>
-    <row r="46" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="E46" s="30"/>
       <c r="I46" s="40"/>
       <c r="K46" s="8"/>
     </row>
-    <row r="47" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="E47" s="30"/>
       <c r="I47" s="40"/>
       <c r="K47" s="8"/>
     </row>
-    <row r="48" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="E48" s="30"/>
       <c r="I48" s="40"/>
       <c r="K48" s="8"/>
     </row>
-    <row r="49" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="E49" s="30"/>
       <c r="I49" s="40"/>
       <c r="K49" s="8"/>
     </row>
-    <row r="50" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="E50" s="30"/>
       <c r="I50" s="40"/>
       <c r="K50" s="8"/>
     </row>
-    <row r="51" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="52" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E52" s="10"/>
     </row>
-    <row r="53" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="54" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="55" spans="1:11" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="56" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E56" s="27"/>
     </row>
-    <row r="57" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E57" s="10"/>
     </row>
-    <row r="58" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E58" s="10"/>
     </row>
-    <row r="59" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E59" s="10"/>
     </row>
-    <row r="60" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E60" s="27"/>
     </row>
-    <row r="61" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E63" s="10"/>
     </row>
-    <row r="64" spans="1:11" ht="14" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E64" s="27"/>
     </row>
-    <row r="65" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="66" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="67" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="68" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="69" ht="14" x14ac:dyDescent="0.15"/>
-    <row r="70" ht="14" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C8:C9"/>
@@ -27590,8 +27580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -36719,7 +36709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFBA40B-94B1-B140-8D57-D55E3398F15E}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added optional value decorations
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC1EBB2-9C06-3745-9CE7-5F04B6FD4CCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DFE54E-C818-AD4A-A42D-B9159F86EAF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="27700" windowHeight="21040" firstSheet="5" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="360" yWindow="760" windowWidth="34320" windowHeight="21040" firstSheet="5" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="235">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -744,6 +744,12 @@
   <si>
     <t>25 or more</t>
   </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>:unknown</t>
+  </si>
 </sst>
 </file>
 
@@ -863,7 +869,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1015,6 +1021,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1414,15 +1423,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="43.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
@@ -1522,60 +1531,58 @@
       </c>
       <c r="K3" s="8"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="10"/>
-      <c r="E4"/>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>85</v>
+      </c>
       <c r="I4" s="40"/>
+      <c r="J4" s="32" t="s">
+        <v>10</v>
+      </c>
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I5" s="40">
-        <v>2.1</v>
-      </c>
-      <c r="J5" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="10"/>
+      <c r="E5"/>
+      <c r="I5" s="40"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>87</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="26"/>
+        <v>11</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>72</v>
+      </c>
       <c r="D6" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E6">
-        <v>0.24582000000000001</v>
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="I6" s="40">
         <v>2.1</v>
@@ -1584,65 +1591,67 @@
         <v>10</v>
       </c>
       <c r="K6" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="26"/>
+      <c r="D7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <v>0.24582000000000001</v>
+      </c>
+      <c r="I7" s="40">
+        <v>2.1</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="10"/>
-      <c r="E7"/>
-      <c r="I7" s="40"/>
-      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>144</v>
+        <v>234</v>
+      </c>
+      <c r="C8" s="26"/>
+      <c r="D8" s="10" t="s">
+        <v>233</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>141</v>
+        <v>0.24582000000000001</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="I8" s="40">
-        <v>1.4</v>
+        <v>2.1</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="E9">
-        <v>0.27340999999999999</v>
-      </c>
-      <c r="I9" s="40">
-        <v>1.4</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="10"/>
+      <c r="E9"/>
+      <c r="I9" s="40"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1650,14 +1659,19 @@
         <v>57</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="31"/>
+        <v>130</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>73</v>
+      </c>
       <c r="D10" s="14" t="s">
-        <v>199</v>
+        <v>144</v>
       </c>
       <c r="E10">
-        <v>0.48875999999999997</v>
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="I10" s="40">
         <v>1.4</v>
@@ -1668,35 +1682,43 @@
       <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="10"/>
-      <c r="E11"/>
-      <c r="I11" s="40"/>
+      <c r="A11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="65"/>
+      <c r="D11" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11">
+        <v>0.27340999999999999</v>
+      </c>
+      <c r="I11" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="J11" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>83</v>
+        <v>132</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="14" t="s">
+        <v>199</v>
       </c>
       <c r="E12">
-        <v>4.9770000000000002E-2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>141</v>
+        <v>0.48875999999999997</v>
       </c>
       <c r="I12" s="40">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="J12" s="32" t="s">
         <v>11</v>
@@ -1704,85 +1726,70 @@
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="10"/>
+      <c r="E13"/>
+      <c r="I13" s="40"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B14" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14">
+        <v>4.9770000000000002E-2</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="40">
+        <v>1.6</v>
+      </c>
+      <c r="J14" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="10" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0</v>
       </c>
-      <c r="I13" s="40">
+      <c r="I15" s="40">
         <v>1.6</v>
-      </c>
-      <c r="J13" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="10"/>
-      <c r="E14"/>
-      <c r="I14" s="40"/>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15">
-        <v>-0.40421000000000001</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="I15" s="40">
-        <v>1.7</v>
       </c>
       <c r="J15" s="32" t="s">
         <v>11</v>
       </c>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>54</v>
-      </c>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="26"/>
-      <c r="D16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16">
-        <v>0.20102</v>
-      </c>
-      <c r="G16" s="10"/>
-      <c r="I16" s="40">
-        <v>1.7</v>
-      </c>
-      <c r="J16" s="32" t="s">
-        <v>11</v>
-      </c>
+      <c r="D16" s="10"/>
+      <c r="E16"/>
+      <c r="I16" s="40"/>
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1790,16 +1797,21 @@
         <v>66</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="10" t="s">
-        <v>63</v>
+        <v>53</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>62</v>
       </c>
       <c r="E17">
-        <v>4.8410000000000002E-2</v>
-      </c>
-      <c r="G17" s="10"/>
+        <v>-0.40421000000000001</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G17" s="13"/>
       <c r="I17" s="40">
         <v>1.7</v>
       </c>
@@ -1813,14 +1825,14 @@
         <v>66</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="10" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.20102</v>
       </c>
       <c r="G18" s="10"/>
       <c r="I18" s="40">
@@ -1831,64 +1843,59 @@
       </c>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="C19" s="26"/>
-      <c r="D19" s="10"/>
-      <c r="E19"/>
-      <c r="I19" s="40"/>
+      <c r="D19" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19">
+        <v>4.8410000000000002E-2</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="I19" s="40">
+        <v>1.7</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>214</v>
+        <v>66</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="58" t="s">
-        <v>176</v>
+        <v>56</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="E20">
-        <v>0.24259</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>98</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G20" s="10"/>
       <c r="I20" s="40">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="J20" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="K20" s="8" t="s">
-        <v>96</v>
-      </c>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="D21" s="58" t="s">
-        <v>177</v>
-      </c>
-      <c r="E21">
-        <v>-5.6439999999999997E-2</v>
-      </c>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="10"/>
+      <c r="E21"/>
       <c r="I21" s="40"/>
-      <c r="J21" s="32" t="s">
-        <v>11</v>
-      </c>
       <c r="K21" s="8"/>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1896,34 +1903,45 @@
         <v>214</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="C22" s="31"/>
+        <v>181</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>77</v>
+      </c>
       <c r="D22" s="58" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E22">
-        <v>-5.0889999999999998E-2</v>
-      </c>
-      <c r="I22" s="40"/>
+        <v>0.24259</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" s="40">
+        <v>1.2</v>
+      </c>
       <c r="J22" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="8"/>
+      <c r="K22" s="8" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>214</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="C23" s="31"/>
+        <v>182</v>
+      </c>
       <c r="D23" s="58" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>-5.6439999999999997E-2</v>
       </c>
       <c r="I23" s="40"/>
       <c r="J23" s="32" t="s">
@@ -1936,14 +1954,14 @@
         <v>214</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="C24" s="56"/>
+        <v>183</v>
+      </c>
+      <c r="C24" s="31"/>
       <c r="D24" s="58" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E24">
-        <v>0.22292000000000001</v>
+        <v>-5.0889999999999998E-2</v>
       </c>
       <c r="I24" s="40"/>
       <c r="J24" s="32" t="s">
@@ -1952,60 +1970,52 @@
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="27"/>
-      <c r="E25"/>
+      <c r="A25" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="31"/>
+      <c r="D25" s="58" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
       <c r="I25" s="40"/>
+      <c r="J25" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>89</v>
+        <v>214</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="57" t="s">
-        <v>203</v>
+        <v>185</v>
+      </c>
+      <c r="C26" s="56"/>
+      <c r="D26" s="58" t="s">
+        <v>180</v>
       </c>
       <c r="E26">
-        <v>-0.15398000000000001</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I26" s="40">
-        <v>2.2000000000000002</v>
-      </c>
+        <v>0.22292000000000001</v>
+      </c>
+      <c r="I26" s="40"/>
       <c r="J26" s="32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>201</v>
-      </c>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="26"/>
-      <c r="D27" s="57" t="s">
-        <v>205</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" s="47"/>
+      <c r="D27" s="27"/>
+      <c r="E27"/>
       <c r="I27" s="40"/>
-      <c r="J27" s="32" t="s">
-        <v>10</v>
-      </c>
       <c r="K27" s="8"/>
     </row>
     <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -2013,98 +2023,102 @@
         <v>89</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C28" s="26"/>
+        <v>200</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>78</v>
+      </c>
       <c r="D28" s="57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E28">
-        <v>-7.1799999999999998E-3</v>
-      </c>
-      <c r="F28" s="47"/>
-      <c r="I28" s="40"/>
+        <v>-0.15398000000000001</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I28" s="40">
+        <v>2.2000000000000002</v>
+      </c>
       <c r="J28" s="32" t="s">
         <v>10</v>
       </c>
       <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>201</v>
+      </c>
       <c r="C29" s="26"/>
-      <c r="D29" s="28"/>
-      <c r="E29"/>
+      <c r="D29" s="57" t="s">
+        <v>205</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
       <c r="F29" s="47"/>
       <c r="I29" s="40"/>
+      <c r="J29" s="32" t="s">
+        <v>10</v>
+      </c>
       <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>206</v>
+        <v>202</v>
+      </c>
+      <c r="C30" s="26"/>
+      <c r="D30" s="57" t="s">
+        <v>204</v>
       </c>
       <c r="E30">
-        <v>0.10249</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I30" s="40">
-        <v>1.5</v>
-      </c>
+        <v>-7.1799999999999998E-3</v>
+      </c>
+      <c r="F30" s="47"/>
+      <c r="I30" s="40"/>
       <c r="J30" s="32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>207</v>
+        <v>234</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="57" t="s">
+        <v>233</v>
       </c>
       <c r="E31">
-        <v>-1.281E-2</v>
+        <v>0</v>
+      </c>
+      <c r="F31" s="47"/>
+      <c r="G31" s="12" t="s">
+        <v>201</v>
       </c>
       <c r="I31" s="40"/>
       <c r="J31" s="32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
+      <c r="A32" s="11"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="28"/>
+      <c r="E32"/>
+      <c r="F32" s="47"/>
       <c r="I32" s="40"/>
-      <c r="J32" s="32" t="s">
-        <v>11</v>
-      </c>
       <c r="K32" s="8"/>
     </row>
     <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -2112,49 +2126,64 @@
         <v>52</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>213</v>
+        <v>210</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>79</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E33">
-        <v>-0.26149</v>
-      </c>
-      <c r="I33" s="40"/>
+        <v>0.10249</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I33" s="40">
+        <v>1.5</v>
+      </c>
       <c r="J33" s="32" t="s">
         <v>11</v>
       </c>
       <c r="K33" s="8"/>
     </row>
     <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="E34"/>
+      <c r="A34" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="E34">
+        <v>-1.281E-2</v>
+      </c>
       <c r="I34" s="40"/>
+      <c r="J34" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="59" t="s">
-        <v>194</v>
+        <v>212</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>208</v>
       </c>
       <c r="E35">
-        <v>0.10959000000000001</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I35" s="40">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I35" s="40"/>
       <c r="J35" s="32" t="s">
         <v>11</v>
       </c>
@@ -2162,19 +2191,17 @@
     </row>
     <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="59" t="s">
-        <v>195</v>
+        <v>213</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>209</v>
       </c>
       <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" s="47"/>
+        <v>-0.26149</v>
+      </c>
       <c r="I36" s="40"/>
       <c r="J36" s="32" t="s">
         <v>11</v>
@@ -2182,24 +2209,10 @@
       <c r="K36" s="8"/>
     </row>
     <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="C37" s="26"/>
-      <c r="D37" s="59" t="s">
-        <v>196</v>
-      </c>
-      <c r="E37">
-        <v>9.579E-2</v>
-      </c>
-      <c r="F37" s="47"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+      <c r="E37"/>
       <c r="I37" s="40"/>
-      <c r="J37" s="32" t="s">
-        <v>11</v>
-      </c>
       <c r="K37" s="8"/>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -2207,53 +2220,65 @@
         <v>68</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="C38" s="26"/>
+        <v>186</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>80</v>
+      </c>
       <c r="D38" s="59" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E38">
-        <v>0.20563999999999999</v>
-      </c>
-      <c r="F38" s="47"/>
-      <c r="I38" s="40"/>
+        <v>0.10959000000000001</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I38" s="40">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="J38" s="32" t="s">
         <v>11</v>
       </c>
       <c r="K38" s="8"/>
     </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>187</v>
+      </c>
       <c r="C39" s="26"/>
-      <c r="D39" s="10"/>
-      <c r="E39"/>
+      <c r="D39" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39" s="47"/>
       <c r="I39" s="40"/>
+      <c r="J39" s="32" t="s">
+        <v>11</v>
+      </c>
       <c r="K39" s="8"/>
     </row>
     <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>190</v>
+        <v>188</v>
+      </c>
+      <c r="C40" s="26"/>
+      <c r="D40" s="59" t="s">
+        <v>196</v>
       </c>
       <c r="E40">
-        <v>0.13420000000000001</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I40" s="40">
-        <v>2.4</v>
-      </c>
+        <v>9.579E-2</v>
+      </c>
+      <c r="F40" s="47"/>
+      <c r="I40" s="40"/>
       <c r="J40" s="32" t="s">
         <v>11</v>
       </c>
@@ -2261,16 +2286,17 @@
     </row>
     <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
+      </c>
+      <c r="C41" s="26"/>
+      <c r="D41" s="59" t="s">
+        <v>197</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>0.20563999999999999</v>
       </c>
       <c r="F41" s="47"/>
       <c r="I41" s="40"/>
@@ -2279,25 +2305,13 @@
       </c>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>174</v>
-      </c>
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="26"/>
-      <c r="D42" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="E42">
-        <v>0.13092999999999999</v>
-      </c>
-      <c r="F42" s="47"/>
+      <c r="D42" s="10"/>
+      <c r="E42"/>
       <c r="I42" s="40"/>
-      <c r="J42" s="32" t="s">
-        <v>11</v>
-      </c>
       <c r="K42" s="8"/>
     </row>
     <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -2305,48 +2319,113 @@
         <v>90</v>
       </c>
       <c r="B43" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>190</v>
+      </c>
+      <c r="E43">
+        <v>0.13420000000000001</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I43" s="40">
+        <v>2.4</v>
+      </c>
+      <c r="J43" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K43" s="8"/>
+    </row>
+    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" s="47"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K44" s="8"/>
+    </row>
+    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C45" s="26"/>
+      <c r="D45" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E45">
+        <v>0.13092999999999999</v>
+      </c>
+      <c r="F45" s="47"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C43" s="64"/>
-      <c r="D43" s="3" t="s">
+      <c r="C46" s="63"/>
+      <c r="D46" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="E43">
+      <c r="E46">
         <v>-0.56130000000000002</v>
       </c>
-      <c r="F43" s="47"/>
-      <c r="I43" s="40"/>
-      <c r="K43" s="8" t="s">
+      <c r="F46" s="47"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="K46" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="64"/>
-      <c r="E44" s="29"/>
-      <c r="I44" s="40"/>
-      <c r="K44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="E45" s="30"/>
-      <c r="I45" s="40"/>
-      <c r="K45" s="8"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="E46" s="30"/>
-      <c r="I46" s="40"/>
-      <c r="K46" s="8"/>
-    </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="E47" s="30"/>
+      <c r="A47" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C47" s="63"/>
+      <c r="D47" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E47" s="29">
+        <v>0</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>173</v>
+      </c>
       <c r="I47" s="40"/>
+      <c r="J47" s="32" t="s">
+        <v>10</v>
+      </c>
       <c r="K47" s="8"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.15">
@@ -2370,23 +2449,35 @@
       <c r="I50" s="40"/>
       <c r="K50" s="8"/>
     </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="E51" s="30"/>
+      <c r="I51" s="40"/>
+      <c r="K51" s="8"/>
+    </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E52" s="10"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E56" s="27"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E58" s="10"/>
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="E52" s="30"/>
+      <c r="I52" s="40"/>
+      <c r="K52" s="8"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="E53" s="30"/>
+      <c r="I53" s="40"/>
+      <c r="K53" s="8"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="E55" s="10"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E59" s="10"/>
+      <c r="E59" s="27"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E60" s="27"/>
+      <c r="E60" s="10"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.15">
       <c r="E61" s="10"/>
@@ -2395,15 +2486,23 @@
       <c r="E62" s="10"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E63" s="10"/>
+      <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="E64" s="27"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E66" s="10"/>
+    </row>
+    <row r="67" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E67" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C43:C44"/>
+  <mergeCells count="1">
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27580,7 +27679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -27845,7 +27944,7 @@
       <c r="B10" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="64" t="s">
         <v>42</v>
       </c>
       <c r="D10" s="48" t="s">
@@ -27878,7 +27977,7 @@
       <c r="B11" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="63"/>
+      <c r="C11" s="64"/>
       <c r="D11" s="50" t="s">
         <v>152</v>
       </c>
@@ -29067,7 +29166,7 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="64"/>
+      <c r="F12" s="65"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -29083,7 +29182,7 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="64"/>
+      <c r="F13" s="65"/>
     </row>
     <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
GT-92 and 107 - result panel and tool labels
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A82B00F-4D57-A34D-A22C-6FB06980276A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E562C-BF1E-DE48-8AED-3A11F0B749EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2080" windowWidth="34320" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1260" yWindow="2080" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -1431,7 +1431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -27673,7 +27673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added donor boxes to lung - GT-94
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E562C-BF1E-DE48-8AED-3A11F0B749EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D62C1A-7D52-FB41-B97E-ECBA3C0635C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="2080" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2246" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="239">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -759,6 +759,9 @@
   <si>
     <t>BMI</t>
   </si>
+  <si>
+    <t>:boxed</t>
+  </si>
 </sst>
 </file>
 
@@ -1429,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:K67"/>
+  <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1445,12 +1448,12 @@
     <col min="6" max="6" width="17.83203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
     <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15" style="32" customWidth="1"/>
-    <col min="11" max="11" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.83203125" style="3"/>
+    <col min="10" max="11" width="15" style="32" customWidth="1"/>
+    <col min="12" max="12" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1481,11 +1484,14 @@
       <c r="J1" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="L1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>79</v>
       </c>
@@ -1513,9 +1519,12 @@
       <c r="J2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>79</v>
       </c>
@@ -1535,9 +1544,12 @@
       <c r="J3" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K3" s="8"/>
-    </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>79</v>
       </c>
@@ -1556,9 +1568,12 @@
       <c r="J4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K4" s="8"/>
-    </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="26"/>
@@ -1566,9 +1581,10 @@
       <c r="E5"/>
       <c r="I5" s="40"/>
       <c r="J5" s="3"/>
-      <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5" s="3"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>82</v>
       </c>
@@ -1596,11 +1612,14 @@
       <c r="J6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>82</v>
       </c>
@@ -1620,11 +1639,14 @@
       <c r="J7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>82</v>
       </c>
@@ -1644,11 +1666,14 @@
       <c r="J8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="26"/>
@@ -1656,9 +1681,10 @@
       <c r="E9"/>
       <c r="I9" s="40"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K9" s="3"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>52</v>
       </c>
@@ -1681,9 +1707,10 @@
         <v>30</v>
       </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K10" s="3"/>
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>52</v>
       </c>
@@ -1701,9 +1728,10 @@
         <v>30</v>
       </c>
       <c r="J11" s="3"/>
-      <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K11" s="3"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
@@ -1721,9 +1749,10 @@
         <v>30</v>
       </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K12" s="3"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="26"/>
@@ -1731,9 +1760,10 @@
       <c r="E13"/>
       <c r="I13" s="40"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K13" s="3"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -1756,9 +1786,10 @@
         <v>70</v>
       </c>
       <c r="J14" s="3"/>
-      <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K14" s="3"/>
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>19</v>
       </c>
@@ -1776,9 +1807,10 @@
         <v>70</v>
       </c>
       <c r="J15" s="3"/>
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K15" s="3"/>
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="26"/>
@@ -1786,9 +1818,10 @@
       <c r="E16"/>
       <c r="I16" s="40"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="3"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>61</v>
       </c>
@@ -1811,9 +1844,10 @@
         <v>20</v>
       </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K17" s="3"/>
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>61</v>
       </c>
@@ -1831,9 +1865,10 @@
         <v>20</v>
       </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="3"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>61</v>
       </c>
@@ -1851,9 +1886,10 @@
         <v>20</v>
       </c>
       <c r="J19" s="3"/>
-      <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" s="3"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>61</v>
       </c>
@@ -1871,9 +1907,10 @@
         <v>20</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K20" s="3"/>
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="26"/>
@@ -1881,9 +1918,10 @@
       <c r="E21"/>
       <c r="I21" s="40"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="8"/>
-    </row>
-    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K21" s="3"/>
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>207</v>
       </c>
@@ -1909,11 +1947,12 @@
         <v>10</v>
       </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="8" t="s">
+      <c r="K22" s="3"/>
+      <c r="L22" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>207</v>
       </c>
@@ -1930,9 +1969,10 @@
         <v>10</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="8"/>
-    </row>
-    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K23" s="3"/>
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>207</v>
       </c>
@@ -1950,9 +1990,10 @@
         <v>10</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="8"/>
-    </row>
-    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K24" s="3"/>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>207</v>
       </c>
@@ -1970,9 +2011,10 @@
         <v>10</v>
       </c>
       <c r="J25" s="3"/>
-      <c r="K25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K25" s="3"/>
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>207</v>
       </c>
@@ -1990,9 +2032,10 @@
         <v>10</v>
       </c>
       <c r="J26" s="3"/>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K26" s="3"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="26"/>
@@ -2000,9 +2043,10 @@
       <c r="E27"/>
       <c r="I27" s="40"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="8"/>
-    </row>
-    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K27" s="3"/>
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>84</v>
       </c>
@@ -2027,9 +2071,12 @@
       <c r="J28" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>84</v>
       </c>
@@ -2050,9 +2097,12 @@
       <c r="J29" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K29" s="8"/>
-    </row>
-    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>84</v>
       </c>
@@ -2073,9 +2123,12 @@
       <c r="J30" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K30" s="8"/>
-    </row>
-    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" s="8"/>
+    </row>
+    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>84</v>
       </c>
@@ -2096,9 +2149,12 @@
       <c r="J31" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K31" s="8"/>
-    </row>
-    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="26"/>
@@ -2107,9 +2163,10 @@
       <c r="F32" s="47"/>
       <c r="I32" s="40"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="8"/>
-    </row>
-    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K32" s="3"/>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>47</v>
       </c>
@@ -2135,9 +2192,10 @@
         <v>40</v>
       </c>
       <c r="J33" s="3"/>
-      <c r="K33" s="8"/>
-    </row>
-    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K33" s="3"/>
+      <c r="L33" s="8"/>
+    </row>
+    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>47</v>
       </c>
@@ -2154,9 +2212,10 @@
         <v>40</v>
       </c>
       <c r="J34" s="3"/>
-      <c r="K34" s="8"/>
-    </row>
-    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K34" s="3"/>
+      <c r="L34" s="8"/>
+    </row>
+    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>47</v>
       </c>
@@ -2173,9 +2232,10 @@
         <v>40</v>
       </c>
       <c r="J35" s="3"/>
-      <c r="K35" s="8"/>
-    </row>
-    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K35" s="3"/>
+      <c r="L35" s="8"/>
+    </row>
+    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>47</v>
       </c>
@@ -2192,17 +2252,19 @@
         <v>40</v>
       </c>
       <c r="J36" s="3"/>
-      <c r="K36" s="8"/>
-    </row>
-    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K36" s="3"/>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="E37"/>
       <c r="I37" s="40"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="8"/>
-    </row>
-    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K37" s="3"/>
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>63</v>
       </c>
@@ -2225,9 +2287,10 @@
         <v>50</v>
       </c>
       <c r="J38" s="3"/>
-      <c r="K38" s="8"/>
-    </row>
-    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K38" s="3"/>
+      <c r="L38" s="8"/>
+    </row>
+    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>63</v>
       </c>
@@ -2246,9 +2309,10 @@
         <v>50</v>
       </c>
       <c r="J39" s="3"/>
-      <c r="K39" s="8"/>
-    </row>
-    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K39" s="3"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>63</v>
       </c>
@@ -2267,9 +2331,10 @@
         <v>50</v>
       </c>
       <c r="J40" s="3"/>
-      <c r="K40" s="8"/>
-    </row>
-    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K40" s="3"/>
+      <c r="L40" s="8"/>
+    </row>
+    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>63</v>
       </c>
@@ -2288,9 +2353,10 @@
         <v>50</v>
       </c>
       <c r="J41" s="3"/>
-      <c r="K41" s="8"/>
-    </row>
-    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K41" s="3"/>
+      <c r="L41" s="8"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="26"/>
@@ -2298,9 +2364,10 @@
       <c r="E42"/>
       <c r="I42" s="40"/>
       <c r="J42" s="3"/>
-      <c r="K42" s="8"/>
-    </row>
-    <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K42" s="3"/>
+      <c r="L42" s="8"/>
+    </row>
+    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>85</v>
       </c>
@@ -2325,9 +2392,10 @@
       <c r="J43" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K43" s="8"/>
-    </row>
-    <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K43" s="3"/>
+      <c r="L43" s="8"/>
+    </row>
+    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>85</v>
       </c>
@@ -2347,9 +2415,10 @@
       <c r="J44" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K44" s="3"/>
+      <c r="L44" s="8"/>
+    </row>
+    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>85</v>
       </c>
@@ -2370,9 +2439,10 @@
       <c r="J45" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K45" s="8"/>
-    </row>
-    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K45" s="3"/>
+      <c r="L45" s="8"/>
+    </row>
+    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>85</v>
       </c>
@@ -2393,11 +2463,12 @@
       <c r="J46" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K46" s="8" t="s">
+      <c r="K46" s="3"/>
+      <c r="L46" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
         <v>85</v>
       </c>
@@ -2417,70 +2488,72 @@
       <c r="J47" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="K47" s="8"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K47" s="3"/>
+      <c r="L47" s="8"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="E48" s="30"/>
       <c r="I48" s="40"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="8"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="K48" s="3"/>
+      <c r="L48" s="8"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="E49" s="30"/>
       <c r="I49" s="40"/>
-      <c r="K49" s="8"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L49" s="8"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="E50" s="30"/>
       <c r="I50" s="40"/>
-      <c r="K50" s="8"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L50" s="8"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="E51" s="30"/>
       <c r="I51" s="40"/>
-      <c r="K51" s="8"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L51" s="8"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="E52" s="30"/>
       <c r="I52" s="40"/>
-      <c r="K52" s="8"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L52" s="8"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="E53" s="30"/>
       <c r="I53" s="40"/>
-      <c r="K53" s="8"/>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L53" s="8"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E55" s="10"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E59" s="27"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E63" s="27"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
COPD abbreviated - GT-101
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D62C1A-7D52-FB41-B97E-ECBA3C0635C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC31780-2A8A-484A-9E34-12B1596999A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2080" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1260" yWindow="2080" windowWidth="34320" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2258" uniqueCount="238">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -223,9 +223,6 @@
     <t>PulmonaryFibrosis</t>
   </si>
   <si>
-    <t>Chronic Obstructive Pulmonary Disease</t>
-  </si>
-  <si>
     <t>:yes?</t>
   </si>
   <si>
@@ -247,12 +244,6 @@
     <t>Positive</t>
   </si>
   <si>
-    <t>Donor history of smoking</t>
-  </si>
-  <si>
-    <t>Recipient daily dose of prednisolone at registration</t>
-  </si>
-  <si>
     <t>Transplant type</t>
   </si>
   <si>
@@ -262,19 +253,7 @@
     <t>Disease Group</t>
   </si>
   <si>
-    <t>Recipient age at transplant</t>
-  </si>
-  <si>
     <t>Donor:recipient calculated TLC mismatch</t>
-  </si>
-  <si>
-    <t>Recipient FVC at registration</t>
-  </si>
-  <si>
-    <t>Recipient bilirubin at registration</t>
-  </si>
-  <si>
-    <t>Recipient cholesterol at registration</t>
   </si>
   <si>
     <t>Negative</t>
@@ -761,6 +740,24 @@
   </si>
   <si>
     <t>:boxed</t>
+  </si>
+  <si>
+    <t>History of smoking</t>
+  </si>
+  <si>
+    <t>Age at transplant</t>
+  </si>
+  <si>
+    <t>FVC at registration</t>
+  </si>
+  <si>
+    <t>Bilirubin at registration</t>
+  </si>
+  <si>
+    <t>Cholesterol at registration</t>
+  </si>
+  <si>
+    <t>CMV</t>
   </si>
 </sst>
 </file>
@@ -1371,7 +1368,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -1401,7 +1398,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1"/>
     </row>
@@ -1411,7 +1408,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B9" s="1"/>
     </row>
@@ -1421,7 +1418,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -1434,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1461,13 +1458,13 @@
         <v>16</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>19</v>
@@ -1479,13 +1476,13 @@
         <v>21</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>22</v>
@@ -1493,31 +1490,31 @@
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>65</v>
+        <v>237</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="I2" s="40">
         <v>100</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>10</v>
@@ -1526,14 +1523,14 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3">
         <v>0.29226000000000002</v>
@@ -1542,7 +1539,7 @@
         <v>100</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>10</v>
@@ -1551,13 +1548,13 @@
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1566,7 +1563,7 @@
         <v>100</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>10</v>
@@ -1586,13 +1583,13 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>67</v>
+        <v>232</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>37</v>
@@ -1604,7 +1601,7 @@
         <v>25</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="I6" s="40">
         <v>80</v>
@@ -1616,12 +1613,12 @@
         <v>10</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>10</v>
@@ -1643,19 +1640,19 @@
         <v>10</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="10" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E8">
         <v>0.24582000000000001</v>
@@ -1670,7 +1667,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1689,19 +1686,19 @@
         <v>52</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I10" s="40">
         <v>30</v>
@@ -1715,11 +1712,11 @@
         <v>52</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C11" s="65"/>
       <c r="D11" s="17" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E11">
         <v>0.27340999999999999</v>
@@ -1736,11 +1733,11 @@
         <v>52</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="14" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E12">
         <v>0.48875999999999997</v>
@@ -1768,19 +1765,19 @@
         <v>19</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E14">
         <v>4.9770000000000002E-2</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I14" s="40">
         <v>70</v>
@@ -1794,11 +1791,11 @@
         <v>19</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="10" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1823,13 +1820,13 @@
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>57</v>
@@ -1838,7 +1835,7 @@
         <v>-0.40421000000000001</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I17" s="40">
         <v>20</v>
@@ -1849,7 +1846,7 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>49</v>
@@ -1870,7 +1867,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>50</v>
@@ -1891,14 +1888,14 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="10" t="s">
-        <v>59</v>
+        <v>225</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1923,25 +1920,25 @@
     </row>
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>72</v>
+        <v>233</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E22">
         <v>0.24259</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I22" s="40">
         <v>10</v>
@@ -1949,18 +1946,18 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="8" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E23">
         <v>-5.6439999999999997E-2</v>
@@ -1974,14 +1971,14 @@
     </row>
     <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="57" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E24">
         <v>-5.0889999999999998E-2</v>
@@ -1995,14 +1992,14 @@
     </row>
     <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="57" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2016,14 +2013,14 @@
     </row>
     <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C26" s="55"/>
       <c r="D26" s="57" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E26">
         <v>0.22292000000000001</v>
@@ -2048,28 +2045,28 @@
     </row>
     <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D28" s="56" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E28">
         <v>-0.15398000000000001</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>10</v>
@@ -2078,14 +2075,14 @@
     </row>
     <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="56" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -2095,7 +2092,7 @@
         <v>90</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>10</v>
@@ -2104,14 +2101,14 @@
     </row>
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="56" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E30">
         <v>-7.1799999999999998E-3</v>
@@ -2121,7 +2118,7 @@
         <v>90</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>10</v>
@@ -2130,14 +2127,14 @@
     </row>
     <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="56" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -2147,7 +2144,7 @@
         <v>90</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>10</v>
@@ -2171,22 +2168,22 @@
         <v>47</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>74</v>
+        <v>234</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E33">
         <v>0.10249</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="I33" s="40">
         <v>40</v>
@@ -2200,10 +2197,10 @@
         <v>47</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="E34">
         <v>-1.281E-2</v>
@@ -2220,10 +2217,10 @@
         <v>47</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2240,10 +2237,10 @@
         <v>47</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E36">
         <v>-0.26149</v>
@@ -2266,22 +2263,22 @@
     </row>
     <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>75</v>
+        <v>235</v>
       </c>
       <c r="D38" s="58" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="E38">
         <v>0.10959000000000001</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I38" s="40">
         <v>50</v>
@@ -2292,14 +2289,14 @@
     </row>
     <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="58" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2314,14 +2311,14 @@
     </row>
     <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="58" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E40">
         <v>9.579E-2</v>
@@ -2336,14 +2333,14 @@
     </row>
     <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C41" s="26"/>
       <c r="D41" s="58" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E41">
         <v>0.20563999999999999</v>
@@ -2369,41 +2366,41 @@
     </row>
     <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>76</v>
+        <v>236</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E43">
         <v>0.13420000000000001</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="I43" s="40">
         <v>60</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="8"/>
     </row>
     <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2413,21 +2410,21 @@
         <v>60</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="27" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E45">
         <v>0.13092999999999999</v>
@@ -2437,21 +2434,21 @@
         <v>60</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="8"/>
     </row>
     <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C46" s="61"/>
       <c r="D46" s="3" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E46">
         <v>-0.56130000000000002</v>
@@ -2461,23 +2458,23 @@
         <v>60</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="8" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="C47" s="61"/>
       <c r="D47" s="3" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="E47" s="29">
         <v>0</v>
@@ -2486,7 +2483,7 @@
         <v>60</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="8"/>
@@ -2594,19 +2591,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2617,10 +2614,10 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2631,10 +2628,10 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2645,10 +2642,10 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2659,10 +2656,10 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2673,10 +2670,10 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2702,104 +2699,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" t="s">
         <v>100</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2831,47 +2828,47 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D2" s="54"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2904,10 +2901,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -27667,7 +27664,7 @@
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>51</v>
@@ -27678,7 +27675,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -27699,7 +27696,7 @@
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>10</v>
@@ -27746,8 +27743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -27762,12 +27759,11 @@
     <col min="8" max="8" width="14.5" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.5" style="3" customWidth="1"/>
     <col min="10" max="10" width="10.5" style="39" customWidth="1"/>
-    <col min="11" max="11" width="15" style="32" customWidth="1"/>
-    <col min="12" max="12" width="4.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.5" style="32" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -27775,10 +27771,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>17</v>
@@ -27796,13 +27792,16 @@
         <v>21</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -27832,7 +27831,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -27858,7 +27857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="16"/>
@@ -27868,9 +27867,9 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>48</v>
@@ -27888,19 +27887,19 @@
         <v>0.74607999999999997</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" s="39">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>49</v>
@@ -27916,7 +27915,7 @@
         <v>0.45213999999999999</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -27924,16 +27923,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="34" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E7">
         <v>-0.40466000000000002</v>
@@ -27942,7 +27941,7 @@
         <v>1.00088</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -27950,16 +27949,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="34" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -27968,7 +27967,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -27976,7 +27975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="16"/>
@@ -27986,18 +27985,18 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C10" s="64" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="48" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -28006,26 +28005,26 @@
         <v>0</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J10" s="39">
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C11" s="64"/>
       <c r="D11" s="50" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E11">
         <v>-0.12438</v>
@@ -28034,7 +28033,7 @@
         <v>0.22475999999999999</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -28042,16 +28041,16 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="48" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E12">
         <v>-6.1949999999999998E-2</v>
@@ -28060,7 +28059,7 @@
         <v>0.44635999999999998</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -28068,7 +28067,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="16"/>
@@ -28079,7 +28078,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>53</v>
       </c>
@@ -28087,7 +28086,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="D14" s="46" t="s">
         <v>37</v>
@@ -28103,13 +28102,13 @@
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J14" s="39">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>53</v>
       </c>
@@ -28135,7 +28134,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="18"/>
@@ -28150,10 +28149,10 @@
         <v>55</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>44</v>
@@ -28169,7 +28168,7 @@
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="39">
         <v>60</v>
@@ -28180,7 +28179,7 @@
         <v>55</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="48" t="s">
@@ -28206,7 +28205,7 @@
         <v>55</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="48" t="s">
@@ -28232,7 +28231,7 @@
         <v>55</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="48" t="s">
@@ -28265,13 +28264,13 @@
     </row>
     <row r="22" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D22" s="48" t="s">
         <v>37</v>
@@ -28296,7 +28295,7 @@
     </row>
     <row r="23" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>10</v>
@@ -28441,16 +28440,16 @@
     </row>
     <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D30" s="60" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E30">
         <v>-9.5509999999999998E-2</v>
@@ -28459,10 +28458,10 @@
         <v>-0.43454999999999999</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="63">
@@ -28471,14 +28470,14 @@
     </row>
     <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C31" s="51"/>
       <c r="D31" s="56" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E31">
         <v>-3.7769999999999998E-2</v>
@@ -28487,7 +28486,7 @@
         <v>-0.38550000000000001</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="32"/>
@@ -28497,14 +28496,14 @@
     </row>
     <row r="32" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C32" s="51"/>
       <c r="D32" s="56" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E32">
         <v>-1.883E-2</v>
@@ -28513,7 +28512,7 @@
         <v>-0.49630000000000002</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="33"/>
@@ -28525,14 +28524,14 @@
     </row>
     <row r="33" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="48" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -28541,7 +28540,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="32"/>
@@ -28553,14 +28552,14 @@
     </row>
     <row r="34" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="56" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E34">
         <v>0.13814000000000001</v>
@@ -28569,7 +28568,7 @@
         <v>-0.12119000000000001</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="32"/>
@@ -28596,13 +28595,13 @@
         <v>47</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="E36">
         <v>-0.42215999999999998</v>
@@ -28611,10 +28610,10 @@
         <v>0.71482000000000001</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="39">
@@ -28626,11 +28625,11 @@
         <v>47</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C37" s="59"/>
       <c r="D37" s="53" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E37">
         <v>-0.22505</v>
@@ -28639,7 +28638,7 @@
         <v>0.39432</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
@@ -28652,11 +28651,11 @@
         <v>47</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="53" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -28665,7 +28664,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
@@ -28678,11 +28677,11 @@
         <v>47</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="53" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E39">
         <v>-0.11767</v>
@@ -28691,7 +28690,7 @@
         <v>0.1</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -28715,13 +28714,13 @@
         <v>56</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D41" s="53" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="E41">
         <v>7.1510000000000004E-2</v>
@@ -28730,10 +28729,10 @@
         <v>0.17363000000000001</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="39">
@@ -28745,10 +28744,10 @@
         <v>56</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -28757,7 +28756,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="J42" s="39">
         <v>90</v>
@@ -28768,10 +28767,10 @@
         <v>56</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="E43">
         <v>2.8039999999999999E-2</v>
@@ -28780,7 +28779,7 @@
         <v>-0.20066000000000001</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="J43" s="39">
         <v>90</v>
@@ -28891,44 +28890,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -28970,7 +28969,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F1" s="6"/>
     </row>
@@ -36816,15 +36815,15 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -36832,7 +36831,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
@@ -36846,7 +36845,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -36857,7 +36856,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -36865,7 +36864,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>51</v>
@@ -36879,7 +36878,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -36887,10 +36886,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -36901,7 +36900,7 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -36909,10 +36908,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -36920,10 +36919,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -36934,7 +36933,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
react-bootstrap v1.6.1 and delinting
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC31780-2A8A-484A-9E34-12B1596999A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82ADED29-11E5-7B43-935D-46722E43C0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2080" windowWidth="34320" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="4500" yWindow="5560" windowWidth="34320" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>

</xml_diff>

<commit_message>
connected up info? column to popups
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1983C3D3-7687-E740-A4A8-F9E251B32073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3784F4-8093-5C4A-8715-CEBAD32E5964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="5500" windowWidth="34320" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="5100" yWindow="5500" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2256" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="231">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -220,9 +220,6 @@
     <t>PulmonaryFibrosis</t>
   </si>
   <si>
-    <t>:yes?</t>
-  </si>
-  <si>
     <t>:d-gp</t>
   </si>
   <si>
@@ -284,12 +281,6 @@
   </si>
   <si>
     <t>Donor has smoked?</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>?how much</t>
   </si>
   <si>
     <t>note that knots are post-t specific</t>
@@ -1356,7 +1347,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -1386,7 +1377,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B7" s="1"/>
     </row>
@@ -1396,7 +1387,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B9" s="1"/>
     </row>
@@ -1406,7 +1397,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B11" s="1"/>
     </row>
@@ -1419,8 +1410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1446,13 +1437,13 @@
         <v>16</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F1" s="11" t="s">
         <v>19</v>
@@ -1464,13 +1455,13 @@
         <v>21</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>22</v>
@@ -1478,31 +1469,28 @@
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>71</v>
-      </c>
       <c r="C2" s="26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>80</v>
+        <v>123</v>
       </c>
       <c r="I2" s="40">
         <v>100</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>10</v>
@@ -1511,14 +1499,14 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="26"/>
       <c r="D3" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3">
         <v>0.29226000000000002</v>
@@ -1527,7 +1515,7 @@
         <v>100</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>10</v>
@@ -1536,13 +1524,13 @@
     </row>
     <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -1551,7 +1539,7 @@
         <v>100</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>10</v>
@@ -1571,13 +1559,13 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>37</v>
@@ -1588,9 +1576,6 @@
       <c r="F6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="I6" s="40">
         <v>80</v>
       </c>
@@ -1601,12 +1586,12 @@
         <v>10</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>10</v>
@@ -1628,19 +1613,19 @@
         <v>10</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E8">
         <v>0.24582000000000001</v>
@@ -1655,7 +1640,7 @@
         <v>10</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -1674,10 +1659,10 @@
         <v>51</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C10" s="65" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D10" s="14">
         <v>0</v>
@@ -1686,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I10" s="40">
         <v>30</v>
@@ -1700,11 +1685,11 @@
         <v>51</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C11" s="65"/>
       <c r="D11" s="17" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E11">
         <v>0.27340999999999999</v>
@@ -1721,11 +1706,11 @@
         <v>51</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="14" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E12">
         <v>0.48875999999999997</v>
@@ -1753,19 +1738,19 @@
         <v>19</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E14">
         <v>4.9770000000000002E-2</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I14" s="40">
         <v>70</v>
@@ -1779,11 +1764,11 @@
         <v>19</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C15" s="26"/>
       <c r="D15" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1808,13 +1793,13 @@
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>56</v>
@@ -1823,7 +1808,7 @@
         <v>-0.40421000000000001</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I17" s="40">
         <v>20</v>
@@ -1834,7 +1819,7 @@
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>48</v>
@@ -1855,7 +1840,7 @@
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>49</v>
@@ -1876,14 +1861,14 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1908,25 +1893,25 @@
     </row>
     <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D22" s="57" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E22">
         <v>0.24259</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I22" s="40">
         <v>10</v>
@@ -1934,18 +1919,18 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E23">
         <v>-5.6439999999999997E-2</v>
@@ -1959,14 +1944,14 @@
     </row>
     <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C24" s="31"/>
       <c r="D24" s="57" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E24">
         <v>-5.0889999999999998E-2</v>
@@ -1980,14 +1965,14 @@
     </row>
     <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C25" s="31"/>
       <c r="D25" s="57" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -2001,14 +1986,14 @@
     </row>
     <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C26" s="55"/>
       <c r="D26" s="57" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E26">
         <v>0.22292000000000001</v>
@@ -2033,28 +2018,28 @@
     </row>
     <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C28" s="26" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" s="56" t="s">
         <v>171</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>174</v>
       </c>
       <c r="E28">
         <v>-0.15398000000000001</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>10</v>
@@ -2063,14 +2048,14 @@
     </row>
     <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C29" s="26"/>
       <c r="D29" s="56" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -2080,7 +2065,7 @@
         <v>90</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>10</v>
@@ -2089,14 +2074,14 @@
     </row>
     <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C30" s="26"/>
       <c r="D30" s="56" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E30">
         <v>-7.1799999999999998E-3</v>
@@ -2106,7 +2091,7 @@
         <v>90</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K30" s="3" t="s">
         <v>10</v>
@@ -2115,14 +2100,14 @@
     </row>
     <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="56" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E31">
         <v>0</v>
@@ -2132,7 +2117,7 @@
         <v>90</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>10</v>
@@ -2156,22 +2141,22 @@
         <v>46</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E33">
         <v>0.10249</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I33" s="40">
         <v>40</v>
@@ -2185,10 +2170,10 @@
         <v>46</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E34">
         <v>-1.281E-2</v>
@@ -2205,10 +2190,10 @@
         <v>46</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2225,10 +2210,10 @@
         <v>46</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E36">
         <v>-0.26149</v>
@@ -2251,22 +2236,22 @@
     </row>
     <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D38" s="58" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E38">
         <v>0.10959000000000001</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I38" s="40">
         <v>50</v>
@@ -2277,14 +2262,14 @@
     </row>
     <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C39" s="26"/>
       <c r="D39" s="58" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2299,14 +2284,14 @@
     </row>
     <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C40" s="26"/>
       <c r="D40" s="58" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E40">
         <v>9.579E-2</v>
@@ -2321,14 +2306,14 @@
     </row>
     <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C41" s="26"/>
       <c r="D41" s="58" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E41">
         <v>0.20563999999999999</v>
@@ -2354,41 +2339,41 @@
     </row>
     <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E43">
         <v>0.13420000000000001</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I43" s="40">
         <v>60</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="8"/>
     </row>
     <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2398,21 +2383,21 @@
         <v>60</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C45" s="26"/>
       <c r="D45" s="27" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="E45">
         <v>0.13092999999999999</v>
@@ -2422,21 +2407,21 @@
         <v>60</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="8"/>
     </row>
     <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C46" s="61"/>
       <c r="D46" s="3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E46">
         <v>-0.56130000000000002</v>
@@ -2446,23 +2431,23 @@
         <v>60</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B47" s="12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C47" s="61"/>
       <c r="D47" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E47" s="29">
         <v>0</v>
@@ -2471,7 +2456,7 @@
         <v>60</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="8"/>
@@ -2579,19 +2564,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2602,10 +2587,10 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D2" s="62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2616,10 +2601,10 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2630,10 +2615,10 @@
         <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D4" s="62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2644,10 +2629,10 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2658,10 +2643,10 @@
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2687,104 +2672,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" s="36" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B3" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" t="s">
         <v>108</v>
-      </c>
-      <c r="E5" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" t="s">
         <v>109</v>
-      </c>
-      <c r="E6" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2816,47 +2801,47 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B1" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D2" s="54"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2889,10 +2874,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -27652,7 +27637,7 @@
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>50</v>
@@ -27663,7 +27648,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
@@ -27684,7 +27669,7 @@
     </row>
     <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>10</v>
@@ -27731,8 +27716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -27759,10 +27744,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>17</v>
@@ -27780,13 +27765,13 @@
         <v>21</v>
       </c>
       <c r="J1" s="38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -27812,9 +27797,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="10"/>
-      <c r="I2" s="10" t="s">
-        <v>10</v>
-      </c>
+      <c r="I2" s="10"/>
       <c r="J2" s="39">
         <v>20</v>
       </c>
@@ -27857,7 +27840,7 @@
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>47</v>
@@ -27875,19 +27858,17 @@
         <v>0.74607999999999997</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H5" s="13"/>
-      <c r="I5" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="I5" s="10"/>
       <c r="J5" s="39">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>48</v>
@@ -27903,7 +27884,7 @@
         <v>0.45213999999999999</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -27913,14 +27894,14 @@
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="34" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E7">
         <v>-0.40466000000000002</v>
@@ -27929,7 +27910,7 @@
         <v>1.00088</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -27939,14 +27920,14 @@
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="34" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -27955,7 +27936,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -27978,10 +27959,10 @@
         <v>51</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D10" s="48">
         <v>0</v>
@@ -27993,12 +27974,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H10" s="10"/>
-      <c r="I10" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="I10" s="10"/>
       <c r="J10" s="39">
         <v>70</v>
       </c>
@@ -28008,11 +27987,11 @@
         <v>51</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C11" s="64"/>
       <c r="D11" s="50" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E11">
         <v>-0.12438</v>
@@ -28021,7 +28000,7 @@
         <v>0.22475999999999999</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -28034,11 +28013,11 @@
         <v>51</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="48" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E12">
         <v>-6.1949999999999998E-2</v>
@@ -28047,7 +28026,7 @@
         <v>0.44635999999999998</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -28074,7 +28053,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D14" s="46" t="s">
         <v>37</v>
@@ -28089,9 +28068,7 @@
         <v>25</v>
       </c>
       <c r="H14" s="10"/>
-      <c r="I14" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="I14" s="10"/>
       <c r="J14" s="39">
         <v>50</v>
       </c>
@@ -28137,10 +28114,10 @@
         <v>54</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>43</v>
@@ -28155,9 +28132,7 @@
         <v>25</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="I17" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="I17" s="10"/>
       <c r="J17" s="39">
         <v>60</v>
       </c>
@@ -28167,7 +28142,7 @@
         <v>54</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="48" t="s">
@@ -28193,7 +28168,7 @@
         <v>54</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="48" t="s">
@@ -28219,7 +28194,7 @@
         <v>54</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="48" t="s">
@@ -28252,13 +28227,13 @@
     </row>
     <row r="22" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="23" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D22" s="48" t="s">
         <v>37</v>
@@ -28283,7 +28258,7 @@
     </row>
     <row r="23" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="23" t="s">
         <v>10</v>
@@ -28428,16 +28403,16 @@
     </row>
     <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D30" s="60" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E30">
         <v>-9.5509999999999998E-2</v>
@@ -28446,10 +28421,10 @@
         <v>-0.43454999999999999</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="63">
@@ -28458,14 +28433,14 @@
     </row>
     <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C31" s="51"/>
       <c r="D31" s="56" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E31">
         <v>-3.7769999999999998E-2</v>
@@ -28474,7 +28449,7 @@
         <v>-0.38550000000000001</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="32"/>
@@ -28484,14 +28459,14 @@
     </row>
     <row r="32" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C32" s="51"/>
       <c r="D32" s="56" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E32">
         <v>-1.883E-2</v>
@@ -28500,7 +28475,7 @@
         <v>-0.49630000000000002</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="33"/>
@@ -28512,14 +28487,14 @@
     </row>
     <row r="33" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="48" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -28528,7 +28503,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="32"/>
@@ -28540,14 +28515,14 @@
     </row>
     <row r="34" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="56" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E34">
         <v>0.13814000000000001</v>
@@ -28556,7 +28531,7 @@
         <v>-0.12119000000000001</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="32"/>
@@ -28583,13 +28558,13 @@
         <v>46</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E36">
         <v>-0.42215999999999998</v>
@@ -28598,10 +28573,10 @@
         <v>0.71482000000000001</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I36" s="10"/>
       <c r="J36" s="39">
@@ -28613,11 +28588,11 @@
         <v>46</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C37" s="59"/>
       <c r="D37" s="53" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="E37">
         <v>-0.22505</v>
@@ -28626,7 +28601,7 @@
         <v>0.39432</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
@@ -28639,11 +28614,11 @@
         <v>46</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C38" s="59"/>
       <c r="D38" s="53" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -28652,7 +28627,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
@@ -28665,11 +28640,11 @@
         <v>46</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C39" s="59"/>
       <c r="D39" s="53" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E39">
         <v>-0.11767</v>
@@ -28678,7 +28653,7 @@
         <v>0.1</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
@@ -28702,13 +28677,13 @@
         <v>55</v>
       </c>
       <c r="B41" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D41" s="53" t="s">
         <v>193</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>208</v>
-      </c>
-      <c r="D41" s="53" t="s">
-        <v>196</v>
       </c>
       <c r="E41">
         <v>7.1510000000000004E-2</v>
@@ -28717,10 +28692,10 @@
         <v>0.17363000000000001</v>
       </c>
       <c r="G41" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="H41" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>129</v>
       </c>
       <c r="I41" s="10"/>
       <c r="J41" s="39">
@@ -28732,10 +28707,10 @@
         <v>55</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -28744,7 +28719,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J42" s="39">
         <v>90</v>
@@ -28755,10 +28730,10 @@
         <v>55</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E43">
         <v>2.8039999999999999E-2</v>
@@ -28767,7 +28742,7 @@
         <v>-0.20066000000000001</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J43" s="39">
         <v>90</v>
@@ -28878,44 +28853,44 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -28957,7 +28932,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F1" s="6"/>
     </row>
@@ -36803,15 +36778,15 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -36819,7 +36794,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>11</v>
@@ -36833,7 +36808,7 @@
         <v>51</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -36844,7 +36819,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -36852,7 +36827,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>50</v>
@@ -36866,7 +36841,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -36874,10 +36849,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -36888,7 +36863,7 @@
         <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -36896,10 +36871,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -36907,10 +36882,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -36921,7 +36896,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Leila lung info boxes - minus text vis
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C001F12-1BD5-284E-A242-47C157EF2820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10576EC-27B0-0C48-B1F8-C7CC5523D6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="520" windowWidth="34320" windowHeight="21040" activeTab="3" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="10820" yWindow="1360" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2249" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="238">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -738,6 +738,49 @@
   <si>
     <t>Donor/Recipient TLC mismatch</t>
   </si>
+  <si>
+    <t xml:space="preserve">{:title "NYHA CLASS – New York Heart Association Classification"
+:content [:&lt;&gt;
+[:p "Class I – for example shortness of breath when walking or climbing stairs"]
+[:p "Class II – for example mild shortness of breath that limits ordinary activities"]
+[:p "Class III – only comfortable at rest, limited in doing normal activities such as walking short distances (20m – 100m)"
+[:p "Class IV – symptoms even at rest, usually bedbound patients."]
+]}
+</t>
+  </si>
+  <si>
+    <t>{:title "FVC - Forced Vital Capacity" 
+ :content "Forced vital capacity.  A measure of lung function."}</t>
+  </si>
+  <si>
+    <t>Has the patient ever had any thoracotomy procedures?</t>
+  </si>
+  <si>
+    <t>{:title "BMI – Body Mass Index"
+:content [:&lt;&gt;
+[:p "Weight (in kg) divided by height (in metres) squared"]
+[:p "For example, for weight 70kg, and height 1.57m, the BMI is 28.4 = 70 ÷ (1.57 × 1.57)"]
+]}</t>
+  </si>
+  <si>
+    <t>{:title "Cholesterol"
+:content "total cholesterol"}</t>
+  </si>
+  <si>
+    <t>{:title "Donor / Recipient TLC mismatch"
+:content 
+[:p "Donor to recipient calculated total lung capacity mismatch"]
+[:p "Total Lung Capacity is the volume (measured in litres) that the lungs can hold."]
+[:p "TLC mismatch means the difference in lung capacity between the donor and the recipient."]
+[:p "This figure is usually calculated when the characteristics of the donor is known."]}</t>
+  </si>
+  <si>
+    <t>{:title "CMV - Cytomegalovirus"
+:content [:&lt;&gt;
+[:p "Has the donor ever had the common virus Cytomegalovirus?"]
+[:p "If  the donor is positive for CMV it means the recipient will receive some medication after transplant."]
+]}</t>
+  </si>
 </sst>
 </file>
 
@@ -747,7 +790,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -802,6 +845,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Symbol"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -850,7 +906,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1013,6 +1069,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1409,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1466,7 +1537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="399" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>69</v>
       </c>
@@ -1484,6 +1555,9 @@
       </c>
       <c r="F2" s="3" t="s">
         <v>123</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>237</v>
       </c>
       <c r="I2" s="40">
         <v>100</v>
@@ -2015,7 +2089,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>74</v>
       </c>
@@ -2033,6 +2107,9 @@
       </c>
       <c r="F28" s="3" t="s">
         <v>123</v>
+      </c>
+      <c r="H28" s="47" t="s">
+        <v>236</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
@@ -2135,7 +2212,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="166" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
@@ -2156,6 +2233,9 @@
       </c>
       <c r="G33" s="3" t="s">
         <v>125</v>
+      </c>
+      <c r="H33" s="47" t="s">
+        <v>232</v>
       </c>
       <c r="I33" s="40">
         <v>40</v>
@@ -2336,7 +2416,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="106" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>75</v>
       </c>
@@ -2354,6 +2434,9 @@
       </c>
       <c r="F43" s="3" t="s">
         <v>123</v>
+      </c>
+      <c r="H43" s="47" t="s">
+        <v>235</v>
       </c>
       <c r="I43" s="40">
         <v>60</v>
@@ -2852,8 +2935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40555AFB-A6C9-3045-A3E5-4DA101B4901E}">
   <dimension ref="A1:D3206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1339" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D1374"/>
+    <sheetView topLeftCell="A1339" workbookViewId="0">
+      <selection activeCell="X1352" sqref="X1352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -27715,8 +27798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -28108,7 +28191,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>54</v>
       </c>
@@ -28131,7 +28214,9 @@
         <v>25</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
+      <c r="I17" s="66" t="s">
+        <v>231</v>
+      </c>
       <c r="J17" s="39">
         <v>60</v>
       </c>
@@ -28157,7 +28242,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
+      <c r="I18" s="67"/>
       <c r="J18" s="39">
         <v>60</v>
       </c>
@@ -28183,7 +28268,7 @@
         <v>25</v>
       </c>
       <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="I19" s="65"/>
       <c r="J19" s="39">
         <v>60</v>
       </c>
@@ -28209,7 +28294,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
+      <c r="I20" s="65"/>
       <c r="J20" s="39">
         <v>60</v>
       </c>
@@ -28222,7 +28307,7 @@
       <c r="E21"/>
       <c r="F21"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
+      <c r="I21" s="65"/>
     </row>
     <row r="22" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
@@ -28247,7 +28332,9 @@
         <v>25</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>233</v>
+      </c>
       <c r="J22" s="39">
         <v>100</v>
       </c>
@@ -28552,7 +28639,7 @@
       <c r="K35" s="32"/>
       <c r="L35" s="32"/>
     </row>
-    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" ht="187" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>46</v>
       </c>
@@ -28577,7 +28664,9 @@
       <c r="H36" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="I36" s="10"/>
+      <c r="I36" s="68" t="s">
+        <v>232</v>
+      </c>
       <c r="J36" s="39">
         <v>80</v>
       </c>
@@ -28671,7 +28760,7 @@
       <c r="I40" s="34"/>
       <c r="J40" s="44"/>
     </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" ht="343" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
@@ -28696,7 +28785,9 @@
       <c r="H41" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="I41" s="10"/>
+      <c r="I41" s="69" t="s">
+        <v>234</v>
+      </c>
       <c r="J41" s="39">
         <v>90</v>
       </c>
@@ -28901,7 +28992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3FE1BB-1AC5-6D40-AB0F-F4D73062F511}">
   <dimension ref="A1:N1015"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A385" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C400"/>
     </sheetView>
   </sheetViews>
@@ -28966,7 +29057,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.9905913207</v>
+        <v>0.99059132100000002</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
@@ -28984,7 +29075,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>0.9810283045</v>
+        <v>0.98102830500000004</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
@@ -29016,7 +29107,7 @@
         <v>13</v>
       </c>
       <c r="C6">
-        <v>0.97140577260000005</v>
+        <v>0.97140577299999997</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
@@ -29032,7 +29123,7 @@
         <v>16</v>
       </c>
       <c r="C7">
-        <v>0.96179730730000002</v>
+        <v>0.96179730699999999</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
@@ -29048,7 +29139,7 @@
         <v>18</v>
       </c>
       <c r="C8">
-        <v>0.95692094130000005</v>
+        <v>0.95692094100000002</v>
       </c>
       <c r="E8" s="3">
         <v>1</v>
@@ -29064,7 +29155,7 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>0.94715603059999998</v>
+        <v>0.94715603100000001</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
@@ -29080,7 +29171,7 @@
         <v>25</v>
       </c>
       <c r="C10">
-        <v>0.94220261329999999</v>
+        <v>0.94220261299999997</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
@@ -29096,7 +29187,7 @@
         <v>26</v>
       </c>
       <c r="C11">
-        <v>0.93716899279999999</v>
+        <v>0.93716899300000001</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -29112,7 +29203,7 @@
         <v>42</v>
       </c>
       <c r="C12">
-        <v>0.93212459039999995</v>
+        <v>0.93212459000000003</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -29128,7 +29219,7 @@
         <v>56</v>
       </c>
       <c r="C13">
-        <v>0.92701903009999997</v>
+        <v>0.92701902999999997</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
@@ -29143,7 +29234,7 @@
         <v>57</v>
       </c>
       <c r="C14">
-        <v>0.92185905420000003</v>
+        <v>0.92185905400000001</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -29157,7 +29248,7 @@
         <v>69</v>
       </c>
       <c r="C15">
-        <v>0.91669159889999996</v>
+        <v>0.91669159899999997</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
@@ -29171,7 +29262,7 @@
         <v>70</v>
       </c>
       <c r="C16">
-        <v>0.90626014580000003</v>
+        <v>0.90626014600000004</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -29185,7 +29276,7 @@
         <v>80</v>
       </c>
       <c r="C17">
-        <v>0.90096447430000004</v>
+        <v>0.90096447400000002</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -29199,7 +29290,7 @@
         <v>96</v>
       </c>
       <c r="C18">
-        <v>0.89558997780000005</v>
+        <v>0.89558997799999995</v>
       </c>
       <c r="E18" s="3">
         <v>1</v>
@@ -29227,7 +29318,7 @@
         <v>105</v>
       </c>
       <c r="C20">
-        <v>0.88451604949999996</v>
+        <v>0.88451605</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -29241,7 +29332,7 @@
         <v>114</v>
       </c>
       <c r="C21">
-        <v>0.87895389970000004</v>
+        <v>0.87895389999999995</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
@@ -29255,7 +29346,7 @@
         <v>121</v>
       </c>
       <c r="C22">
-        <v>0.87328199549999996</v>
+        <v>0.873281996</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
@@ -29269,7 +29360,7 @@
         <v>122</v>
       </c>
       <c r="C23">
-        <v>0.86756776719999995</v>
+        <v>0.86756776700000005</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -29283,7 +29374,7 @@
         <v>138</v>
       </c>
       <c r="C24">
-        <v>0.86180697979999998</v>
+        <v>0.86180698</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
@@ -29297,7 +29388,7 @@
         <v>157</v>
       </c>
       <c r="C25">
-        <v>0.85601025529999997</v>
+        <v>0.85601025500000005</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
@@ -29311,7 +29402,7 @@
         <v>173</v>
       </c>
       <c r="C26">
-        <v>0.84427747249999996</v>
+        <v>0.844277473</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -29325,7 +29416,7 @@
         <v>177</v>
       </c>
       <c r="C27">
-        <v>0.83826440479999997</v>
+        <v>0.83826440499999999</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
@@ -29339,7 +29430,7 @@
         <v>193</v>
       </c>
       <c r="C28">
-        <v>0.83223046919999999</v>
+        <v>0.83223046899999997</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
@@ -29353,7 +29444,7 @@
         <v>237</v>
       </c>
       <c r="C29">
-        <v>0.82619825830000004</v>
+        <v>0.82619825800000002</v>
       </c>
       <c r="E29" s="3">
         <v>1</v>
@@ -29367,7 +29458,7 @@
         <v>276</v>
       </c>
       <c r="C30">
-        <v>0.82012119610000001</v>
+        <v>0.820121196</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
@@ -29381,7 +29472,7 @@
         <v>289</v>
       </c>
       <c r="C31">
-        <v>0.81401348419999997</v>
+        <v>0.81401348399999995</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
@@ -29395,7 +29486,7 @@
         <v>292</v>
       </c>
       <c r="C32">
-        <v>0.80781451179999997</v>
+        <v>0.80781451199999998</v>
       </c>
       <c r="E32" s="3">
         <v>1</v>
@@ -29409,7 +29500,7 @@
         <v>297</v>
       </c>
       <c r="C33">
-        <v>0.80158932569999997</v>
+        <v>0.80158932599999999</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
@@ -29423,7 +29514,7 @@
         <v>303</v>
       </c>
       <c r="C34">
-        <v>0.79533016229999998</v>
+        <v>0.79533016199999995</v>
       </c>
       <c r="E34" s="3">
         <v>1</v>
@@ -29437,7 +29528,7 @@
         <v>310</v>
       </c>
       <c r="C35">
-        <v>0.78899315820000004</v>
+        <v>0.78899315800000003</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
@@ -29451,7 +29542,7 @@
         <v>328</v>
       </c>
       <c r="C36">
-        <v>0.78261299610000001</v>
+        <v>0.78261299600000001</v>
       </c>
       <c r="E36" s="3">
         <v>1</v>
@@ -29465,7 +29556,7 @@
         <v>403</v>
       </c>
       <c r="C37">
-        <v>0.77553552889999999</v>
+        <v>0.775535529</v>
       </c>
       <c r="E37" s="3">
         <v>1</v>
@@ -29479,7 +29570,7 @@
         <v>439</v>
       </c>
       <c r="C38">
-        <v>0.76840616559999997</v>
+        <v>0.768406166</v>
       </c>
       <c r="E38" s="3">
         <v>1</v>
@@ -29507,7 +29598,7 @@
         <v>553</v>
       </c>
       <c r="C40">
-        <v>0.74696827929999998</v>
+        <v>0.74696827899999996</v>
       </c>
       <c r="E40" s="3">
         <v>1</v>
@@ -29521,7 +29612,7 @@
         <v>558</v>
       </c>
       <c r="C41">
-        <v>0.73960507750000004</v>
+        <v>0.73960507799999997</v>
       </c>
       <c r="E41" s="3">
         <v>1</v>
@@ -29535,7 +29626,7 @@
         <v>723</v>
       </c>
       <c r="C42">
-        <v>0.73144059459999999</v>
+        <v>0.73144059500000003</v>
       </c>
       <c r="E42" s="3">
         <v>1</v>
@@ -29549,7 +29640,7 @@
         <v>732</v>
       </c>
       <c r="C43">
-        <v>0.72292952749999995</v>
+        <v>0.72292952799999999</v>
       </c>
       <c r="E43" s="3">
         <v>1</v>
@@ -29563,7 +29654,7 @@
         <v>827</v>
       </c>
       <c r="C44">
-        <v>0.71339093990000002</v>
+        <v>0.71339094000000003</v>
       </c>
       <c r="E44" s="3">
         <v>1</v>
@@ -29577,7 +29668,7 @@
         <v>1258</v>
       </c>
       <c r="C45">
-        <v>0.70309116009999995</v>
+        <v>0.70309116000000005</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
@@ -29591,7 +29682,7 @@
         <v>1572</v>
       </c>
       <c r="C46">
-        <v>0.6886668091</v>
+        <v>0.68866680899999999</v>
       </c>
       <c r="E46" s="3">
         <v>1</v>
@@ -29605,7 +29696,7 @@
         <v>1582</v>
       </c>
       <c r="C47">
-        <v>0.67395089279999998</v>
+        <v>0.673950893</v>
       </c>
       <c r="E47" s="3">
         <v>1</v>
@@ -29619,7 +29710,7 @@
         <v>1826</v>
       </c>
       <c r="C48">
-        <v>0.67395089279999998</v>
+        <v>0.673950893</v>
       </c>
       <c r="E48" s="3">
         <v>47</v>
@@ -29647,7 +29738,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0.99595214759999995</v>
+        <v>0.99595214799999998</v>
       </c>
       <c r="E50" s="3">
         <f>E49+1</f>
@@ -29662,7 +29753,7 @@
         <v>1</v>
       </c>
       <c r="C51">
-        <v>0.99189401850000003</v>
+        <v>0.99189401899999996</v>
       </c>
       <c r="E51" s="3">
         <f t="shared" ref="E51:E114" si="0">E50+1</f>
@@ -29677,7 +29768,7 @@
         <v>3</v>
       </c>
       <c r="C52">
-        <v>0.98781764490000001</v>
+        <v>0.98781764500000002</v>
       </c>
       <c r="E52" s="3">
         <f t="shared" si="0"/>
@@ -29692,7 +29783,7 @@
         <v>4</v>
       </c>
       <c r="C53">
-        <v>0.98577652729999998</v>
+        <v>0.98577652699999996</v>
       </c>
       <c r="E53" s="3">
         <f t="shared" si="0"/>
@@ -29707,7 +29798,7 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>0.98169148279999996</v>
+        <v>0.98169148299999998</v>
       </c>
       <c r="E54" s="3">
         <f t="shared" si="0"/>
@@ -29737,7 +29828,7 @@
         <v>8</v>
       </c>
       <c r="C56">
-        <v>0.97758839230000005</v>
+        <v>0.97758839200000003</v>
       </c>
       <c r="E56" s="3">
         <f t="shared" si="0"/>
@@ -29752,7 +29843,7 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>0.97552817140000003</v>
+        <v>0.975528171</v>
       </c>
       <c r="E57" s="3">
         <f t="shared" si="0"/>
@@ -29767,7 +29858,7 @@
         <v>10</v>
       </c>
       <c r="C58">
-        <v>0.97346472070000001</v>
+        <v>0.97346472100000003</v>
       </c>
       <c r="E58" s="3">
         <f t="shared" si="0"/>
@@ -29782,7 +29873,7 @@
         <v>11</v>
       </c>
       <c r="C59">
-        <v>0.97139814680000003</v>
+        <v>0.97139814700000005</v>
       </c>
       <c r="E59" s="3">
         <f t="shared" si="0"/>
@@ -29797,7 +29888,7 @@
         <v>13</v>
       </c>
       <c r="C60">
-        <v>0.96932595109999997</v>
+        <v>0.96932595099999996</v>
       </c>
       <c r="E60" s="3">
         <f t="shared" si="0"/>
@@ -29812,7 +29903,7 @@
         <v>15</v>
       </c>
       <c r="C61">
-        <v>0.96724892839999999</v>
+        <v>0.96724892799999995</v>
       </c>
       <c r="E61" s="3">
         <f t="shared" si="0"/>
@@ -29827,7 +29918,7 @@
         <v>16</v>
       </c>
       <c r="C62">
-        <v>0.96516623589999995</v>
+        <v>0.96516623599999996</v>
       </c>
       <c r="E62" s="3">
         <f t="shared" si="0"/>
@@ -29842,7 +29933,7 @@
         <v>19</v>
       </c>
       <c r="C63">
-        <v>0.96100342569999997</v>
+        <v>0.96100342599999999</v>
       </c>
       <c r="E63" s="3">
         <f t="shared" si="0"/>
@@ -29857,7 +29948,7 @@
         <v>25</v>
       </c>
       <c r="C64">
-        <v>0.95891491549999996</v>
+        <v>0.95891491600000001</v>
       </c>
       <c r="E64" s="3">
         <f t="shared" si="0"/>
@@ -29872,7 +29963,7 @@
         <v>29</v>
       </c>
       <c r="C65">
-        <v>0.95682276369999997</v>
+        <v>0.95682276399999999</v>
       </c>
       <c r="E65" s="3">
         <f t="shared" si="0"/>
@@ -29887,7 +29978,7 @@
         <v>38</v>
       </c>
       <c r="C66">
-        <v>0.95473155620000005</v>
+        <v>0.95473155600000004</v>
       </c>
       <c r="E66" s="3">
         <f t="shared" si="0"/>
@@ -29902,7 +29993,7 @@
         <v>41</v>
       </c>
       <c r="C67">
-        <v>0.95263867310000006</v>
+        <v>0.95263867300000005</v>
       </c>
       <c r="E67" s="3">
         <f t="shared" si="0"/>
@@ -29917,7 +30008,7 @@
         <v>42</v>
       </c>
       <c r="C68">
-        <v>0.94845026649999997</v>
+        <v>0.94845026700000001</v>
       </c>
       <c r="E68" s="3">
         <f t="shared" si="0"/>
@@ -29932,7 +30023,7 @@
         <v>44</v>
       </c>
       <c r="C69">
-        <v>0.94634940290000003</v>
+        <v>0.94634940300000003</v>
       </c>
       <c r="E69" s="3">
         <f t="shared" si="0"/>
@@ -29947,7 +30038,7 @@
         <v>49</v>
       </c>
       <c r="C70">
-        <v>0.94424345210000005</v>
+        <v>0.94424345200000004</v>
       </c>
       <c r="E70" s="3">
         <f t="shared" si="0"/>
@@ -29962,7 +30053,7 @@
         <v>52</v>
       </c>
       <c r="C71">
-        <v>0.94003248589999999</v>
+        <v>0.940032486</v>
       </c>
       <c r="E71" s="3">
         <f t="shared" si="0"/>
@@ -29977,7 +30068,7 @@
         <v>64</v>
       </c>
       <c r="C72">
-        <v>0.93791963919999999</v>
+        <v>0.93791963899999997</v>
       </c>
       <c r="E72" s="3">
         <f t="shared" si="0"/>
@@ -29992,7 +30083,7 @@
         <v>72</v>
       </c>
       <c r="C73">
-        <v>0.93579956720000002</v>
+        <v>0.935799567</v>
       </c>
       <c r="E73" s="3">
         <f t="shared" si="0"/>
@@ -30007,7 +30098,7 @@
         <v>115</v>
       </c>
       <c r="C74">
-        <v>0.93362172710000002</v>
+        <v>0.93362172700000001</v>
       </c>
       <c r="E74" s="3">
         <f t="shared" si="0"/>
@@ -30022,7 +30113,7 @@
         <v>118</v>
       </c>
       <c r="C75">
-        <v>0.93144532710000005</v>
+        <v>0.93144532700000005</v>
       </c>
       <c r="E75" s="3">
         <f t="shared" si="0"/>
@@ -30037,7 +30128,7 @@
         <v>121</v>
       </c>
       <c r="C76">
-        <v>0.92926759120000002</v>
+        <v>0.929267591</v>
       </c>
       <c r="E76" s="3">
         <f t="shared" si="0"/>
@@ -30067,7 +30158,7 @@
         <v>127</v>
       </c>
       <c r="C78">
-        <v>0.92490771780000003</v>
+        <v>0.92490771800000005</v>
       </c>
       <c r="E78" s="3">
         <f t="shared" si="0"/>
@@ -30082,7 +30173,7 @@
         <v>141</v>
       </c>
       <c r="C79">
-        <v>0.92272432510000002</v>
+        <v>0.92272432500000001</v>
       </c>
       <c r="E79" s="3">
         <f t="shared" si="0"/>
@@ -30097,7 +30188,7 @@
         <v>144</v>
       </c>
       <c r="C80">
-        <v>0.92054093250000002</v>
+        <v>0.92054093299999995</v>
       </c>
       <c r="E80" s="3">
         <f t="shared" si="0"/>
@@ -30112,7 +30203,7 @@
         <v>163</v>
       </c>
       <c r="C81">
-        <v>0.91835374910000001</v>
+        <v>0.918353749</v>
       </c>
       <c r="E81" s="3">
         <f t="shared" si="0"/>
@@ -30127,7 +30218,7 @@
         <v>164</v>
       </c>
       <c r="C82">
-        <v>0.91616604189999995</v>
+        <v>0.91616604199999996</v>
       </c>
       <c r="E82" s="3">
         <f t="shared" si="0"/>
@@ -30142,7 +30233,7 @@
         <v>166</v>
       </c>
       <c r="C83">
-        <v>0.91396695539999995</v>
+        <v>0.91396695500000003</v>
       </c>
       <c r="E83" s="3">
         <f t="shared" si="0"/>
@@ -30157,7 +30248,7 @@
         <v>190</v>
       </c>
       <c r="C84">
-        <v>0.91176486069999996</v>
+        <v>0.91176486099999998</v>
       </c>
       <c r="E84" s="3">
         <f t="shared" si="0"/>
@@ -30172,7 +30263,7 @@
         <v>191</v>
       </c>
       <c r="C85">
-        <v>0.90955653569999995</v>
+        <v>0.90955653599999997</v>
       </c>
       <c r="E85" s="3">
         <f t="shared" si="0"/>
@@ -30187,7 +30278,7 @@
         <v>198</v>
       </c>
       <c r="C86">
-        <v>0.90734337430000001</v>
+        <v>0.90734337399999998</v>
       </c>
       <c r="E86" s="3">
         <f t="shared" si="0"/>
@@ -30202,7 +30293,7 @@
         <v>203</v>
       </c>
       <c r="C87">
-        <v>0.90512700540000002</v>
+        <v>0.90512700499999998</v>
       </c>
       <c r="E87" s="3">
         <f t="shared" si="0"/>
@@ -30217,7 +30308,7 @@
         <v>213</v>
       </c>
       <c r="C88">
-        <v>0.90291124060000005</v>
+        <v>0.90291124099999998</v>
       </c>
       <c r="E88" s="3">
         <f t="shared" si="0"/>
@@ -30232,7 +30323,7 @@
         <v>215</v>
       </c>
       <c r="C89">
-        <v>0.90069523269999996</v>
+        <v>0.90069523299999998</v>
       </c>
       <c r="E89" s="3">
         <f t="shared" si="0"/>
@@ -30247,7 +30338,7 @@
         <v>216</v>
       </c>
       <c r="C90">
-        <v>0.89847549230000001</v>
+        <v>0.89847549199999999</v>
       </c>
       <c r="E90" s="3">
         <f t="shared" si="0"/>
@@ -30262,7 +30353,7 @@
         <v>269</v>
       </c>
       <c r="C91">
-        <v>0.89625520039999995</v>
+        <v>0.89625520000000003</v>
       </c>
       <c r="E91" s="3">
         <f t="shared" si="0"/>
@@ -30277,7 +30368,7 @@
         <v>298</v>
       </c>
       <c r="C92">
-        <v>0.89402620430000002</v>
+        <v>0.89402620399999999</v>
       </c>
       <c r="E92" s="3">
         <f t="shared" si="0"/>
@@ -30307,7 +30398,7 @@
         <v>348</v>
       </c>
       <c r="C94">
-        <v>0.88953363760000004</v>
+        <v>0.88953363799999996</v>
       </c>
       <c r="E94" s="3">
         <f t="shared" si="0"/>
@@ -30322,7 +30413,7 @@
         <v>351</v>
       </c>
       <c r="C95">
-        <v>0.88726569070000005</v>
+        <v>0.88726569099999997</v>
       </c>
       <c r="E95" s="3">
         <f t="shared" si="0"/>
@@ -30337,7 +30428,7 @@
         <v>361</v>
       </c>
       <c r="C96">
-        <v>0.88497506370000001</v>
+        <v>0.88497506400000003</v>
       </c>
       <c r="E96" s="3">
         <f t="shared" si="0"/>
@@ -30352,7 +30443,7 @@
         <v>375</v>
       </c>
       <c r="C97">
-        <v>0.88267546659999996</v>
+        <v>0.88267546699999999</v>
       </c>
       <c r="E97" s="3">
         <f t="shared" si="0"/>
@@ -30367,7 +30458,7 @@
         <v>398</v>
       </c>
       <c r="C98">
-        <v>0.88031540949999998</v>
+        <v>0.88031541000000002</v>
       </c>
       <c r="E98" s="3">
         <f t="shared" si="0"/>
@@ -30382,7 +30473,7 @@
         <v>412</v>
       </c>
       <c r="C99">
-        <v>0.87793052439999997</v>
+        <v>0.87793052400000005</v>
       </c>
       <c r="E99" s="3">
         <f t="shared" si="0"/>
@@ -30397,7 +30488,7 @@
         <v>415</v>
       </c>
       <c r="C100">
-        <v>0.87554539539999998</v>
+        <v>0.87554539499999995</v>
       </c>
       <c r="E100" s="3">
         <f t="shared" si="0"/>
@@ -30412,7 +30503,7 @@
         <v>436</v>
       </c>
       <c r="C101">
-        <v>0.87314483890000005</v>
+        <v>0.87314483899999995</v>
       </c>
       <c r="E101" s="3">
         <f t="shared" si="0"/>
@@ -30427,7 +30518,7 @@
         <v>441</v>
       </c>
       <c r="C102">
-        <v>0.87073922439999996</v>
+        <v>0.87073922400000003</v>
       </c>
       <c r="E102" s="3">
         <f t="shared" si="0"/>
@@ -30442,7 +30533,7 @@
         <v>463</v>
       </c>
       <c r="C103">
-        <v>0.86832145260000004</v>
+        <v>0.86832145299999997</v>
       </c>
       <c r="E103" s="3">
         <f t="shared" si="0"/>
@@ -30472,7 +30563,7 @@
         <v>548</v>
       </c>
       <c r="C105">
-        <v>0.86104089039999998</v>
+        <v>0.86104088999999995</v>
       </c>
       <c r="E105" s="3">
         <f t="shared" si="0"/>
@@ -30487,7 +30578,7 @@
         <v>552</v>
       </c>
       <c r="C106">
-        <v>0.8586034561</v>
+        <v>0.85860345599999999</v>
       </c>
       <c r="E106" s="3">
         <f t="shared" si="0"/>
@@ -30502,7 +30593,7 @@
         <v>575</v>
       </c>
       <c r="C107">
-        <v>0.85616503909999997</v>
+        <v>0.85616503899999996</v>
       </c>
       <c r="E107" s="3">
         <f t="shared" si="0"/>
@@ -30517,7 +30608,7 @@
         <v>644</v>
       </c>
       <c r="C108">
-        <v>0.8537199446</v>
+        <v>0.85371994500000004</v>
       </c>
       <c r="E108" s="3">
         <f t="shared" si="0"/>
@@ -30532,7 +30623,7 @@
         <v>652</v>
       </c>
       <c r="C109">
-        <v>0.85124728650000003</v>
+        <v>0.85124728699999996</v>
       </c>
       <c r="E109" s="3">
         <f t="shared" si="0"/>
@@ -30547,7 +30638,7 @@
         <v>660</v>
       </c>
       <c r="C110">
-        <v>0.84875995309999996</v>
+        <v>0.84875995299999996</v>
       </c>
       <c r="E110" s="3">
         <f t="shared" si="0"/>
@@ -30562,7 +30653,7 @@
         <v>661</v>
       </c>
       <c r="C111">
-        <v>0.84626992670000001</v>
+        <v>0.84626992700000003</v>
       </c>
       <c r="E111" s="3">
         <f t="shared" si="0"/>
@@ -30577,7 +30668,7 @@
         <v>697</v>
       </c>
       <c r="C112">
-        <v>0.84371941910000003</v>
+        <v>0.84371941900000003</v>
       </c>
       <c r="E112" s="3">
         <f t="shared" si="0"/>
@@ -30592,7 +30683,7 @@
         <v>739</v>
       </c>
       <c r="C113">
-        <v>0.84096157920000003</v>
+        <v>0.84096157900000001</v>
       </c>
       <c r="E113" s="3">
         <f t="shared" si="0"/>
@@ -30607,7 +30698,7 @@
         <v>740</v>
       </c>
       <c r="C114">
-        <v>0.83820055459999998</v>
+        <v>0.83820055500000001</v>
       </c>
       <c r="E114" s="3">
         <f t="shared" si="0"/>
@@ -30622,7 +30713,7 @@
         <v>753</v>
       </c>
       <c r="C115">
-        <v>0.83538700789999998</v>
+        <v>0.83538700799999999</v>
       </c>
       <c r="E115" s="3">
         <f t="shared" ref="E115:E142" si="1">E114+1</f>
@@ -30637,7 +30728,7 @@
         <v>755</v>
       </c>
       <c r="C116">
-        <v>0.83255572990000004</v>
+        <v>0.83255573000000005</v>
       </c>
       <c r="E116" s="3">
         <f t="shared" si="1"/>
@@ -30652,7 +30743,7 @@
         <v>811</v>
       </c>
       <c r="C117">
-        <v>0.82948640090000003</v>
+        <v>0.82948640100000004</v>
       </c>
       <c r="E117" s="3">
         <f t="shared" si="1"/>
@@ -30667,7 +30758,7 @@
         <v>826</v>
       </c>
       <c r="C118">
-        <v>0.82639208180000001</v>
+        <v>0.82639208200000003</v>
       </c>
       <c r="E118" s="3">
         <f t="shared" si="1"/>
@@ -30682,7 +30773,7 @@
         <v>836</v>
       </c>
       <c r="C119">
-        <v>0.82329505130000002</v>
+        <v>0.823295051</v>
       </c>
       <c r="E119" s="3">
         <f t="shared" si="1"/>
@@ -30697,7 +30788,7 @@
         <v>838</v>
       </c>
       <c r="C120">
-        <v>0.8201905625</v>
+        <v>0.82019056300000004</v>
       </c>
       <c r="E120" s="3">
         <f t="shared" si="1"/>
@@ -30712,7 +30803,7 @@
         <v>907</v>
       </c>
       <c r="C121">
-        <v>0.81708320290000003</v>
+        <v>0.81708320300000004</v>
       </c>
       <c r="E121" s="3">
         <f t="shared" si="1"/>
@@ -30727,7 +30818,7 @@
         <v>938</v>
       </c>
       <c r="C122">
-        <v>0.81396899649999999</v>
+        <v>0.81396899700000003</v>
       </c>
       <c r="E122" s="3">
         <f t="shared" si="1"/>
@@ -30742,7 +30833,7 @@
         <v>954</v>
       </c>
       <c r="C123">
-        <v>0.81084977120000001</v>
+        <v>0.810849771</v>
       </c>
       <c r="E123" s="3">
         <f t="shared" si="1"/>
@@ -30757,7 +30848,7 @@
         <v>987</v>
       </c>
       <c r="C124">
-        <v>0.80771277850000001</v>
+        <v>0.80771277900000005</v>
       </c>
       <c r="E124" s="3">
         <f t="shared" si="1"/>
@@ -30772,7 +30863,7 @@
         <v>1008</v>
       </c>
       <c r="C125">
-        <v>0.80454621790000003</v>
+        <v>0.80454621800000004</v>
       </c>
       <c r="E125" s="3">
         <f t="shared" si="1"/>
@@ -30787,7 +30878,7 @@
         <v>1059</v>
       </c>
       <c r="C126">
-        <v>0.80133932959999998</v>
+        <v>0.80133933000000002</v>
       </c>
       <c r="E126" s="3">
         <f t="shared" si="1"/>
@@ -30802,7 +30893,7 @@
         <v>1066</v>
       </c>
       <c r="C127">
-        <v>0.79810030580000002</v>
+        <v>0.79810030600000004</v>
       </c>
       <c r="E127" s="3">
         <f t="shared" si="1"/>
@@ -30817,7 +30908,7 @@
         <v>1136</v>
       </c>
       <c r="C128">
-        <v>0.79436713049999996</v>
+        <v>0.794367131</v>
       </c>
       <c r="E128" s="3">
         <f t="shared" si="1"/>
@@ -30832,7 +30923,7 @@
         <v>1148</v>
       </c>
       <c r="C129">
-        <v>0.79056284430000001</v>
+        <v>0.79056284399999999</v>
       </c>
       <c r="E129" s="3">
         <f t="shared" si="1"/>
@@ -30847,7 +30938,7 @@
         <v>1191</v>
       </c>
       <c r="C130">
-        <v>0.78662663460000004</v>
+        <v>0.78662663499999996</v>
       </c>
       <c r="E130" s="3">
         <f t="shared" si="1"/>
@@ -30862,7 +30953,7 @@
         <v>1317</v>
       </c>
       <c r="C131">
-        <v>0.78264898810000005</v>
+        <v>0.78264898800000005</v>
       </c>
       <c r="E131" s="3">
         <f t="shared" si="1"/>
@@ -30877,7 +30968,7 @@
         <v>1343</v>
       </c>
       <c r="C132">
-        <v>0.77863818549999997</v>
+        <v>0.77863818600000001</v>
       </c>
       <c r="E132" s="3">
         <f t="shared" si="1"/>
@@ -30892,7 +30983,7 @@
         <v>1351</v>
       </c>
       <c r="C133">
-        <v>0.77457579980000002</v>
+        <v>0.77457580000000004</v>
       </c>
       <c r="E133" s="3">
         <f t="shared" si="1"/>
@@ -30907,7 +30998,7 @@
         <v>1557</v>
       </c>
       <c r="C134">
-        <v>0.76878888460000006</v>
+        <v>0.76878888499999998</v>
       </c>
       <c r="E134" s="3">
         <f t="shared" si="1"/>
@@ -30922,7 +31013,7 @@
         <v>1563</v>
       </c>
       <c r="C135">
-        <v>0.76299650279999998</v>
+        <v>0.76299650299999999</v>
       </c>
       <c r="E135" s="3">
         <f t="shared" si="1"/>
@@ -30937,7 +31028,7 @@
         <v>1645</v>
       </c>
       <c r="C136">
-        <v>0.75706410280000003</v>
+        <v>0.75706410300000004</v>
       </c>
       <c r="E136" s="3">
         <f t="shared" si="1"/>
@@ -30952,7 +31043,7 @@
         <v>1733</v>
       </c>
       <c r="C137">
-        <v>0.75110615550000004</v>
+        <v>0.75110615599999997</v>
       </c>
       <c r="E137" s="3">
         <f t="shared" si="1"/>
@@ -30967,7 +31058,7 @@
         <v>1745</v>
       </c>
       <c r="C138">
-        <v>0.74512972570000002</v>
+        <v>0.74512972600000005</v>
       </c>
       <c r="E138" s="3">
         <f t="shared" si="1"/>
@@ -30982,7 +31073,7 @@
         <v>1762</v>
       </c>
       <c r="C139">
-        <v>0.73899710169999999</v>
+        <v>0.73899710200000002</v>
       </c>
       <c r="E139" s="3">
         <f t="shared" si="1"/>
@@ -30997,7 +31088,7 @@
         <v>1783</v>
       </c>
       <c r="C140">
-        <v>0.73258415750000005</v>
+        <v>0.73258415799999999</v>
       </c>
       <c r="E140" s="3">
         <f t="shared" si="1"/>
@@ -31056,7 +31147,7 @@
         <v>0</v>
       </c>
       <c r="C144">
-        <v>0.99709106359999999</v>
+        <v>0.99709106400000003</v>
       </c>
       <c r="E144" s="3">
         <f t="shared" ref="E144:E207" si="2">E143+1</f>
@@ -31086,7 +31177,7 @@
         <v>2</v>
       </c>
       <c r="C146">
-        <v>0.99126163570000003</v>
+        <v>0.99126163599999995</v>
       </c>
       <c r="E146" s="3">
         <f t="shared" si="2"/>
@@ -31101,7 +31192,7 @@
         <v>5</v>
       </c>
       <c r="C147">
-        <v>0.98833676820000005</v>
+        <v>0.98833676800000003</v>
       </c>
       <c r="E147" s="3">
         <f t="shared" si="2"/>
@@ -31116,7 +31207,7 @@
         <v>10</v>
       </c>
       <c r="C148">
-        <v>0.98539286039999996</v>
+        <v>0.98539286000000004</v>
       </c>
       <c r="E148" s="3">
         <f t="shared" si="2"/>
@@ -31131,7 +31222,7 @@
         <v>28</v>
       </c>
       <c r="C149">
-        <v>0.98242341860000004</v>
+        <v>0.98242341899999996</v>
       </c>
       <c r="E149" s="3">
         <f t="shared" si="2"/>
@@ -31146,7 +31237,7 @@
         <v>51</v>
       </c>
       <c r="C150">
-        <v>0.97944666960000004</v>
+        <v>0.97944666999999996</v>
       </c>
       <c r="E150" s="3">
         <f t="shared" si="2"/>
@@ -31161,7 +31252,7 @@
         <v>52</v>
       </c>
       <c r="C151">
-        <v>0.97646330930000003</v>
+        <v>0.976463309</v>
       </c>
       <c r="E151" s="3">
         <f t="shared" si="2"/>
@@ -31176,7 +31267,7 @@
         <v>53</v>
       </c>
       <c r="C152">
-        <v>0.97348155930000002</v>
+        <v>0.973481559</v>
       </c>
       <c r="E152" s="3">
         <f t="shared" si="2"/>
@@ -31191,7 +31282,7 @@
         <v>58</v>
       </c>
       <c r="C153">
-        <v>0.97048518340000001</v>
+        <v>0.97048518299999997</v>
       </c>
       <c r="E153" s="3">
         <f t="shared" si="2"/>
@@ -31206,7 +31297,7 @@
         <v>82</v>
       </c>
       <c r="C154">
-        <v>0.96745803919999995</v>
+        <v>0.96745803900000005</v>
       </c>
       <c r="E154" s="3">
         <f t="shared" si="2"/>
@@ -31221,7 +31312,7 @@
         <v>88</v>
       </c>
       <c r="C155">
-        <v>0.9644238141</v>
+        <v>0.96442381399999999</v>
       </c>
       <c r="E155" s="3">
         <f t="shared" si="2"/>
@@ -31236,7 +31327,7 @@
         <v>91</v>
       </c>
       <c r="C156">
-        <v>0.96138915059999996</v>
+        <v>0.961389151</v>
       </c>
       <c r="E156" s="3">
         <f t="shared" si="2"/>
@@ -31251,7 +31342,7 @@
         <v>103</v>
       </c>
       <c r="C157">
-        <v>0.95831493540000001</v>
+        <v>0.95831493499999998</v>
       </c>
       <c r="E157" s="3">
         <f t="shared" si="2"/>
@@ -31266,7 +31357,7 @@
         <v>112</v>
       </c>
       <c r="C158">
-        <v>0.95521207060000002</v>
+        <v>0.95521207100000005</v>
       </c>
       <c r="E158" s="3">
         <f t="shared" si="2"/>
@@ -31281,7 +31372,7 @@
         <v>119</v>
       </c>
       <c r="C159">
-        <v>0.95210651180000005</v>
+        <v>0.95210651199999996</v>
       </c>
       <c r="E159" s="3">
         <f t="shared" si="2"/>
@@ -31296,7 +31387,7 @@
         <v>154</v>
       </c>
       <c r="C160">
-        <v>0.94590151509999998</v>
+        <v>0.94590151499999997</v>
       </c>
       <c r="E160" s="3">
         <f t="shared" si="2"/>
@@ -31311,7 +31402,7 @@
         <v>188</v>
       </c>
       <c r="C161">
-        <v>0.94277780389999999</v>
+        <v>0.942777804</v>
       </c>
       <c r="E161" s="3">
         <f t="shared" si="2"/>
@@ -31341,7 +31432,7 @@
         <v>208</v>
       </c>
       <c r="C163">
-        <v>0.93647499810000001</v>
+        <v>0.936474998</v>
       </c>
       <c r="E163" s="3">
         <f t="shared" si="2"/>
@@ -31356,7 +31447,7 @@
         <v>246</v>
       </c>
       <c r="C164">
-        <v>0.93330510739999994</v>
+        <v>0.93330510700000002</v>
       </c>
       <c r="E164" s="3">
         <f t="shared" si="2"/>
@@ -31371,7 +31462,7 @@
         <v>262</v>
       </c>
       <c r="C165">
-        <v>0.93012490329999997</v>
+        <v>0.93012490299999995</v>
       </c>
       <c r="E165" s="3">
         <f t="shared" si="2"/>
@@ -31386,7 +31477,7 @@
         <v>267</v>
       </c>
       <c r="C166">
-        <v>0.92694525049999998</v>
+        <v>0.92694525100000003</v>
       </c>
       <c r="E166" s="3">
         <f t="shared" si="2"/>
@@ -31401,7 +31492,7 @@
         <v>268</v>
       </c>
       <c r="C167">
-        <v>0.92375646730000005</v>
+        <v>0.92375646700000003</v>
       </c>
       <c r="E167" s="3">
         <f t="shared" si="2"/>
@@ -31416,7 +31507,7 @@
         <v>274</v>
       </c>
       <c r="C168">
-        <v>0.9205493937</v>
+        <v>0.92054939400000002</v>
       </c>
       <c r="E168" s="3">
         <f t="shared" si="2"/>
@@ -31431,7 +31522,7 @@
         <v>301</v>
       </c>
       <c r="C169">
-        <v>0.91732764460000005</v>
+        <v>0.91732764499999997</v>
       </c>
       <c r="E169" s="3">
         <f t="shared" si="2"/>
@@ -31446,7 +31537,7 @@
         <v>312</v>
       </c>
       <c r="C170">
-        <v>0.91409033490000002</v>
+        <v>0.91409033500000003</v>
       </c>
       <c r="E170" s="3">
         <f t="shared" si="2"/>
@@ -31461,7 +31552,7 @@
         <v>318</v>
       </c>
       <c r="C171">
-        <v>0.91083740840000005</v>
+        <v>0.91083740800000002</v>
       </c>
       <c r="E171" s="3">
         <f t="shared" si="2"/>
@@ -31476,7 +31567,7 @@
         <v>327</v>
       </c>
       <c r="C172">
-        <v>0.90755319369999998</v>
+        <v>0.90755319400000001</v>
       </c>
       <c r="E172" s="3">
         <f t="shared" si="2"/>
@@ -31491,7 +31582,7 @@
         <v>330</v>
       </c>
       <c r="C173">
-        <v>0.90426033780000004</v>
+        <v>0.90426033800000005</v>
       </c>
       <c r="E173" s="3">
         <f t="shared" si="2"/>
@@ -31506,7 +31597,7 @@
         <v>331</v>
       </c>
       <c r="C174">
-        <v>0.8976743948</v>
+        <v>0.89767439500000001</v>
       </c>
       <c r="E174" s="3">
         <f t="shared" si="2"/>
@@ -31521,7 +31612,7 @@
         <v>344</v>
       </c>
       <c r="C175">
-        <v>0.89092815709999995</v>
+        <v>0.89092815700000005</v>
       </c>
       <c r="E175" s="3">
         <f t="shared" si="2"/>
@@ -31536,7 +31627,7 @@
         <v>373</v>
       </c>
       <c r="C176">
-        <v>0.88739951409999995</v>
+        <v>0.88739951399999994</v>
       </c>
       <c r="E176" s="3">
         <f t="shared" si="2"/>
@@ -31551,7 +31642,7 @@
         <v>374</v>
       </c>
       <c r="C177">
-        <v>0.88384901849999997</v>
+        <v>0.88384901900000001</v>
       </c>
       <c r="E177" s="3">
         <f t="shared" si="2"/>
@@ -31566,7 +31657,7 @@
         <v>394</v>
       </c>
       <c r="C178">
-        <v>0.88028088950000005</v>
+        <v>0.88028088999999998</v>
       </c>
       <c r="E178" s="3">
         <f t="shared" si="2"/>
@@ -31581,7 +31672,7 @@
         <v>415</v>
       </c>
       <c r="C179">
-        <v>0.87670175480000001</v>
+        <v>0.87670175500000003</v>
       </c>
       <c r="E179" s="3">
         <f t="shared" si="2"/>
@@ -31596,7 +31687,7 @@
         <v>439</v>
       </c>
       <c r="C180">
-        <v>0.87309248809999995</v>
+        <v>0.87309248800000006</v>
       </c>
       <c r="E180" s="3">
         <f t="shared" si="2"/>
@@ -31611,7 +31702,7 @@
         <v>449</v>
       </c>
       <c r="C181">
-        <v>0.86947705529999997</v>
+        <v>0.86947705500000005</v>
       </c>
       <c r="E181" s="3">
         <f t="shared" si="2"/>
@@ -31626,7 +31717,7 @@
         <v>450</v>
       </c>
       <c r="C182">
-        <v>0.86586011060000001</v>
+        <v>0.86586011100000004</v>
       </c>
       <c r="E182" s="3">
         <f t="shared" si="2"/>
@@ -31641,7 +31732,7 @@
         <v>452</v>
       </c>
       <c r="C183">
-        <v>0.8622248964</v>
+        <v>0.86222489599999996</v>
       </c>
       <c r="E183" s="3">
         <f t="shared" si="2"/>
@@ -31656,7 +31747,7 @@
         <v>472</v>
       </c>
       <c r="C184">
-        <v>0.8585799798</v>
+        <v>0.85857998000000002</v>
       </c>
       <c r="E184" s="3">
         <f t="shared" si="2"/>
@@ -31671,7 +31762,7 @@
         <v>480</v>
       </c>
       <c r="C185">
-        <v>0.85490774270000003</v>
+        <v>0.85490774300000005</v>
       </c>
       <c r="E185" s="3">
         <f t="shared" si="2"/>
@@ -31701,7 +31792,7 @@
         <v>511</v>
       </c>
       <c r="C187">
-        <v>0.84751451730000005</v>
+        <v>0.84751451700000002</v>
       </c>
       <c r="E187" s="3">
         <f t="shared" si="2"/>
@@ -31716,7 +31807,7 @@
         <v>568</v>
       </c>
       <c r="C188">
-        <v>0.84379798289999997</v>
+        <v>0.84379798299999997</v>
       </c>
       <c r="E188" s="3">
         <f t="shared" si="2"/>
@@ -31731,7 +31822,7 @@
         <v>593</v>
       </c>
       <c r="C189">
-        <v>0.84005665190000001</v>
+        <v>0.84005665200000001</v>
       </c>
       <c r="E189" s="3">
         <f t="shared" si="2"/>
@@ -31746,7 +31837,7 @@
         <v>595</v>
       </c>
       <c r="C190">
-        <v>0.83630768150000001</v>
+        <v>0.83630768200000005</v>
       </c>
       <c r="E190" s="3">
         <f t="shared" si="2"/>
@@ -31761,7 +31852,7 @@
         <v>604</v>
       </c>
       <c r="C191">
-        <v>0.83253725609999996</v>
+        <v>0.83253725599999995</v>
       </c>
       <c r="E191" s="3">
         <f t="shared" si="2"/>
@@ -31776,7 +31867,7 @@
         <v>620</v>
       </c>
       <c r="C192">
-        <v>0.82874480890000002</v>
+        <v>0.82874480900000003</v>
       </c>
       <c r="E192" s="3">
         <f t="shared" si="2"/>
@@ -31791,7 +31882,7 @@
         <v>625</v>
       </c>
       <c r="C193">
-        <v>0.82493477979999996</v>
+        <v>0.82493477999999998</v>
       </c>
       <c r="E193" s="3">
         <f t="shared" si="2"/>
@@ -31806,7 +31897,7 @@
         <v>665</v>
       </c>
       <c r="C194">
-        <v>0.82101773430000002</v>
+        <v>0.821017734</v>
       </c>
       <c r="E194" s="3">
         <f t="shared" si="2"/>
@@ -31821,7 +31912,7 @@
         <v>703</v>
       </c>
       <c r="C195">
-        <v>0.81686419750000006</v>
+        <v>0.81686419799999999</v>
       </c>
       <c r="E195" s="3">
         <f t="shared" si="2"/>
@@ -31836,7 +31927,7 @@
         <v>704</v>
       </c>
       <c r="C196">
-        <v>0.81269338710000005</v>
+        <v>0.81269338700000004</v>
       </c>
       <c r="E196" s="3">
         <f t="shared" si="2"/>
@@ -31851,7 +31942,7 @@
         <v>756</v>
       </c>
       <c r="C197">
-        <v>0.80814806650000004</v>
+        <v>0.80814806699999997</v>
       </c>
       <c r="E197" s="3">
         <f t="shared" si="2"/>
@@ -31866,7 +31957,7 @@
         <v>772</v>
       </c>
       <c r="C198">
-        <v>0.8035584536</v>
+        <v>0.80355845400000003</v>
       </c>
       <c r="E198" s="3">
         <f t="shared" si="2"/>
@@ -31881,7 +31972,7 @@
         <v>776</v>
       </c>
       <c r="C199">
-        <v>0.79892511879999994</v>
+        <v>0.79892511899999996</v>
       </c>
       <c r="E199" s="3">
         <f t="shared" si="2"/>
@@ -31896,7 +31987,7 @@
         <v>869</v>
       </c>
       <c r="C200">
-        <v>0.7941874699</v>
+        <v>0.79418747000000001</v>
       </c>
       <c r="E200" s="3">
         <f t="shared" si="2"/>
@@ -31911,7 +32002,7 @@
         <v>876</v>
       </c>
       <c r="C201">
-        <v>0.78944069179999998</v>
+        <v>0.789440692</v>
       </c>
       <c r="E201" s="3">
         <f t="shared" si="2"/>
@@ -31926,7 +32017,7 @@
         <v>923</v>
       </c>
       <c r="C202">
-        <v>0.78467348459999997</v>
+        <v>0.784673485</v>
       </c>
       <c r="E202" s="3">
         <f t="shared" si="2"/>
@@ -31956,7 +32047,7 @@
         <v>1007</v>
       </c>
       <c r="C204">
-        <v>0.77504419459999996</v>
+        <v>0.77504419499999999</v>
       </c>
       <c r="E204" s="3">
         <f t="shared" si="2"/>
@@ -31971,7 +32062,7 @@
         <v>1030</v>
       </c>
       <c r="C205">
-        <v>0.77020665290000001</v>
+        <v>0.77020665300000002</v>
       </c>
       <c r="E205" s="3">
         <f t="shared" si="2"/>
@@ -31986,7 +32077,7 @@
         <v>1045</v>
       </c>
       <c r="C206">
-        <v>0.76527930690000001</v>
+        <v>0.76527930700000002</v>
       </c>
       <c r="E206" s="3">
         <f t="shared" si="2"/>
@@ -32001,7 +32092,7 @@
         <v>1082</v>
       </c>
       <c r="C207">
-        <v>0.76001342640000003</v>
+        <v>0.76001342599999999</v>
       </c>
       <c r="E207" s="3">
         <f t="shared" si="2"/>
@@ -32031,7 +32122,7 @@
         <v>1147</v>
       </c>
       <c r="C209">
-        <v>0.74875934759999996</v>
+        <v>0.74875934799999999</v>
       </c>
       <c r="E209" s="3">
         <f t="shared" si="3"/>
@@ -32061,7 +32152,7 @@
         <v>1171</v>
       </c>
       <c r="C211">
-        <v>0.73711789029999997</v>
+        <v>0.73711789000000005</v>
       </c>
       <c r="E211" s="3">
         <f t="shared" si="3"/>
@@ -32076,7 +32167,7 @@
         <v>1186</v>
       </c>
       <c r="C212">
-        <v>0.73115367060000003</v>
+        <v>0.73115367099999995</v>
       </c>
       <c r="E212" s="3">
         <f t="shared" si="3"/>
@@ -32091,7 +32182,7 @@
         <v>1224</v>
       </c>
       <c r="C213">
-        <v>0.72519142640000001</v>
+        <v>0.72519142599999997</v>
       </c>
       <c r="E213" s="3">
         <f t="shared" si="3"/>
@@ -32106,7 +32197,7 @@
         <v>1225</v>
       </c>
       <c r="C214">
-        <v>0.71913837579999995</v>
+        <v>0.71913837599999997</v>
       </c>
       <c r="E214" s="3">
         <f t="shared" si="3"/>
@@ -32121,7 +32212,7 @@
         <v>1293</v>
       </c>
       <c r="C215">
-        <v>0.71301023249999995</v>
+        <v>0.71301023299999999</v>
       </c>
       <c r="E215" s="3">
         <f t="shared" si="3"/>
@@ -32136,7 +32227,7 @@
         <v>1445</v>
       </c>
       <c r="C216">
-        <v>0.70646509759999998</v>
+        <v>0.70646509800000001</v>
       </c>
       <c r="E216" s="3">
         <f t="shared" si="3"/>
@@ -32151,7 +32242,7 @@
         <v>1582</v>
       </c>
       <c r="C217">
-        <v>0.69910233519999998</v>
+        <v>0.69910233499999996</v>
       </c>
       <c r="E217" s="3">
         <f t="shared" si="3"/>
@@ -32166,7 +32257,7 @@
         <v>1588</v>
       </c>
       <c r="C218">
-        <v>0.69169601479999998</v>
+        <v>0.691696015</v>
       </c>
       <c r="E218" s="3">
         <f t="shared" si="3"/>
@@ -32181,7 +32272,7 @@
         <v>1662</v>
       </c>
       <c r="C219">
-        <v>0.68423449589999996</v>
+        <v>0.68423449599999997</v>
       </c>
       <c r="E219" s="3">
         <f t="shared" si="3"/>
@@ -32196,7 +32287,7 @@
         <v>1773</v>
       </c>
       <c r="C220">
-        <v>0.67663608259999997</v>
+        <v>0.676636083</v>
       </c>
       <c r="E220" s="3">
         <f t="shared" si="3"/>
@@ -32211,7 +32302,7 @@
         <v>1806</v>
       </c>
       <c r="C221">
-        <v>0.66859595449999998</v>
+        <v>0.66859595500000002</v>
       </c>
       <c r="E221" s="3">
         <f t="shared" si="3"/>
@@ -32226,7 +32317,7 @@
         <v>1826</v>
       </c>
       <c r="C222">
-        <v>0.66859595449999998</v>
+        <v>0.66859595500000002</v>
       </c>
       <c r="E222" s="3">
         <f t="shared" si="3"/>
@@ -32255,7 +32346,7 @@
         <v>1</v>
       </c>
       <c r="C224">
-        <v>0.99822328449999997</v>
+        <v>0.99822328500000002</v>
       </c>
       <c r="E224" s="3">
         <f t="shared" si="3"/>
@@ -32300,7 +32391,7 @@
         <v>6</v>
       </c>
       <c r="C227">
-        <v>0.9928608847</v>
+        <v>0.99286088500000003</v>
       </c>
       <c r="E227" s="3">
         <f t="shared" si="3"/>
@@ -32315,7 +32406,7 @@
         <v>8</v>
       </c>
       <c r="C228">
-        <v>0.99106883830000003</v>
+        <v>0.99106883800000001</v>
       </c>
       <c r="E228" s="3">
         <f t="shared" si="3"/>
@@ -32330,7 +32421,7 @@
         <v>10</v>
       </c>
       <c r="C229">
-        <v>0.98927371080000004</v>
+        <v>0.98927371099999994</v>
       </c>
       <c r="E229" s="3">
         <f t="shared" si="3"/>
@@ -32360,7 +32451,7 @@
         <v>12</v>
       </c>
       <c r="C231">
-        <v>0.98566890910000005</v>
+        <v>0.98566890900000004</v>
       </c>
       <c r="E231" s="3">
         <f t="shared" si="3"/>
@@ -32375,7 +32466,7 @@
         <v>14</v>
       </c>
       <c r="C232">
-        <v>0.98204815729999995</v>
+        <v>0.98204815700000003</v>
       </c>
       <c r="E232" s="3">
         <f t="shared" si="3"/>
@@ -32390,7 +32481,7 @@
         <v>17</v>
       </c>
       <c r="C233">
-        <v>0.97840048180000005</v>
+        <v>0.97840048199999996</v>
       </c>
       <c r="E233" s="3">
         <f t="shared" si="3"/>
@@ -32405,7 +32496,7 @@
         <v>18</v>
       </c>
       <c r="C234">
-        <v>0.97474568390000005</v>
+        <v>0.97474568399999995</v>
       </c>
       <c r="E234" s="3">
         <f t="shared" si="3"/>
@@ -32420,7 +32511,7 @@
         <v>19</v>
       </c>
       <c r="C235">
-        <v>0.96925919920000003</v>
+        <v>0.96925919900000002</v>
       </c>
       <c r="E235" s="3">
         <f t="shared" si="3"/>
@@ -32435,7 +32526,7 @@
         <v>21</v>
       </c>
       <c r="C236">
-        <v>0.96741790270000005</v>
+        <v>0.96741790299999997</v>
       </c>
       <c r="E236" s="3">
         <f t="shared" si="3"/>
@@ -32450,7 +32541,7 @@
         <v>24</v>
       </c>
       <c r="C237">
-        <v>0.96373202670000002</v>
+        <v>0.96373202700000005</v>
       </c>
       <c r="E237" s="3">
         <f t="shared" si="3"/>
@@ -32465,7 +32556,7 @@
         <v>26</v>
       </c>
       <c r="C238">
-        <v>0.96188435839999997</v>
+        <v>0.96188435800000005</v>
       </c>
       <c r="E238" s="3">
         <f t="shared" si="3"/>
@@ -32480,7 +32571,7 @@
         <v>31</v>
       </c>
       <c r="C239">
-        <v>0.96002263480000005</v>
+        <v>0.96002263499999996</v>
       </c>
       <c r="E239" s="3">
         <f t="shared" si="3"/>
@@ -32495,7 +32586,7 @@
         <v>32</v>
       </c>
       <c r="C240">
-        <v>0.95629910809999996</v>
+        <v>0.95629910799999995</v>
       </c>
       <c r="E240" s="3">
         <f t="shared" si="3"/>
@@ -32510,7 +32601,7 @@
         <v>34</v>
       </c>
       <c r="C241">
-        <v>0.95442967970000003</v>
+        <v>0.95442967999999995</v>
       </c>
       <c r="E241" s="3">
         <f t="shared" si="3"/>
@@ -32525,7 +32616,7 @@
         <v>43</v>
       </c>
       <c r="C242">
-        <v>0.95254054369999996</v>
+        <v>0.95254054399999999</v>
       </c>
       <c r="E242" s="3">
         <f t="shared" si="3"/>
@@ -32540,7 +32631,7 @@
         <v>45</v>
       </c>
       <c r="C243">
-        <v>0.95064929009999999</v>
+        <v>0.95064928999999998</v>
       </c>
       <c r="E243" s="3">
         <f t="shared" si="3"/>
@@ -32555,7 +32646,7 @@
         <v>46</v>
       </c>
       <c r="C244">
-        <v>0.94875756580000004</v>
+        <v>0.94875756600000005</v>
       </c>
       <c r="E244" s="3">
         <f t="shared" si="3"/>
@@ -32570,7 +32661,7 @@
         <v>49</v>
       </c>
       <c r="C245">
-        <v>0.94496553139999995</v>
+        <v>0.94496553100000003</v>
       </c>
       <c r="E245" s="3">
         <f t="shared" si="3"/>
@@ -32585,7 +32676,7 @@
         <v>55</v>
       </c>
       <c r="C246">
-        <v>0.94305899810000005</v>
+        <v>0.94305899800000004</v>
       </c>
       <c r="E246" s="3">
         <f t="shared" si="3"/>
@@ -32600,7 +32691,7 @@
         <v>61</v>
       </c>
       <c r="C247">
-        <v>0.94115235159999999</v>
+        <v>0.94115235200000003</v>
       </c>
       <c r="E247" s="3">
         <f t="shared" si="3"/>
@@ -32615,7 +32706,7 @@
         <v>62</v>
       </c>
       <c r="C248">
-        <v>0.93924318090000003</v>
+        <v>0.93924318100000004</v>
       </c>
       <c r="E248" s="3">
         <f t="shared" si="3"/>
@@ -32630,7 +32721,7 @@
         <v>84</v>
       </c>
       <c r="C249">
-        <v>0.93732315749999995</v>
+        <v>0.93732315799999999</v>
       </c>
       <c r="E249" s="3">
         <f t="shared" si="3"/>
@@ -32645,7 +32736,7 @@
         <v>90</v>
       </c>
       <c r="C250">
-        <v>0.93537604679999997</v>
+        <v>0.93537604699999999</v>
       </c>
       <c r="E250" s="3">
         <f t="shared" si="3"/>
@@ -32660,7 +32751,7 @@
         <v>102</v>
       </c>
       <c r="C251">
-        <v>0.93337817840000004</v>
+        <v>0.933378178</v>
       </c>
       <c r="E251" s="3">
         <f t="shared" si="3"/>
@@ -32675,7 +32766,7 @@
         <v>109</v>
       </c>
       <c r="C252">
-        <v>0.93137676550000004</v>
+        <v>0.93137676599999997</v>
       </c>
       <c r="E252" s="3">
         <f t="shared" si="3"/>
@@ -32690,7 +32781,7 @@
         <v>118</v>
       </c>
       <c r="C253">
-        <v>0.92936628290000001</v>
+        <v>0.92936628300000002</v>
       </c>
       <c r="E253" s="3">
         <f t="shared" si="3"/>
@@ -32705,7 +32796,7 @@
         <v>127</v>
       </c>
       <c r="C254">
-        <v>0.92735618040000001</v>
+        <v>0.92735617999999997</v>
       </c>
       <c r="E254" s="3">
         <f t="shared" si="3"/>
@@ -32720,7 +32811,7 @@
         <v>132</v>
       </c>
       <c r="C255">
-        <v>0.92534422650000003</v>
+        <v>0.92534422699999996</v>
       </c>
       <c r="E255" s="3">
         <f t="shared" si="3"/>
@@ -32735,7 +32826,7 @@
         <v>149</v>
       </c>
       <c r="C256">
-        <v>0.92332069780000003</v>
+        <v>0.92332069800000005</v>
       </c>
       <c r="E256" s="3">
         <f t="shared" si="3"/>
@@ -32750,7 +32841,7 @@
         <v>163</v>
       </c>
       <c r="C257">
-        <v>0.92128873730000005</v>
+        <v>0.92128873700000002</v>
       </c>
       <c r="E257" s="3">
         <f t="shared" si="3"/>
@@ -32765,7 +32856,7 @@
         <v>166</v>
       </c>
       <c r="C258">
-        <v>0.9172157742</v>
+        <v>0.91721577399999998</v>
       </c>
       <c r="E258" s="3">
         <f t="shared" si="3"/>
@@ -32795,7 +32886,7 @@
         <v>177</v>
       </c>
       <c r="C260">
-        <v>0.91309391159999997</v>
+        <v>0.91309391200000001</v>
       </c>
       <c r="E260" s="3">
         <f t="shared" si="3"/>
@@ -32810,7 +32901,7 @@
         <v>180</v>
       </c>
       <c r="C261">
-        <v>0.91102387080000002</v>
+        <v>0.91102387100000004</v>
       </c>
       <c r="E261" s="3">
         <f t="shared" si="3"/>
@@ -32825,7 +32916,7 @@
         <v>182</v>
       </c>
       <c r="C262">
-        <v>0.90894871980000003</v>
+        <v>0.90894872000000004</v>
       </c>
       <c r="E262" s="3">
         <f t="shared" si="3"/>
@@ -32840,7 +32931,7 @@
         <v>185</v>
       </c>
       <c r="C263">
-        <v>0.90686712660000002</v>
+        <v>0.90686712700000005</v>
       </c>
       <c r="E263" s="3">
         <f t="shared" si="3"/>
@@ -32855,7 +32946,7 @@
         <v>189</v>
       </c>
       <c r="C264">
-        <v>0.90478227180000004</v>
+        <v>0.90478227200000005</v>
       </c>
       <c r="E264" s="3">
         <f t="shared" si="3"/>
@@ -32870,7 +32961,7 @@
         <v>191</v>
       </c>
       <c r="C265">
-        <v>0.90269619369999998</v>
+        <v>0.90269619400000001</v>
       </c>
       <c r="E265" s="3">
         <f t="shared" si="3"/>
@@ -32885,7 +32976,7 @@
         <v>227</v>
       </c>
       <c r="C266">
-        <v>0.90060766410000004</v>
+        <v>0.90060766400000003</v>
       </c>
       <c r="E266" s="3">
         <f t="shared" si="3"/>
@@ -32900,7 +32991,7 @@
         <v>231</v>
       </c>
       <c r="C267">
-        <v>0.89850252620000004</v>
+        <v>0.89850252600000002</v>
       </c>
       <c r="E267" s="3">
         <f t="shared" si="3"/>
@@ -32915,7 +33006,7 @@
         <v>252</v>
       </c>
       <c r="C268">
-        <v>0.89639285319999995</v>
+        <v>0.89639285300000004</v>
       </c>
       <c r="E268" s="3">
         <f t="shared" si="3"/>
@@ -32930,7 +33021,7 @@
         <v>256</v>
       </c>
       <c r="C269">
-        <v>0.89427591849999999</v>
+        <v>0.89427591900000003</v>
       </c>
       <c r="E269" s="3">
         <f t="shared" si="3"/>
@@ -32945,7 +33036,7 @@
         <v>271</v>
       </c>
       <c r="C270">
-        <v>0.89215725430000004</v>
+        <v>0.89215725400000001</v>
       </c>
       <c r="E270" s="3">
         <f t="shared" si="3"/>
@@ -32960,7 +33051,7 @@
         <v>300</v>
       </c>
       <c r="C271">
-        <v>0.89003385950000002</v>
+        <v>0.89003385999999995</v>
       </c>
       <c r="E271" s="3">
         <f t="shared" si="3"/>
@@ -32975,7 +33066,7 @@
         <v>301</v>
       </c>
       <c r="C272">
-        <v>0.88790398290000005</v>
+        <v>0.88790398299999995</v>
       </c>
       <c r="E272" s="3">
         <f t="shared" ref="E272:E335" si="4">E271+1</f>
@@ -32990,7 +33081,7 @@
         <v>316</v>
       </c>
       <c r="C273">
-        <v>0.88575710240000005</v>
+        <v>0.88575710200000002</v>
       </c>
       <c r="E273" s="3">
         <f t="shared" si="4"/>
@@ -33005,7 +33096,7 @@
         <v>349</v>
       </c>
       <c r="C274">
-        <v>0.88359839480000002</v>
+        <v>0.88359839500000004</v>
       </c>
       <c r="E274" s="3">
         <f t="shared" si="4"/>
@@ -33020,7 +33111,7 @@
         <v>373</v>
       </c>
       <c r="C275">
-        <v>0.8813143175</v>
+        <v>0.88131431800000004</v>
       </c>
       <c r="E275" s="3">
         <f t="shared" si="4"/>
@@ -33035,7 +33126,7 @@
         <v>375</v>
       </c>
       <c r="C276">
-        <v>0.87901920109999998</v>
+        <v>0.87901920099999997</v>
       </c>
       <c r="E276" s="3">
         <f t="shared" si="4"/>
@@ -33050,7 +33141,7 @@
         <v>421</v>
       </c>
       <c r="C277">
-        <v>0.87665212589999997</v>
+        <v>0.87665212599999998</v>
       </c>
       <c r="E277" s="3">
         <f t="shared" si="4"/>
@@ -33065,7 +33156,7 @@
         <v>444</v>
       </c>
       <c r="C278">
-        <v>0.87427690319999996</v>
+        <v>0.87427690300000005</v>
       </c>
       <c r="E278" s="3">
         <f t="shared" si="4"/>
@@ -33080,7 +33171,7 @@
         <v>463</v>
       </c>
       <c r="C279">
-        <v>0.87190112210000004</v>
+        <v>0.87190112200000003</v>
       </c>
       <c r="E279" s="3">
         <f t="shared" si="4"/>
@@ -33095,7 +33186,7 @@
         <v>465</v>
       </c>
       <c r="C280">
-        <v>0.8695009575</v>
+        <v>0.86950095800000005</v>
       </c>
       <c r="E280" s="3">
         <f t="shared" si="4"/>
@@ -33110,7 +33201,7 @@
         <v>471</v>
       </c>
       <c r="C281">
-        <v>0.86707915680000003</v>
+        <v>0.86707915700000004</v>
       </c>
       <c r="E281" s="3">
         <f t="shared" si="4"/>
@@ -33125,7 +33216,7 @@
         <v>490</v>
       </c>
       <c r="C282">
-        <v>0.86464920359999997</v>
+        <v>0.864649204</v>
       </c>
       <c r="E282" s="3">
         <f t="shared" si="4"/>
@@ -33140,7 +33231,7 @@
         <v>492</v>
       </c>
       <c r="C283">
-        <v>0.86221332669999995</v>
+        <v>0.86221332699999997</v>
       </c>
       <c r="E283" s="3">
         <f t="shared" si="4"/>
@@ -33155,7 +33246,7 @@
         <v>528</v>
       </c>
       <c r="C284">
-        <v>0.85977017320000004</v>
+        <v>0.85977017300000003</v>
       </c>
       <c r="E284" s="3">
         <f t="shared" si="4"/>
@@ -33170,7 +33261,7 @@
         <v>534</v>
       </c>
       <c r="C285">
-        <v>0.8573142748</v>
+        <v>0.85731427500000001</v>
       </c>
       <c r="E285" s="3">
         <f t="shared" si="4"/>
@@ -33215,7 +33306,7 @@
         <v>969</v>
       </c>
       <c r="C288">
-        <v>0.84867178070000004</v>
+        <v>0.84867178099999996</v>
       </c>
       <c r="E288" s="3">
         <f t="shared" si="4"/>
@@ -33230,7 +33321,7 @@
         <v>999</v>
       </c>
       <c r="C289">
-        <v>0.84547471640000005</v>
+        <v>0.84547471600000002</v>
       </c>
       <c r="E289" s="3">
         <f t="shared" si="4"/>
@@ -33245,7 +33336,7 @@
         <v>1032</v>
       </c>
       <c r="C290">
-        <v>0.84216958850000001</v>
+        <v>0.84216958900000005</v>
       </c>
       <c r="E290" s="3">
         <f t="shared" si="4"/>
@@ -33260,7 +33351,7 @@
         <v>1038</v>
       </c>
       <c r="C291">
-        <v>0.8388198617</v>
+        <v>0.83881986200000003</v>
       </c>
       <c r="E291" s="3">
         <f t="shared" si="4"/>
@@ -33275,7 +33366,7 @@
         <v>1049</v>
       </c>
       <c r="C292">
-        <v>0.83544807430000001</v>
+        <v>0.83544807399999998</v>
       </c>
       <c r="E292" s="3">
         <f t="shared" si="4"/>
@@ -33290,7 +33381,7 @@
         <v>1066</v>
       </c>
       <c r="C293">
-        <v>0.83204344149999998</v>
+        <v>0.83204344200000002</v>
       </c>
       <c r="E293" s="3">
         <f t="shared" si="4"/>
@@ -33305,7 +33396,7 @@
         <v>1087</v>
       </c>
       <c r="C294">
-        <v>0.82861138020000003</v>
+        <v>0.82861138000000001</v>
       </c>
       <c r="E294" s="3">
         <f t="shared" si="4"/>
@@ -33320,7 +33411,7 @@
         <v>1090</v>
       </c>
       <c r="C295">
-        <v>0.82514730960000005</v>
+        <v>0.82514730999999997</v>
       </c>
       <c r="E295" s="3">
         <f t="shared" si="4"/>
@@ -33335,7 +33426,7 @@
         <v>1100</v>
       </c>
       <c r="C296">
-        <v>0.82167182719999998</v>
+        <v>0.82167182699999997</v>
       </c>
       <c r="E296" s="3">
         <f t="shared" si="4"/>
@@ -33350,7 +33441,7 @@
         <v>1107</v>
       </c>
       <c r="C297">
-        <v>0.81814095249999996</v>
+        <v>0.818140953</v>
       </c>
       <c r="E297" s="3">
         <f t="shared" si="4"/>
@@ -33365,7 +33456,7 @@
         <v>1117</v>
       </c>
       <c r="C298">
-        <v>0.81458832069999998</v>
+        <v>0.814588321</v>
       </c>
       <c r="E298" s="3">
         <f t="shared" si="4"/>
@@ -33380,7 +33471,7 @@
         <v>1191</v>
       </c>
       <c r="C299">
-        <v>0.81090810120000001</v>
+        <v>0.81090810099999999</v>
       </c>
       <c r="E299" s="3">
         <f t="shared" si="4"/>
@@ -33425,7 +33516,7 @@
         <v>1440</v>
       </c>
       <c r="C302">
-        <v>0.79942335129999997</v>
+        <v>0.79942335099999995</v>
       </c>
       <c r="E302" s="3">
         <f t="shared" si="4"/>
@@ -33440,7 +33531,7 @@
         <v>1571</v>
       </c>
       <c r="C303">
-        <v>0.79521596530000005</v>
+        <v>0.79521596500000002</v>
       </c>
       <c r="E303" s="3">
         <f t="shared" si="4"/>
@@ -33455,7 +33546,7 @@
         <v>1606</v>
       </c>
       <c r="C304">
-        <v>0.79099583029999998</v>
+        <v>0.79099582999999996</v>
       </c>
       <c r="E304" s="3">
         <f t="shared" si="4"/>
@@ -33470,7 +33561,7 @@
         <v>1618</v>
       </c>
       <c r="C305">
-        <v>0.78676793779999998</v>
+        <v>0.786767938</v>
       </c>
       <c r="E305" s="3">
         <f t="shared" si="4"/>
@@ -33485,7 +33576,7 @@
         <v>1678</v>
       </c>
       <c r="C306">
-        <v>0.78253370460000005</v>
+        <v>0.78253370499999997</v>
       </c>
       <c r="E306" s="3">
         <f t="shared" si="4"/>
@@ -33500,7 +33591,7 @@
         <v>1700</v>
       </c>
       <c r="C307">
-        <v>0.7782642582</v>
+        <v>0.77826425799999999</v>
       </c>
       <c r="E307" s="3">
         <f t="shared" si="4"/>
@@ -33515,7 +33606,7 @@
         <v>1796</v>
       </c>
       <c r="C308">
-        <v>0.77378174690000001</v>
+        <v>0.77378174700000002</v>
       </c>
       <c r="E308" s="3">
         <f t="shared" si="4"/>
@@ -33530,7 +33621,7 @@
         <v>1807</v>
       </c>
       <c r="C309">
-        <v>0.76928884220000004</v>
+        <v>0.76928884200000003</v>
       </c>
       <c r="E309" s="3">
         <f t="shared" si="4"/>
@@ -33545,7 +33636,7 @@
         <v>1808</v>
       </c>
       <c r="C310">
-        <v>0.76472526620000003</v>
+        <v>0.76472526600000001</v>
       </c>
       <c r="E310" s="3">
         <f t="shared" si="4"/>
@@ -33560,7 +33651,7 @@
         <v>1826</v>
       </c>
       <c r="C311">
-        <v>0.76472526620000003</v>
+        <v>0.76472526600000001</v>
       </c>
       <c r="E311" s="3">
         <f t="shared" si="4"/>
@@ -33589,7 +33680,7 @@
         <v>0</v>
       </c>
       <c r="C313">
-        <v>0.99022890070000003</v>
+        <v>0.99022890100000005</v>
       </c>
       <c r="E313" s="3">
         <f t="shared" si="4"/>
@@ -33604,7 +33695,7 @@
         <v>3</v>
       </c>
       <c r="C314">
-        <v>0.98773943109999995</v>
+        <v>0.98773943099999995</v>
       </c>
       <c r="E314" s="3">
         <f t="shared" si="4"/>
@@ -33619,7 +33710,7 @@
         <v>6</v>
       </c>
       <c r="C315">
-        <v>0.98524048190000002</v>
+        <v>0.98524048200000003</v>
       </c>
       <c r="E315" s="3">
         <f t="shared" si="4"/>
@@ -33634,7 +33725,7 @@
         <v>12</v>
       </c>
       <c r="C316">
-        <v>0.98273183490000005</v>
+        <v>0.98273183500000005</v>
       </c>
       <c r="E316" s="3">
         <f t="shared" si="4"/>
@@ -33649,7 +33740,7 @@
         <v>16</v>
       </c>
       <c r="C317">
-        <v>0.97771445450000005</v>
+        <v>0.97771445499999998</v>
       </c>
       <c r="E317" s="3">
         <f t="shared" si="4"/>
@@ -33664,7 +33755,7 @@
         <v>19</v>
       </c>
       <c r="C318">
-        <v>0.97519127549999995</v>
+        <v>0.975191276</v>
       </c>
       <c r="E318" s="3">
         <f t="shared" si="4"/>
@@ -33679,7 +33770,7 @@
         <v>25</v>
       </c>
       <c r="C319">
-        <v>0.97266268280000001</v>
+        <v>0.97266268300000003</v>
       </c>
       <c r="E319" s="3">
         <f t="shared" si="4"/>
@@ -33694,7 +33785,7 @@
         <v>33</v>
       </c>
       <c r="C320">
-        <v>0.97013074450000003</v>
+        <v>0.97013074499999996</v>
       </c>
       <c r="E320" s="3">
         <f t="shared" si="4"/>
@@ -33709,7 +33800,7 @@
         <v>47</v>
       </c>
       <c r="C321">
-        <v>0.96759424429999996</v>
+        <v>0.96759424400000005</v>
       </c>
       <c r="E321" s="3">
         <f t="shared" si="4"/>
@@ -33724,7 +33815,7 @@
         <v>48</v>
       </c>
       <c r="C322">
-        <v>0.96504996340000004</v>
+        <v>0.96504996300000001</v>
       </c>
       <c r="E322" s="3">
         <f t="shared" si="4"/>
@@ -33739,7 +33830,7 @@
         <v>66</v>
       </c>
       <c r="C323">
-        <v>0.96249545830000005</v>
+        <v>0.96249545800000003</v>
       </c>
       <c r="E323" s="3">
         <f t="shared" si="4"/>
@@ -33754,7 +33845,7 @@
         <v>81</v>
       </c>
       <c r="C324">
-        <v>0.95993792909999998</v>
+        <v>0.95993792899999997</v>
       </c>
       <c r="E324" s="3">
         <f t="shared" si="4"/>
@@ -33769,7 +33860,7 @@
         <v>82</v>
       </c>
       <c r="C325">
-        <v>0.95736761420000005</v>
+        <v>0.95736761400000003</v>
       </c>
       <c r="E325" s="3">
         <f t="shared" si="4"/>
@@ -33784,7 +33875,7 @@
         <v>87</v>
       </c>
       <c r="C326">
-        <v>0.95479496890000004</v>
+        <v>0.95479496900000005</v>
       </c>
       <c r="E326" s="3">
         <f t="shared" si="4"/>
@@ -33799,7 +33890,7 @@
         <v>91</v>
       </c>
       <c r="C327">
-        <v>0.95222055839999997</v>
+        <v>0.95222055800000005</v>
       </c>
       <c r="E327" s="3">
         <f t="shared" si="4"/>
@@ -33814,7 +33905,7 @@
         <v>94</v>
       </c>
       <c r="C328">
-        <v>0.94963708690000004</v>
+        <v>0.94963708700000005</v>
       </c>
       <c r="E328" s="3">
         <f t="shared" si="4"/>
@@ -33829,7 +33920,7 @@
         <v>95</v>
       </c>
       <c r="C329">
-        <v>0.94704827270000003</v>
+        <v>0.94704827300000005</v>
       </c>
       <c r="E329" s="3">
         <f t="shared" si="4"/>
@@ -33844,7 +33935,7 @@
         <v>99</v>
       </c>
       <c r="C330">
-        <v>0.94186336130000003</v>
+        <v>0.94186336100000001</v>
       </c>
       <c r="E330" s="3">
         <f t="shared" si="4"/>
@@ -33859,7 +33950,7 @@
         <v>104</v>
       </c>
       <c r="C331">
-        <v>0.93924749829999998</v>
+        <v>0.93924749799999996</v>
       </c>
       <c r="E331" s="3">
         <f t="shared" si="4"/>
@@ -33889,7 +33980,7 @@
         <v>128</v>
       </c>
       <c r="C333">
-        <v>0.93399187439999998</v>
+        <v>0.93399187400000006</v>
       </c>
       <c r="E333" s="3">
         <f t="shared" si="4"/>
@@ -33919,7 +34010,7 @@
         <v>140</v>
       </c>
       <c r="C335">
-        <v>0.92869571149999997</v>
+        <v>0.92869571200000001</v>
       </c>
       <c r="E335" s="3">
         <f t="shared" si="4"/>
@@ -33934,7 +34025,7 @@
         <v>145</v>
       </c>
       <c r="C336">
-        <v>0.92603334289999994</v>
+        <v>0.92603334299999995</v>
       </c>
       <c r="E336" s="3">
         <f t="shared" ref="E336:E399" si="5">E335+1</f>
@@ -33964,7 +34055,7 @@
         <v>184</v>
       </c>
       <c r="C338">
-        <v>0.92069476729999999</v>
+        <v>0.92069476699999997</v>
       </c>
       <c r="E338" s="3">
         <f t="shared" si="5"/>
@@ -33979,7 +34070,7 @@
         <v>189</v>
       </c>
       <c r="C339">
-        <v>0.91802462659999995</v>
+        <v>0.91802462699999998</v>
       </c>
       <c r="E339" s="3">
         <f t="shared" si="5"/>
@@ -33994,7 +34085,7 @@
         <v>196</v>
       </c>
       <c r="C340">
-        <v>0.9153488783</v>
+        <v>0.91534887799999998</v>
       </c>
       <c r="E340" s="3">
         <f t="shared" si="5"/>
@@ -34009,7 +34100,7 @@
         <v>198</v>
       </c>
       <c r="C341">
-        <v>0.91265288119999999</v>
+        <v>0.91265288099999997</v>
       </c>
       <c r="E341" s="3">
         <f t="shared" si="5"/>
@@ -34024,7 +34115,7 @@
         <v>208</v>
       </c>
       <c r="C342">
-        <v>0.90995381269999998</v>
+        <v>0.909953813</v>
       </c>
       <c r="E342" s="3">
         <f t="shared" si="5"/>
@@ -34039,7 +34130,7 @@
         <v>238</v>
       </c>
       <c r="C343">
-        <v>0.9072503864</v>
+        <v>0.90725038599999996</v>
       </c>
       <c r="E343" s="3">
         <f t="shared" si="5"/>
@@ -34054,7 +34145,7 @@
         <v>240</v>
       </c>
       <c r="C344">
-        <v>0.90453807909999995</v>
+        <v>0.90453807900000005</v>
       </c>
       <c r="E344" s="3">
         <f t="shared" si="5"/>
@@ -34069,7 +34160,7 @@
         <v>244</v>
       </c>
       <c r="C345">
-        <v>0.90181552539999998</v>
+        <v>0.90181552499999995</v>
       </c>
       <c r="E345" s="3">
         <f t="shared" si="5"/>
@@ -34084,7 +34175,7 @@
         <v>256</v>
       </c>
       <c r="C346">
-        <v>0.89909226760000005</v>
+        <v>0.89909226799999997</v>
       </c>
       <c r="E346" s="3">
         <f t="shared" si="5"/>
@@ -34099,7 +34190,7 @@
         <v>268</v>
       </c>
       <c r="C347">
-        <v>0.89635411789999997</v>
+        <v>0.89635411799999998</v>
       </c>
       <c r="E347" s="3">
         <f t="shared" si="5"/>
@@ -34129,7 +34220,7 @@
         <v>323</v>
       </c>
       <c r="C349">
-        <v>0.89086674320000003</v>
+        <v>0.89086674300000002</v>
       </c>
       <c r="E349" s="3">
         <f t="shared" si="5"/>
@@ -34144,7 +34235,7 @@
         <v>324</v>
       </c>
       <c r="C350">
-        <v>0.88810333379999995</v>
+        <v>0.88810333399999997</v>
       </c>
       <c r="E350" s="3">
         <f t="shared" si="5"/>
@@ -34159,7 +34250,7 @@
         <v>343</v>
       </c>
       <c r="C351">
-        <v>0.88531409809999995</v>
+        <v>0.88531409800000005</v>
       </c>
       <c r="E351" s="3">
         <f t="shared" si="5"/>
@@ -34174,7 +34265,7 @@
         <v>349</v>
       </c>
       <c r="C352">
-        <v>0.88252656029999998</v>
+        <v>0.88252655999999996</v>
       </c>
       <c r="E352" s="3">
         <f t="shared" si="5"/>
@@ -34189,7 +34280,7 @@
         <v>350</v>
       </c>
       <c r="C353">
-        <v>0.87694961370000002</v>
+        <v>0.87694961400000004</v>
       </c>
       <c r="E353" s="3">
         <f t="shared" si="5"/>
@@ -34204,7 +34295,7 @@
         <v>373</v>
       </c>
       <c r="C354">
-        <v>0.87412092360000004</v>
+        <v>0.87412092399999997</v>
       </c>
       <c r="E354" s="3">
         <f t="shared" si="5"/>
@@ -34219,7 +34310,7 @@
         <v>385</v>
       </c>
       <c r="C355">
-        <v>0.87123842070000002</v>
+        <v>0.87123842100000004</v>
       </c>
       <c r="E355" s="3">
         <f t="shared" si="5"/>
@@ -34234,7 +34325,7 @@
         <v>448</v>
       </c>
       <c r="C356">
-        <v>0.86831415980000004</v>
+        <v>0.86831415999999995</v>
       </c>
       <c r="E356" s="3">
         <f t="shared" si="5"/>
@@ -34249,7 +34340,7 @@
         <v>458</v>
       </c>
       <c r="C357">
-        <v>0.86538318359999999</v>
+        <v>0.86538318400000003</v>
       </c>
       <c r="E357" s="3">
         <f t="shared" si="5"/>
@@ -34264,7 +34355,7 @@
         <v>473</v>
       </c>
       <c r="C358">
-        <v>0.86244597840000004</v>
+        <v>0.862445978</v>
       </c>
       <c r="E358" s="3">
         <f t="shared" si="5"/>
@@ -34294,7 +34385,7 @@
         <v>482</v>
       </c>
       <c r="C360">
-        <v>0.85651108679999999</v>
+        <v>0.856511087</v>
       </c>
       <c r="E360" s="3">
         <f t="shared" si="5"/>
@@ -34309,7 +34400,7 @@
         <v>487</v>
       </c>
       <c r="C361">
-        <v>0.85352748310000004</v>
+        <v>0.85352748300000003</v>
       </c>
       <c r="E361" s="3">
         <f t="shared" si="5"/>
@@ -34324,7 +34415,7 @@
         <v>491</v>
       </c>
       <c r="C362">
-        <v>0.85054011910000005</v>
+        <v>0.85054011900000004</v>
       </c>
       <c r="E362" s="3">
         <f t="shared" si="5"/>
@@ -34339,7 +34430,7 @@
         <v>507</v>
       </c>
       <c r="C363">
-        <v>0.84755215539999995</v>
+        <v>0.84755215500000003</v>
       </c>
       <c r="E363" s="3">
         <f t="shared" si="5"/>
@@ -34354,7 +34445,7 @@
         <v>524</v>
       </c>
       <c r="C364">
-        <v>0.84155982979999999</v>
+        <v>0.84155983000000001</v>
       </c>
       <c r="E364" s="3">
         <f t="shared" si="5"/>
@@ -34369,7 +34460,7 @@
         <v>535</v>
       </c>
       <c r="C365">
-        <v>0.83853677140000005</v>
+        <v>0.83853677100000001</v>
       </c>
       <c r="E365" s="3">
         <f t="shared" si="5"/>
@@ -34384,7 +34475,7 @@
         <v>543</v>
       </c>
       <c r="C366">
-        <v>0.83550792460000001</v>
+        <v>0.83550792500000004</v>
       </c>
       <c r="E366" s="3">
         <f t="shared" si="5"/>
@@ -34399,7 +34490,7 @@
         <v>579</v>
       </c>
       <c r="C367">
-        <v>0.83246744039999998</v>
+        <v>0.83246743999999995</v>
       </c>
       <c r="E367" s="3">
         <f t="shared" si="5"/>
@@ -34414,7 +34505,7 @@
         <v>603</v>
       </c>
       <c r="C368">
-        <v>0.82942695619999995</v>
+        <v>0.82942695600000005</v>
       </c>
       <c r="E368" s="3">
         <f t="shared" si="5"/>
@@ -34429,7 +34520,7 @@
         <v>613</v>
       </c>
       <c r="C369">
-        <v>0.82637887050000003</v>
+        <v>0.82637887099999996</v>
       </c>
       <c r="E369" s="3">
         <f t="shared" si="5"/>
@@ -34444,7 +34535,7 @@
         <v>621</v>
       </c>
       <c r="C370">
-        <v>0.82330777420000001</v>
+        <v>0.82330777399999999</v>
       </c>
       <c r="E370" s="3">
         <f t="shared" si="5"/>
@@ -34459,7 +34550,7 @@
         <v>654</v>
       </c>
       <c r="C371">
-        <v>0.82020171980000001</v>
+        <v>0.82020172000000002</v>
       </c>
       <c r="E371" s="3">
         <f t="shared" si="5"/>
@@ -34489,7 +34580,7 @@
         <v>685</v>
       </c>
       <c r="C373">
-        <v>0.81388394070000003</v>
+        <v>0.81388394100000006</v>
       </c>
       <c r="E373" s="3">
         <f t="shared" si="5"/>
@@ -34504,7 +34595,7 @@
         <v>721</v>
       </c>
       <c r="C374">
-        <v>0.80731364790000004</v>
+        <v>0.80731364800000005</v>
       </c>
       <c r="E374" s="3">
         <f t="shared" si="5"/>
@@ -34519,7 +34610,7 @@
         <v>789</v>
       </c>
       <c r="C375">
-        <v>0.80385707679999996</v>
+        <v>0.80385707699999998</v>
       </c>
       <c r="E375" s="3">
         <f t="shared" si="5"/>
@@ -34534,7 +34625,7 @@
         <v>821</v>
       </c>
       <c r="C376">
-        <v>0.80033978130000005</v>
+        <v>0.80033978100000003</v>
       </c>
       <c r="E376" s="3">
         <f t="shared" si="5"/>
@@ -34549,7 +34640,7 @@
         <v>849</v>
       </c>
       <c r="C377">
-        <v>0.79678670709999999</v>
+        <v>0.79678670699999998</v>
       </c>
       <c r="E377" s="3">
         <f t="shared" si="5"/>
@@ -34564,7 +34655,7 @@
         <v>859</v>
       </c>
       <c r="C378">
-        <v>0.79322726870000004</v>
+        <v>0.79322726899999996</v>
       </c>
       <c r="E378" s="3">
         <f t="shared" si="5"/>
@@ -34594,7 +34685,7 @@
         <v>880</v>
       </c>
       <c r="C380">
-        <v>0.78602025939999998</v>
+        <v>0.78602025900000005</v>
       </c>
       <c r="E380" s="3">
         <f t="shared" si="5"/>
@@ -34609,7 +34700,7 @@
         <v>899</v>
       </c>
       <c r="C381">
-        <v>0.78238555939999999</v>
+        <v>0.78238555899999995</v>
       </c>
       <c r="E381" s="3">
         <f t="shared" si="5"/>
@@ -34624,7 +34715,7 @@
         <v>923</v>
       </c>
       <c r="C382">
-        <v>0.77871336729999996</v>
+        <v>0.77871336700000005</v>
       </c>
       <c r="E382" s="3">
         <f t="shared" si="5"/>
@@ -34639,7 +34730,7 @@
         <v>944</v>
       </c>
       <c r="C383">
-        <v>0.77503139359999995</v>
+        <v>0.77503139399999998</v>
       </c>
       <c r="E383" s="3">
         <f t="shared" si="5"/>
@@ -34654,7 +34745,7 @@
         <v>1027</v>
       </c>
       <c r="C384">
-        <v>0.77132617660000002</v>
+        <v>0.77132617699999995</v>
       </c>
       <c r="E384" s="3">
         <f t="shared" si="5"/>
@@ -34669,7 +34760,7 @@
         <v>1126</v>
       </c>
       <c r="C385">
-        <v>0.76702642470000004</v>
+        <v>0.76702642499999996</v>
       </c>
       <c r="E385" s="3">
         <f t="shared" si="5"/>
@@ -34684,7 +34775,7 @@
         <v>1127</v>
       </c>
       <c r="C386">
-        <v>0.76270204190000002</v>
+        <v>0.76270204200000002</v>
       </c>
       <c r="E386" s="3">
         <f t="shared" si="5"/>
@@ -34699,7 +34790,7 @@
         <v>1289</v>
       </c>
       <c r="C387">
-        <v>0.75830302979999997</v>
+        <v>0.75830302999999999</v>
       </c>
       <c r="E387" s="3">
         <f t="shared" si="5"/>
@@ -34714,7 +34805,7 @@
         <v>1335</v>
       </c>
       <c r="C388">
-        <v>0.75385839939999999</v>
+        <v>0.75385839899999996</v>
       </c>
       <c r="E388" s="3">
         <f t="shared" si="5"/>
@@ -34729,7 +34820,7 @@
         <v>1353</v>
       </c>
       <c r="C389">
-        <v>0.74939363520000002</v>
+        <v>0.749393635</v>
       </c>
       <c r="E389" s="3">
         <f t="shared" si="5"/>
@@ -34744,7 +34835,7 @@
         <v>1361</v>
       </c>
       <c r="C390">
-        <v>0.74489552370000001</v>
+        <v>0.74489552400000003</v>
       </c>
       <c r="E390" s="3">
         <f t="shared" si="5"/>
@@ -34759,7 +34850,7 @@
         <v>1408</v>
       </c>
       <c r="C391">
-        <v>0.74036438459999998</v>
+        <v>0.74036438500000001</v>
       </c>
       <c r="E391" s="3">
         <f t="shared" si="5"/>
@@ -34789,7 +34880,7 @@
         <v>1468</v>
       </c>
       <c r="C393">
-        <v>0.73066556920000003</v>
+        <v>0.73066556900000001</v>
       </c>
       <c r="E393" s="3">
         <f t="shared" si="5"/>
@@ -34804,7 +34895,7 @@
         <v>1512</v>
       </c>
       <c r="C394">
-        <v>0.72516744119999998</v>
+        <v>0.72516744099999997</v>
       </c>
       <c r="E394" s="3">
         <f t="shared" si="5"/>
@@ -34834,7 +34925,7 @@
         <v>1562</v>
       </c>
       <c r="C396">
-        <v>0.71308995350000004</v>
+        <v>0.71308995399999997</v>
       </c>
       <c r="E396" s="3">
         <f t="shared" si="5"/>
@@ -34849,7 +34940,7 @@
         <v>1624</v>
       </c>
       <c r="C397">
-        <v>0.70700655290000003</v>
+        <v>0.70700655300000004</v>
       </c>
       <c r="E397" s="3">
         <f t="shared" si="5"/>
@@ -34864,7 +34955,7 @@
         <v>1790</v>
       </c>
       <c r="C398">
-        <v>0.70066076509999997</v>
+        <v>0.70066076499999996</v>
       </c>
       <c r="E398" s="3">
         <f t="shared" si="5"/>
@@ -34879,7 +34970,7 @@
         <v>1815</v>
       </c>
       <c r="C399">
-        <v>0.69415153549999997</v>
+        <v>0.69415153600000001</v>
       </c>
       <c r="E399" s="3">
         <f t="shared" si="5"/>
@@ -34894,7 +34985,7 @@
         <v>1826</v>
       </c>
       <c r="C400">
-        <v>0.69415153549999997</v>
+        <v>0.69415153600000001</v>
       </c>
       <c r="E400" s="3">
         <f t="shared" ref="E400" si="6">E399+1</f>

</xml_diff>

<commit_message>
remved debug. recoloured tool buttons. kidney info
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10576EC-27B0-0C48-B1F8-C7CC5523D6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564E18CF-B98F-FF4D-AF27-F9DB9141A590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10820" yWindow="1360" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="11980" yWindow="2560" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -753,9 +753,6 @@
  :content "Forced vital capacity.  A measure of lung function."}</t>
   </si>
   <si>
-    <t>Has the patient ever had any thoracotomy procedures?</t>
-  </si>
-  <si>
     <t>{:title "BMI – Body Mass Index"
 :content [:&lt;&gt;
 [:p "Weight (in kg) divided by height (in metres) squared"]
@@ -780,6 +777,10 @@
 [:p "Has the donor ever had the common virus Cytomegalovirus?"]
 [:p "If  the donor is positive for CMV it means the recipient will receive some medication after transplant."]
 ]}</t>
+  </si>
+  <si>
+    <t>{:title "Previous thoractotim?"
+:content "Has the patient ever had any thoracotomy procedures?"}</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -1537,7 +1538,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="399" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>69</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>123</v>
       </c>
       <c r="H2" s="47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I2" s="40">
         <v>100</v>
@@ -1995,7 +1996,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>178</v>
       </c>
@@ -2015,7 +2016,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>178</v>
       </c>
@@ -2036,7 +2037,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>178</v>
       </c>
@@ -2057,7 +2058,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>178</v>
       </c>
@@ -2078,7 +2079,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="26"/>
@@ -2089,7 +2090,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>74</v>
       </c>
@@ -2109,7 +2110,7 @@
         <v>123</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
@@ -2212,7 +2213,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="1:12" ht="166" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" ht="166" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
@@ -2416,7 +2417,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="8"/>
     </row>
-    <row r="43" spans="1:12" ht="106" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" ht="106" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>75</v>
       </c>
@@ -2436,7 +2437,7 @@
         <v>123</v>
       </c>
       <c r="H43" s="47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I43" s="40">
         <v>60</v>
@@ -27798,8 +27799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -28309,7 +28310,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="65"/>
     </row>
-    <row r="22" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="8" customFormat="1" ht="196" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>59</v>
       </c>
@@ -28332,8 +28333,8 @@
         <v>25</v>
       </c>
       <c r="H22" s="3"/>
-      <c r="I22" s="3" t="s">
-        <v>233</v>
+      <c r="I22" s="47" t="s">
+        <v>237</v>
       </c>
       <c r="J22" s="39">
         <v>100</v>
@@ -28786,7 +28787,7 @@
         <v>126</v>
       </c>
       <c r="I41" s="69" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J41" s="39">
         <v>90</v>

</xml_diff>

<commit_message>
corrected info-box, added lung-banner
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564E18CF-B98F-FF4D-AF27-F9DB9141A590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADEEA54-5643-014A-ACAC-8BECC8D43E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="2560" windowWidth="34320" windowHeight="21040" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="11980" yWindow="2560" windowWidth="34320" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -739,16 +739,6 @@
     <t>Donor/Recipient TLC mismatch</t>
   </si>
   <si>
-    <t xml:space="preserve">{:title "NYHA CLASS – New York Heart Association Classification"
-:content [:&lt;&gt;
-[:p "Class I – for example shortness of breath when walking or climbing stairs"]
-[:p "Class II – for example mild shortness of breath that limits ordinary activities"]
-[:p "Class III – only comfortable at rest, limited in doing normal activities such as walking short distances (20m – 100m)"
-[:p "Class IV – symptoms even at rest, usually bedbound patients."]
-]}
-</t>
-  </si>
-  <si>
     <t>{:title "FVC - Forced Vital Capacity" 
  :content "Forced vital capacity.  A measure of lung function."}</t>
   </si>
@@ -782,6 +772,16 @@
     <t>{:title "Previous thoractotim?"
 :content "Has the patient ever had any thoracotomy procedures?"}</t>
   </si>
+  <si>
+    <t xml:space="preserve">{:title "NYHA CLASS – New York Heart Association Classification"
+:content [:&lt;&gt;
+[:p "Class I – for example shortness of breath when walking or climbing stairs"]
+[:p "Class II – for example mild shortness of breath that limits ordinary activities"]
+[:p "Class III – only comfortable at rest, limited in doing normal activities such as walking short distances (20m – 100m)"]
+[:p "Class IV – symptoms even at rest, usually bedbound patients."]
+]}
+</t>
+  </si>
 </sst>
 </file>
 
@@ -791,7 +791,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -849,12 +849,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
-      <name val="Symbol"/>
-      <charset val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -907,7 +901,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1065,26 +1059,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1481,7 +1472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -1558,7 +1549,7 @@
         <v>123</v>
       </c>
       <c r="H2" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I2" s="40">
         <v>100</v>
@@ -1735,7 +1726,7 @@
       <c r="B10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="68" t="s">
         <v>223</v>
       </c>
       <c r="D10" s="14">
@@ -1761,7 +1752,7 @@
       <c r="B11" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="64"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="17" t="s">
         <v>226</v>
       </c>
@@ -2110,7 +2101,7 @@
         <v>123</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
@@ -2236,7 +2227,7 @@
         <v>125</v>
       </c>
       <c r="H33" s="47" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I33" s="40">
         <v>40</v>
@@ -2437,7 +2428,7 @@
         <v>123</v>
       </c>
       <c r="H43" s="47" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="I43" s="40">
         <v>60</v>
@@ -27799,21 +27790,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="38" style="3" customWidth="1"/>
-    <col min="3" max="3" width="42.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.83203125" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" style="32" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="3" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="62.83203125" style="3" customWidth="1"/>
     <col min="10" max="10" width="10.5" style="39" customWidth="1"/>
     <col min="11" max="12" width="11.5" style="32" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="3"/>
@@ -27921,7 +27912,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -27949,7 +27940,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>58</v>
       </c>
@@ -27975,7 +27966,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>58</v>
       </c>
@@ -28001,7 +27992,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>58</v>
       </c>
@@ -28027,7 +28018,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="16"/>
@@ -28037,14 +28028,14 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" ht="10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="67" t="s">
         <v>223</v>
       </c>
       <c r="D10" s="48">
@@ -28065,14 +28056,14 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="63"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="50" t="s">
         <v>224</v>
       </c>
@@ -28091,7 +28082,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>51</v>
       </c>
@@ -28117,7 +28108,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="16"/>
@@ -28128,7 +28119,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>52</v>
       </c>
@@ -28156,7 +28147,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>52</v>
       </c>
@@ -28182,7 +28173,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="18"/>
@@ -28215,8 +28206,8 @@
         <v>25</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="I17" s="66" t="s">
-        <v>231</v>
+      <c r="I17" s="47" t="s">
+        <v>237</v>
       </c>
       <c r="J17" s="39">
         <v>60</v>
@@ -28243,7 +28234,7 @@
         <v>25</v>
       </c>
       <c r="H18" s="10"/>
-      <c r="I18" s="67"/>
+      <c r="I18" s="64"/>
       <c r="J18" s="39">
         <v>60</v>
       </c>
@@ -28269,7 +28260,7 @@
         <v>25</v>
       </c>
       <c r="H19" s="10"/>
-      <c r="I19" s="65"/>
+      <c r="I19" s="63"/>
       <c r="J19" s="39">
         <v>60</v>
       </c>
@@ -28295,7 +28286,7 @@
         <v>25</v>
       </c>
       <c r="H20" s="10"/>
-      <c r="I20" s="65"/>
+      <c r="I20" s="63"/>
       <c r="J20" s="39">
         <v>60</v>
       </c>
@@ -28308,7 +28299,7 @@
       <c r="E21"/>
       <c r="F21"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="65"/>
+      <c r="I21" s="63"/>
     </row>
     <row r="22" spans="1:13" s="8" customFormat="1" ht="196" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
@@ -28334,7 +28325,7 @@
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J22" s="39">
         <v>100</v>
@@ -28665,8 +28656,8 @@
       <c r="H36" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="I36" s="68" t="s">
-        <v>232</v>
+      <c r="I36" s="65" t="s">
+        <v>231</v>
       </c>
       <c r="J36" s="39">
         <v>80</v>
@@ -28786,8 +28777,8 @@
       <c r="H41" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="I41" s="69" t="s">
-        <v>233</v>
+      <c r="I41" s="66" t="s">
+        <v>232</v>
       </c>
       <c r="J41" s="39">
         <v>90</v>
@@ -29209,7 +29200,7 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="64"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -29225,7 +29216,7 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="64"/>
+      <c r="F13" s="68"/>
     </row>
     <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
harmonising names with R - pre dd-pred to pred
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADEEA54-5643-014A-ACAC-8BECC8D43E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C5A329-4B64-6244-BE81-6AF2BB60EA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="2560" windowWidth="34320" windowHeight="21040" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="32000" windowHeight="24000" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2257" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="305">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -782,6 +782,207 @@
 ]}
 </t>
   </si>
+  <si>
+    <t>:r-name</t>
+  </si>
+  <si>
+    <t>sex_1</t>
+  </si>
+  <si>
+    <t>sex_2</t>
+  </si>
+  <si>
+    <t>dis_cf</t>
+  </si>
+  <si>
+    <t>dis_oth</t>
+  </si>
+  <si>
+    <t>dis_pf</t>
+  </si>
+  <si>
+    <t>dis_copd</t>
+  </si>
+  <si>
+    <t>pred_0</t>
+  </si>
+  <si>
+    <t>pred_1_14</t>
+  </si>
+  <si>
+    <t>pred_15</t>
+  </si>
+  <si>
+    <t>in_hosp_1</t>
+  </si>
+  <si>
+    <t>in_hosp_2</t>
+  </si>
+  <si>
+    <t>nyha_1</t>
+  </si>
+  <si>
+    <t>nyha_2</t>
+  </si>
+  <si>
+    <t>nyha_3</t>
+  </si>
+  <si>
+    <t>nyha_4</t>
+  </si>
+  <si>
+    <t>prev_thor_1</t>
+  </si>
+  <si>
+    <t>prev_thor_2</t>
+  </si>
+  <si>
+    <t>bld_1</t>
+  </si>
+  <si>
+    <t>bld_2</t>
+  </si>
+  <si>
+    <t>bld_3</t>
+  </si>
+  <si>
+    <t>bld_4</t>
+  </si>
+  <si>
+    <t>rage_1</t>
+  </si>
+  <si>
+    <t>rage_2</t>
+  </si>
+  <si>
+    <t>rage_3</t>
+  </si>
+  <si>
+    <t>rage_4</t>
+  </si>
+  <si>
+    <t>rage_5</t>
+  </si>
+  <si>
+    <t>fvc_1</t>
+  </si>
+  <si>
+    <t>fvc_2</t>
+  </si>
+  <si>
+    <t>fvc_3</t>
+  </si>
+  <si>
+    <t>fvc_4</t>
+  </si>
+  <si>
+    <t>bmi_1</t>
+  </si>
+  <si>
+    <t>bmi_2</t>
+  </si>
+  <si>
+    <t>bmi_3</t>
+  </si>
+  <si>
+    <t>dcmv_1</t>
+  </si>
+  <si>
+    <t>dcmv_2</t>
+  </si>
+  <si>
+    <t>dsmoke_1</t>
+  </si>
+  <si>
+    <t>dsmoke_2</t>
+  </si>
+  <si>
+    <t>pred_grp_1</t>
+  </si>
+  <si>
+    <t>pred_grp_2</t>
+  </si>
+  <si>
+    <t>pred_grp_3</t>
+  </si>
+  <si>
+    <t>tx_type_1</t>
+  </si>
+  <si>
+    <t>tx_type_2</t>
+  </si>
+  <si>
+    <t>dis_grp_cf</t>
+  </si>
+  <si>
+    <t>dis_grp_oth</t>
+  </si>
+  <si>
+    <t>dis_grp_pf</t>
+  </si>
+  <si>
+    <t>dis_grp_copd</t>
+  </si>
+  <si>
+    <t>rage_grp_1</t>
+  </si>
+  <si>
+    <t>rage_grp_2</t>
+  </si>
+  <si>
+    <t>rage_grp_3</t>
+  </si>
+  <si>
+    <t>rage_grp_4</t>
+  </si>
+  <si>
+    <t>rage_grp_5</t>
+  </si>
+  <si>
+    <t>tlc_mis_1</t>
+  </si>
+  <si>
+    <t>tlc_mis_2</t>
+  </si>
+  <si>
+    <t>tlc_mis_3</t>
+  </si>
+  <si>
+    <t>fvc_grp_1</t>
+  </si>
+  <si>
+    <t>fvc_grp_2</t>
+  </si>
+  <si>
+    <t>fvc_grp_3</t>
+  </si>
+  <si>
+    <t>fvc_grp_4</t>
+  </si>
+  <si>
+    <t>bili_grp_1</t>
+  </si>
+  <si>
+    <t>bili_grp_2</t>
+  </si>
+  <si>
+    <t>bili_grp_3</t>
+  </si>
+  <si>
+    <t>bili_grp_4</t>
+  </si>
+  <si>
+    <t>chol_grp_1</t>
+  </si>
+  <si>
+    <t>chol_grp_2</t>
+  </si>
+  <si>
+    <t>chol_grp_3</t>
+  </si>
+  <si>
+    <t>chol_grp_4</t>
+  </si>
 </sst>
 </file>
 
@@ -901,7 +1102,7 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1077,6 +1278,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1470,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1483,15 +1685,16 @@
     <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
-    <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
-    <col min="10" max="11" width="15" style="32" customWidth="1"/>
-    <col min="12" max="12" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="3"/>
+    <col min="6" max="6" width="17.83203125" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="34.5" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="10.5" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="15" style="32" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="32" customWidth="1"/>
+    <col min="13" max="13" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -1525,11 +1728,14 @@
       <c r="K1" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>69</v>
       </c>
@@ -1560,9 +1766,12 @@
       <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>69</v>
       </c>
@@ -1585,9 +1794,12 @@
       <c r="K3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L3" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>69</v>
       </c>
@@ -1609,9 +1821,10 @@
       <c r="K4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L4" s="3"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="26"/>
@@ -1620,9 +1833,10 @@
       <c r="I5" s="40"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="3"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>72</v>
       </c>
@@ -1650,11 +1864,14 @@
       <c r="K6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>72</v>
       </c>
@@ -1677,11 +1894,14 @@
       <c r="K7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>72</v>
       </c>
@@ -1704,11 +1924,12 @@
       <c r="K8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L8" s="8" t="s">
+      <c r="L8" s="3"/>
+      <c r="M8" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="26"/>
@@ -1717,9 +1938,10 @@
       <c r="I9" s="40"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L9" s="3"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>51</v>
       </c>
@@ -1743,9 +1965,12 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L10" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>51</v>
       </c>
@@ -1764,9 +1989,12 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L11" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>51</v>
       </c>
@@ -1785,9 +2013,12 @@
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L12" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="26"/>
@@ -1796,9 +2027,10 @@
       <c r="I13" s="40"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L13" s="3"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
@@ -1822,9 +2054,12 @@
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L14" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>19</v>
       </c>
@@ -1843,9 +2078,12 @@
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L15" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="26"/>
@@ -1854,9 +2092,10 @@
       <c r="I16" s="40"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L16" s="3"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>58</v>
       </c>
@@ -1880,9 +2119,12 @@
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L17" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>58</v>
       </c>
@@ -1901,9 +2143,12 @@
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L18" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>58</v>
       </c>
@@ -1922,9 +2167,12 @@
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L19" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>58</v>
       </c>
@@ -1943,9 +2191,12 @@
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L20" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="M20" s="8"/>
+    </row>
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="26"/>
@@ -1954,9 +2205,10 @@
       <c r="I21" s="40"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L21" s="3"/>
+      <c r="M21" s="8"/>
+    </row>
+    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="12" t="s">
         <v>178</v>
       </c>
@@ -1983,11 +2235,14 @@
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="8" t="s">
+      <c r="L22" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="M22" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="10" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>178</v>
       </c>
@@ -2005,9 +2260,12 @@
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L23" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
         <v>178</v>
       </c>
@@ -2026,9 +2284,12 @@
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="M24" s="8"/>
+    </row>
+    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>178</v>
       </c>
@@ -2047,9 +2308,12 @@
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L25" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="M25" s="8"/>
+    </row>
+    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>178</v>
       </c>
@@ -2068,9 +2332,12 @@
       </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L26" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="M26" s="8"/>
+    </row>
+    <row r="27" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="26"/>
@@ -2079,9 +2346,10 @@
       <c r="I27" s="40"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" ht="1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L27" s="3"/>
+      <c r="M27" s="8"/>
+    </row>
+    <row r="28" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>74</v>
       </c>
@@ -2112,9 +2380,12 @@
       <c r="K28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L28" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
         <v>74</v>
       </c>
@@ -2138,9 +2409,12 @@
       <c r="K29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L29" s="8"/>
-    </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L29" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>74</v>
       </c>
@@ -2164,9 +2438,12 @@
       <c r="K30" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L30" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>74</v>
       </c>
@@ -2190,9 +2467,10 @@
       <c r="K31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L31" s="3"/>
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="26"/>
@@ -2202,9 +2480,10 @@
       <c r="I32" s="40"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" ht="166" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L32" s="3"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="1:13" ht="166" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>46</v>
       </c>
@@ -2234,9 +2513,12 @@
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="8"/>
-    </row>
-    <row r="34" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L33" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="M33" s="8"/>
+    </row>
+    <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>46</v>
       </c>
@@ -2254,9 +2536,12 @@
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="8"/>
-    </row>
-    <row r="35" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L34" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="M34" s="8"/>
+    </row>
+    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
         <v>46</v>
       </c>
@@ -2274,9 +2559,12 @@
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L35" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="M35" s="8"/>
+    </row>
+    <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>46</v>
       </c>
@@ -2294,18 +2582,22 @@
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L36" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="M36" s="8"/>
+    </row>
+    <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="E37"/>
       <c r="I37" s="40"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L37" s="3"/>
+      <c r="M37" s="8"/>
+    </row>
+    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>60</v>
       </c>
@@ -2329,9 +2621,12 @@
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="8"/>
-    </row>
-    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L38" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="M38" s="8"/>
+    </row>
+    <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>60</v>
       </c>
@@ -2351,9 +2646,12 @@
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L39" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="M39" s="8"/>
+    </row>
+    <row r="40" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
         <v>60</v>
       </c>
@@ -2373,9 +2671,12 @@
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="8"/>
-    </row>
-    <row r="41" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L40" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="M40" s="8"/>
+    </row>
+    <row r="41" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
@@ -2395,9 +2696,12 @@
       </c>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="8"/>
-    </row>
-    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L41" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="M41" s="8"/>
+    </row>
+    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="26"/>
@@ -2406,9 +2710,10 @@
       <c r="I42" s="40"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
-      <c r="L42" s="8"/>
-    </row>
-    <row r="43" spans="1:12" ht="106" hidden="1" x14ac:dyDescent="0.2">
+      <c r="L42" s="3"/>
+      <c r="M42" s="8"/>
+    </row>
+    <row r="43" spans="1:13" ht="106" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>75</v>
       </c>
@@ -2437,9 +2742,12 @@
         <v>151</v>
       </c>
       <c r="K43" s="3"/>
-      <c r="L43" s="8"/>
-    </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L43" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="M43" s="8"/>
+    </row>
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
         <v>75</v>
       </c>
@@ -2460,9 +2768,12 @@
         <v>151</v>
       </c>
       <c r="K44" s="3"/>
-      <c r="L44" s="8"/>
-    </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L44" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="M44" s="8"/>
+    </row>
+    <row r="45" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
         <v>75</v>
       </c>
@@ -2484,9 +2795,12 @@
         <v>151</v>
       </c>
       <c r="K45" s="3"/>
-      <c r="L45" s="8"/>
-    </row>
-    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="L45" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="M45" s="8"/>
+    </row>
+    <row r="46" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="12" t="s">
         <v>75</v>
       </c>
@@ -2508,11 +2822,14 @@
         <v>151</v>
       </c>
       <c r="K46" s="3"/>
-      <c r="L46" s="8" t="s">
+      <c r="L46" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="M46" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A47" s="12" t="s">
         <v>75</v>
       </c>
@@ -2533,71 +2850,73 @@
         <v>151</v>
       </c>
       <c r="K47" s="3"/>
-      <c r="L47" s="8"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="L47" s="3"/>
+      <c r="M47" s="8"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="E48" s="30"/>
       <c r="I48" s="40"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
-      <c r="L48" s="8"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="L48" s="3"/>
+      <c r="M48" s="8"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="E49" s="30"/>
       <c r="I49" s="40"/>
-      <c r="L49" s="8"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M49" s="8"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="E50" s="30"/>
       <c r="I50" s="40"/>
-      <c r="L50" s="8"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M50" s="8"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="E51" s="30"/>
       <c r="I51" s="40"/>
-      <c r="L51" s="8"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M51" s="8"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="E52" s="30"/>
       <c r="I52" s="40"/>
-      <c r="L52" s="8"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M52" s="8"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="E53" s="30"/>
       <c r="I53" s="40"/>
-      <c r="L53" s="8"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="M53" s="8"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E55" s="10"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E59" s="27"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E60" s="10"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E61" s="10"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E62" s="10"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E63" s="27"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
       <c r="E64" s="10"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.15">
@@ -27788,10 +28107,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -27802,15 +28121,16 @@
     <col min="4" max="4" width="22.33203125" style="32" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="62.83203125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="39" customWidth="1"/>
-    <col min="11" max="12" width="11.5" style="32" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="3"/>
+    <col min="7" max="7" width="18.83203125" style="3" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="3" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="62.83203125" style="3" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="39" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="11.5" style="32" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="32" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
         <v>15</v>
       </c>
@@ -27847,8 +28167,11 @@
       <c r="L1" s="11" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M1" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -27875,8 +28198,11 @@
       <c r="J2" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M2" s="32" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>8</v>
       </c>
@@ -27901,8 +28227,11 @@
       <c r="J3" s="39">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M3" s="32" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="16"/>
@@ -27912,7 +28241,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:12" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>58</v>
       </c>
@@ -27939,8 +28268,11 @@
       <c r="J5" s="39">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="32" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>58</v>
       </c>
@@ -27965,8 +28297,11 @@
       <c r="J6" s="39">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M6" s="32" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
         <v>58</v>
       </c>
@@ -27991,8 +28326,11 @@
       <c r="J7" s="39">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
         <v>58</v>
       </c>
@@ -28017,8 +28355,11 @@
       <c r="J8" s="39">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M8" s="32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="16"/>
@@ -28028,7 +28369,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:12" ht="10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
         <v>51</v>
       </c>
@@ -28055,8 +28396,11 @@
       <c r="J10" s="39">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="16" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="32" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="12" t="s">
         <v>51</v>
       </c>
@@ -28081,8 +28425,11 @@
       <c r="J11" s="39">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M11" s="69" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
         <v>51</v>
       </c>
@@ -28107,8 +28454,11 @@
       <c r="J12" s="39">
         <v>70</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M12" s="32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
       <c r="C13" s="16"/>
@@ -28119,7 +28469,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>52</v>
       </c>
@@ -28146,8 +28496,11 @@
       <c r="J14" s="39">
         <v>50</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M14" s="69" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
         <v>52</v>
       </c>
@@ -28172,8 +28525,11 @@
       <c r="J15" s="39">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="M15" s="69" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="18"/>
@@ -28183,7 +28539,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="166" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>54</v>
       </c>
@@ -28212,8 +28568,11 @@
       <c r="J17" s="39">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M17" s="32" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
         <v>54</v>
       </c>
@@ -28238,8 +28597,11 @@
       <c r="J18" s="39">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M18" s="32" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>54</v>
       </c>
@@ -28264,8 +28626,11 @@
       <c r="J19" s="39">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M19" s="32" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>54</v>
       </c>
@@ -28290,8 +28655,11 @@
       <c r="J20" s="39">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M20" s="32" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="16"/>
@@ -28301,7 +28669,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="63"/>
     </row>
-    <row r="22" spans="1:13" s="8" customFormat="1" ht="196" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="8" customFormat="1" ht="31" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
         <v>59</v>
       </c>
@@ -28332,9 +28700,12 @@
       </c>
       <c r="K22" s="32"/>
       <c r="L22" s="32"/>
-      <c r="M22" s="3"/>
-    </row>
-    <row r="23" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M22" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="1:14" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
         <v>59</v>
       </c>
@@ -28361,9 +28732,12 @@
       </c>
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M23" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="16"/>
@@ -28373,7 +28747,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
         <v>12</v>
       </c>
@@ -28398,8 +28772,11 @@
       <c r="J25" s="39">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M25" s="32" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
         <v>12</v>
       </c>
@@ -28422,8 +28799,11 @@
       <c r="J26" s="39">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M26" s="32" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>12</v>
       </c>
@@ -28446,8 +28826,11 @@
       <c r="J27" s="39">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M27" s="32" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>12</v>
       </c>
@@ -28470,8 +28853,11 @@
       <c r="J28" s="39">
         <v>30</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M28" s="32" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="23"/>
       <c r="B29" s="12"/>
       <c r="C29" s="16"/>
@@ -28479,7 +28865,7 @@
       <c r="E29"/>
       <c r="F29"/>
     </row>
-    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="12" t="s">
         <v>185</v>
       </c>
@@ -28508,8 +28894,11 @@
       <c r="J30" s="62">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+      <c r="M30" s="32" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="12" t="s">
         <v>185</v>
       </c>
@@ -28534,8 +28923,11 @@
       <c r="J31" s="62">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M31" s="32" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
         <v>185</v>
       </c>
@@ -28562,8 +28954,11 @@
       </c>
       <c r="K32" s="32"/>
       <c r="L32" s="32"/>
-    </row>
-    <row r="33" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M32" s="32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>185</v>
       </c>
@@ -28590,8 +28985,11 @@
       </c>
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
-    </row>
-    <row r="34" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M33" s="32" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>185</v>
       </c>
@@ -28616,8 +29014,11 @@
       <c r="J34" s="62"/>
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
-    </row>
-    <row r="35" spans="1:12" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M34" s="32" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="58"/>
@@ -28630,8 +29031,9 @@
       <c r="J35" s="62"/>
       <c r="K35" s="32"/>
       <c r="L35" s="32"/>
-    </row>
-    <row r="36" spans="1:12" ht="187" x14ac:dyDescent="0.2">
+      <c r="M35" s="32"/>
+    </row>
+    <row r="36" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>46</v>
       </c>
@@ -28662,8 +29064,11 @@
       <c r="J36" s="39">
         <v>80</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M36" s="32" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="12" t="s">
         <v>46</v>
       </c>
@@ -28688,8 +29093,11 @@
       <c r="J37" s="39">
         <v>80</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M37" s="32" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>46</v>
       </c>
@@ -28714,8 +29122,11 @@
       <c r="J38" s="39">
         <v>80</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M38" s="32" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
         <v>46</v>
       </c>
@@ -28740,8 +29151,11 @@
       <c r="J39" s="39">
         <v>80</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="M39" s="32" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="45"/>
@@ -28752,7 +29166,7 @@
       <c r="I40" s="34"/>
       <c r="J40" s="44"/>
     </row>
-    <row r="41" spans="1:12" ht="343" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="91" x14ac:dyDescent="0.2">
       <c r="A41" s="12" t="s">
         <v>55</v>
       </c>
@@ -28783,8 +29197,11 @@
       <c r="J41" s="39">
         <v>90</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M41" s="32" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="12" t="s">
         <v>55</v>
       </c>
@@ -28806,8 +29223,11 @@
       <c r="J42" s="39">
         <v>90</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M42" s="32" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>55</v>
       </c>
@@ -28829,20 +29249,23 @@
       <c r="J43" s="39">
         <v>90</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M43" s="32" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B44"/>
     </row>
-    <row r="45" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="20"/>
     </row>
-    <row r="46" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B47"/>
     </row>
-    <row r="48" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="B48"/>
     </row>
     <row r="49" spans="2:2" ht="16" x14ac:dyDescent="0.2">
@@ -28916,6 +29339,11 @@
     <mergeCell ref="C10:C11"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="M15" r:id="rId1" display="in@hosp_2" xr:uid="{77894A4B-BAC5-FB44-B49C-B0661D49A04E}"/>
+    <hyperlink ref="M14" r:id="rId2" display="in@hosp_1" xr:uid="{A5715F6A-F9B0-E64C-A09D-555586FC24C5}"/>
+    <hyperlink ref="M11" r:id="rId3" display="pred_1@14" xr:uid="{438275D5-2949-3540-933B-6D2304E114A1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Included more Leila popup texts
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C5A329-4B64-6244-BE81-6AF2BB60EA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81507167-9A72-9141-B62C-331AD7EA8216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="0" windowWidth="32000" windowHeight="24000" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="6780" yWindow="1500" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Average donor values by centre" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="307">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -754,14 +755,6 @@
 :content "total cholesterol"}</t>
   </si>
   <si>
-    <t>{:title "Donor / Recipient TLC mismatch"
-:content 
-[:p "Donor to recipient calculated total lung capacity mismatch"]
-[:p "Total Lung Capacity is the volume (measured in litres) that the lungs can hold."]
-[:p "TLC mismatch means the difference in lung capacity between the donor and the recipient."]
-[:p "This figure is usually calculated when the characteristics of the donor is known."]}</t>
-  </si>
-  <si>
     <t>{:title "CMV - Cytomegalovirus"
 :content [:&lt;&gt;
 [:p "Has the donor ever had the common virus Cytomegalovirus?"]
@@ -982,6 +975,36 @@
   </si>
   <si>
     <t>chol_grp_4</t>
+  </si>
+  <si>
+    <t>{:title "Disease Group"
+:content 
+[:p  [:b "Cystic Fibrosis (CF):"] " either ‘Cystic Fibrosis’ or ‘Bronchitectasis"]
+[:p [:b "Pulmonary fibrosis (PF):"] " 'Fibrosing Lung Disease'"]
+[:p [:b "Chronic obstructive pulmonary disease (COPD):"] " either ‘alpha-1-antitrypsin deficiency’ or ‘emphysema’"]
+[:p [:b "Other: "] " Patients registered on to the lung waiting list with Primary Disease not listed under any of the above categories." ]}</t>
+  </si>
+  <si>
+    <t>{:title "Disease Group"
+:content [:&lt;&gt;
+[:p  [:b "Cystic Fibrosis (CF):"] " either ‘Cystic Fibrosis’ or ‘Bronchitectasis"]
+[:p [:b "Pulmonary fibrosis (PF):"] " 'Fibrosing Lung Disease'"]
+[:p [:b "Chronic obstructive pulmonary disease (COPD):"] " either ‘alpha-1-antitrypsin deficiency’ or ‘emphysema’"]
+[:p [:b "Other: "] " Patients registered on to the lung waiting list with Primary Disease not listed under any of the above categories." ]]}</t>
+  </si>
+  <si>
+    <t>{:title "Donor / Recipient TLC mismatch"
+:content  [:&lt;&gt;
+[:p "Donor to recipient calculated Total Lung Capacity mismatch"]
+[:p "Total Lung Capacity is the volume (measured in litres) that the lungs can hold."]
+[:p "TLC mismatch means the difference in lung capacity between the donor and the recipient."]
+[:p "This figure is usually calculated when the characteristics of the donor are known."]
+[:p "Mismatch = recipient calculated TLC – donor calculated TLC"]
+[:p "where calculated TLC is:"]
+[:div {:style {:margin-left "20px"}} 
+ [:p "If male, TLC = 7.99*(height(cm)/100) - 7.08"]
+ [:p "If female, TLC = 6.6*(height(cm)/100) - 5.79"]
+]]}</t>
   </si>
 </sst>
 </file>
@@ -1272,13 +1295,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1674,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E17" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1685,11 +1708,10 @@
     <col min="3" max="3" width="47.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="3" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="34.5" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="10.5" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="15" style="32" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="15" style="32" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.5" style="3" customWidth="1"/>
+    <col min="8" max="9" width="10.5" style="3" customWidth="1"/>
+    <col min="10" max="12" width="15" style="32" customWidth="1"/>
     <col min="13" max="13" width="28.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.83203125" style="3"/>
   </cols>
@@ -1729,7 +1751,7 @@
         <v>206</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M1" s="9" t="s">
         <v>22</v>
@@ -1755,7 +1777,7 @@
         <v>123</v>
       </c>
       <c r="H2" s="47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I2" s="40">
         <v>100</v>
@@ -1767,7 +1789,7 @@
         <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M2" s="8"/>
     </row>
@@ -1795,7 +1817,7 @@
         <v>10</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M3" s="8"/>
     </row>
@@ -1865,7 +1887,7 @@
         <v>10</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>76</v>
@@ -1895,7 +1917,7 @@
         <v>10</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>78</v>
@@ -1948,7 +1970,7 @@
       <c r="B10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="69" t="s">
         <v>223</v>
       </c>
       <c r="D10" s="14">
@@ -1966,7 +1988,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M10" s="8"/>
     </row>
@@ -1977,7 +1999,7 @@
       <c r="B11" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="17" t="s">
         <v>226</v>
       </c>
@@ -1990,7 +2012,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M11" s="8"/>
     </row>
@@ -2014,7 +2036,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M12" s="8"/>
     </row>
@@ -2055,7 +2077,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M14" s="8"/>
     </row>
@@ -2079,7 +2101,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M15" s="8"/>
     </row>
@@ -2114,13 +2136,16 @@
       <c r="F17" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="H17" s="47" t="s">
+        <v>305</v>
+      </c>
       <c r="I17" s="40">
         <v>20</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M17" s="8"/>
     </row>
@@ -2144,7 +2169,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M18" s="8"/>
     </row>
@@ -2168,7 +2193,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M19" s="8"/>
     </row>
@@ -2192,7 +2217,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M20" s="8"/>
     </row>
@@ -2236,7 +2261,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="M22" s="8" t="s">
         <v>79</v>
@@ -2261,7 +2286,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M23" s="8"/>
     </row>
@@ -2285,7 +2310,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M24" s="8"/>
     </row>
@@ -2309,7 +2334,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M25" s="8"/>
     </row>
@@ -2333,7 +2358,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="M26" s="8"/>
     </row>
@@ -2369,7 +2394,7 @@
         <v>123</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>234</v>
+        <v>306</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
@@ -2381,7 +2406,7 @@
         <v>10</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M28" s="8"/>
     </row>
@@ -2410,7 +2435,7 @@
         <v>10</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M29" s="8"/>
     </row>
@@ -2439,7 +2464,7 @@
         <v>10</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M30" s="8"/>
     </row>
@@ -2514,7 +2539,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M33" s="8"/>
     </row>
@@ -2537,7 +2562,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M34" s="8"/>
     </row>
@@ -2560,7 +2585,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="M35" s="8"/>
     </row>
@@ -2583,7 +2608,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M36" s="8"/>
     </row>
@@ -2622,7 +2647,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="M38" s="8"/>
     </row>
@@ -2647,7 +2672,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M39" s="8"/>
     </row>
@@ -2672,7 +2697,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M40" s="8"/>
     </row>
@@ -2697,7 +2722,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M41" s="8"/>
     </row>
@@ -2743,7 +2768,7 @@
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M43" s="8"/>
     </row>
@@ -2769,7 +2794,7 @@
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M44" s="8"/>
     </row>
@@ -2796,7 +2821,7 @@
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M45" s="8"/>
     </row>
@@ -2823,7 +2848,7 @@
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>77</v>
@@ -28109,8 +28134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -28121,12 +28146,11 @@
     <col min="4" max="4" width="22.33203125" style="32" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="3" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="62.83203125" style="3" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="39" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="11.5" style="32" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="32" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="3" customWidth="1"/>
+    <col min="9" max="9" width="62.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="39" customWidth="1"/>
+    <col min="11" max="13" width="11.5" style="32" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
@@ -28168,7 +28192,7 @@
         <v>206</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28199,7 +28223,7 @@
         <v>20</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28228,7 +28252,7 @@
         <v>20</v>
       </c>
       <c r="M3" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28269,10 +28293,10 @@
         <v>40</v>
       </c>
       <c r="M5" s="32" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>58</v>
       </c>
@@ -28293,12 +28317,14 @@
         <v>123</v>
       </c>
       <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="I6" s="66" t="s">
+        <v>304</v>
+      </c>
       <c r="J6" s="39">
         <v>40</v>
       </c>
       <c r="M6" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28327,7 +28353,7 @@
         <v>40</v>
       </c>
       <c r="M7" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28356,7 +28382,7 @@
         <v>40</v>
       </c>
       <c r="M8" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28376,7 +28402,7 @@
       <c r="B10" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C10" s="67" t="s">
+      <c r="C10" s="68" t="s">
         <v>223</v>
       </c>
       <c r="D10" s="48">
@@ -28397,7 +28423,7 @@
         <v>70</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28407,7 +28433,7 @@
       <c r="B11" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="67"/>
+      <c r="C11" s="68"/>
       <c r="D11" s="50" t="s">
         <v>224</v>
       </c>
@@ -28425,8 +28451,8 @@
       <c r="J11" s="39">
         <v>70</v>
       </c>
-      <c r="M11" s="69" t="s">
-        <v>246</v>
+      <c r="M11" s="67" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28455,7 +28481,7 @@
         <v>70</v>
       </c>
       <c r="M12" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28496,8 +28522,8 @@
       <c r="J14" s="39">
         <v>50</v>
       </c>
-      <c r="M14" s="69" t="s">
-        <v>248</v>
+      <c r="M14" s="67" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28525,8 +28551,8 @@
       <c r="J15" s="39">
         <v>50</v>
       </c>
-      <c r="M15" s="69" t="s">
-        <v>249</v>
+      <c r="M15" s="67" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28563,13 +28589,13 @@
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="47" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J17" s="39">
         <v>60</v>
       </c>
       <c r="M17" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28598,7 +28624,7 @@
         <v>60</v>
       </c>
       <c r="M18" s="32" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28627,7 +28653,7 @@
         <v>60</v>
       </c>
       <c r="M19" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28656,7 +28682,7 @@
         <v>60</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28693,7 +28719,7 @@
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J22" s="39">
         <v>100</v>
@@ -28701,7 +28727,7 @@
       <c r="K22" s="32"/>
       <c r="L22" s="32"/>
       <c r="M22" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N22" s="3"/>
     </row>
@@ -28733,7 +28759,7 @@
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
       <c r="M23" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N23" s="3"/>
     </row>
@@ -28773,7 +28799,7 @@
         <v>30</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28800,7 +28826,7 @@
         <v>30</v>
       </c>
       <c r="M26" s="32" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28827,7 +28853,7 @@
         <v>30</v>
       </c>
       <c r="M27" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28854,7 +28880,7 @@
         <v>30</v>
       </c>
       <c r="M28" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28895,7 +28921,7 @@
         <v>10</v>
       </c>
       <c r="M30" s="32" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28924,7 +28950,7 @@
         <v>10</v>
       </c>
       <c r="M31" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -28955,7 +28981,7 @@
       <c r="K32" s="32"/>
       <c r="L32" s="32"/>
       <c r="M32" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -28986,7 +29012,7 @@
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
       <c r="M33" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -29015,7 +29041,7 @@
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
       <c r="M34" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -29065,7 +29091,7 @@
         <v>80</v>
       </c>
       <c r="M36" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29094,7 +29120,7 @@
         <v>80</v>
       </c>
       <c r="M37" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29123,7 +29149,7 @@
         <v>80</v>
       </c>
       <c r="M38" s="32" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29152,7 +29178,7 @@
         <v>80</v>
       </c>
       <c r="M39" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -29198,7 +29224,7 @@
         <v>90</v>
       </c>
       <c r="M41" s="32" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29224,7 +29250,7 @@
         <v>90</v>
       </c>
       <c r="M42" s="32" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29250,7 +29276,7 @@
         <v>90</v>
       </c>
       <c r="M43" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29628,7 +29654,7 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="68"/>
+      <c r="F12" s="69"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -29644,7 +29670,7 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="68"/>
+      <c r="F13" s="69"/>
     </row>
     <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
to lung: (less cache updates) disease group info
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42D63C5-FF2C-F945-9D2B-A8F1DB68C56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3F32E1-31AD-444A-8C8C-E24779CDE929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1500" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="6780" yWindow="1500" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -1293,13 +1293,13 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1696,7 +1696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -1970,7 +1970,7 @@
       <c r="B10" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="69" t="s">
+      <c r="C10" s="70" t="s">
         <v>222</v>
       </c>
       <c r="D10" s="14">
@@ -1999,7 +1999,7 @@
       <c r="B11" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="69"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="17" t="s">
         <v>225</v>
       </c>
@@ -2508,7 +2508,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="8"/>
     </row>
-    <row r="33" spans="1:13" ht="166" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="46" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
         <v>45</v>
       </c>
@@ -2738,7 +2738,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="8"/>
     </row>
-    <row r="43" spans="1:13" ht="106" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="31" x14ac:dyDescent="0.2">
       <c r="A43" s="12" t="s">
         <v>74</v>
       </c>
@@ -28134,7 +28134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -28265,15 +28265,15 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="181" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>57</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="70" t="s">
-        <v>304</v>
+      <c r="C5" s="68" t="s">
+        <v>65</v>
       </c>
       <c r="D5" s="49" t="s">
         <v>55</v>
@@ -28402,7 +28402,7 @@
       <c r="B10" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="69" t="s">
         <v>222</v>
       </c>
       <c r="D10" s="48">
@@ -28433,7 +28433,7 @@
       <c r="B11" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="68"/>
+      <c r="C11" s="69"/>
       <c r="D11" s="50" t="s">
         <v>223</v>
       </c>
@@ -29654,7 +29654,7 @@
       <c r="E12" s="3">
         <v>1</v>
       </c>
-      <c r="F12" s="69"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -29670,7 +29670,7 @@
       <c r="E13" s="3">
         <v>1</v>
       </c>
-      <c r="F13" s="69"/>
+      <c r="F13" s="70"/>
     </row>
     <row r="14" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
corrected lung diseases group info
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3F32E1-31AD-444A-8C8C-E24779CDE929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CDBBAB-BF1A-4143-88AB-4E1A76861830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1500" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="6780" yWindow="1500" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="305">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -974,14 +974,6 @@
   </si>
   <si>
     <t>{:title "Disease Group"
-:content 
-[:p  [:b "Cystic Fibrosis (CF):"] " either ‘Cystic Fibrosis’ or ‘Bronchitectasis"]
-[:p [:b "Pulmonary fibrosis (PF):"] " 'Fibrosing Lung Disease'"]
-[:p [:b "Chronic obstructive pulmonary disease (COPD):"] " either ‘alpha-1-antitrypsin deficiency’ or ‘emphysema’"]
-[:p [:b "Other: "] " Patients registered on to the lung waiting list with Primary Disease not listed under any of the above categories." ]}</t>
-  </si>
-  <si>
-    <t>{:title "Disease Group"
 :content [:&lt;&gt;
 [:p  [:b "Cystic Fibrosis (CF):"] " either ‘Cystic Fibrosis’ or ‘Bronchitectasis"]
 [:p [:b "Pulmonary fibrosis (PF):"] " 'Fibrosing Lung Disease'"]
@@ -1696,7 +1688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -2137,7 +2129,7 @@
         <v>122</v>
       </c>
       <c r="H17" s="47" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I17" s="40">
         <v>20</v>
@@ -2394,7 +2386,7 @@
         <v>122</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
@@ -28134,8 +28126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -28265,7 +28257,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="121" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>57</v>
       </c>
@@ -28288,7 +28280,9 @@
         <v>122</v>
       </c>
       <c r="H5" s="13"/>
-      <c r="I5" s="10"/>
+      <c r="I5" s="66" t="s">
+        <v>303</v>
+      </c>
       <c r="J5" s="39">
         <v>40</v>
       </c>
@@ -28296,7 +28290,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="136" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>57</v>
       </c>
@@ -28317,9 +28311,7 @@
         <v>122</v>
       </c>
       <c r="H6" s="10"/>
-      <c r="I6" s="66" t="s">
-        <v>303</v>
-      </c>
+      <c r="I6" s="66"/>
       <c r="J6" s="39">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
really fix FVC and CMV abbreviations
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CDBBAB-BF1A-4143-88AB-4E1A76861830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D943244-47F1-2C43-BE45-40DD22DF9ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6780" yWindow="1500" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="5" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="14960" yWindow="2340" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="306">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -994,6 +994,9 @@
  [:p "If female, TLC = 6.6*(height(cm)/100) - 5.79"]
 ]]}</t>
   </si>
+  <si>
+    <t>:fvcreg</t>
+  </si>
 </sst>
 </file>
 
@@ -1688,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -2502,7 +2505,7 @@
     </row>
     <row r="33" spans="1:13" ht="46" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>173</v>
@@ -2537,7 +2540,7 @@
     </row>
     <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>174</v>
@@ -2560,7 +2563,7 @@
     </row>
     <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>175</v>
@@ -2583,7 +2586,7 @@
     </row>
     <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>176</v>
@@ -28126,8 +28129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I10"/>
+    <sheetView topLeftCell="A26" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -28257,7 +28260,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" spans="1:13" ht="121" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
r names extended to expanded levels
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D943244-47F1-2C43-BE45-40DD22DF9ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A515E82-3FFC-B742-90BE-B215C00E8C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14960" yWindow="2340" windowWidth="32000" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="1520" yWindow="500" windowWidth="46480" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -1691,7 +1691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
       <selection activeCell="A33" sqref="A33:A36"/>
     </sheetView>
   </sheetViews>
@@ -28129,7 +28129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
All model tests passing. Also GT-217
</commit_message>
<xml_diff>
--- a/resources/lung-models-master.xlsx
+++ b/resources/lung-models-master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmp26/clojure/transplants/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A515E82-3FFC-B742-90BE-B215C00E8C15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F36160E-98C0-6B47-A803-0223BF172373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="500" windowWidth="46480" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
+    <workbookView xWindow="2560" yWindow="2320" windowWidth="46480" windowHeight="23500" firstSheet="1" activeTab="9" xr2:uid="{DCE360BB-F5F6-6A48-96D6-61AA4EA0180C}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="18" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="290">
   <si>
     <t>Do not change orange cells</t>
   </si>
@@ -781,31 +781,10 @@
     <t>sex_2</t>
   </si>
   <si>
-    <t>dis_cf</t>
-  </si>
-  <si>
-    <t>dis_oth</t>
-  </si>
-  <si>
-    <t>dis_pf</t>
-  </si>
-  <si>
-    <t>dis_copd</t>
-  </si>
-  <si>
     <t>pred_0</t>
   </si>
   <si>
-    <t>pred_1_14</t>
-  </si>
-  <si>
     <t>pred_15</t>
-  </si>
-  <si>
-    <t>in_hosp_1</t>
-  </si>
-  <si>
-    <t>in_hosp_2</t>
   </si>
   <si>
     <t>nyha_1</t>
@@ -818,12 +797,6 @@
   </si>
   <si>
     <t>nyha_4</t>
-  </si>
-  <si>
-    <t>prev_thor_1</t>
-  </si>
-  <si>
-    <t>prev_thor_2</t>
   </si>
   <si>
     <t>bld_1</t>
@@ -886,93 +859,6 @@
     <t>dsmoke_2</t>
   </si>
   <si>
-    <t>pred_grp_1</t>
-  </si>
-  <si>
-    <t>pred_grp_2</t>
-  </si>
-  <si>
-    <t>pred_grp_3</t>
-  </si>
-  <si>
-    <t>tx_type_1</t>
-  </si>
-  <si>
-    <t>tx_type_2</t>
-  </si>
-  <si>
-    <t>dis_grp_cf</t>
-  </si>
-  <si>
-    <t>dis_grp_oth</t>
-  </si>
-  <si>
-    <t>dis_grp_pf</t>
-  </si>
-  <si>
-    <t>dis_grp_copd</t>
-  </si>
-  <si>
-    <t>rage_grp_1</t>
-  </si>
-  <si>
-    <t>rage_grp_2</t>
-  </si>
-  <si>
-    <t>rage_grp_3</t>
-  </si>
-  <si>
-    <t>rage_grp_4</t>
-  </si>
-  <si>
-    <t>rage_grp_5</t>
-  </si>
-  <si>
-    <t>tlc_mis_1</t>
-  </si>
-  <si>
-    <t>tlc_mis_2</t>
-  </si>
-  <si>
-    <t>tlc_mis_3</t>
-  </si>
-  <si>
-    <t>fvc_grp_1</t>
-  </si>
-  <si>
-    <t>fvc_grp_2</t>
-  </si>
-  <si>
-    <t>fvc_grp_3</t>
-  </si>
-  <si>
-    <t>fvc_grp_4</t>
-  </si>
-  <si>
-    <t>bili_grp_1</t>
-  </si>
-  <si>
-    <t>bili_grp_2</t>
-  </si>
-  <si>
-    <t>bili_grp_3</t>
-  </si>
-  <si>
-    <t>bili_grp_4</t>
-  </si>
-  <si>
-    <t>chol_grp_1</t>
-  </si>
-  <si>
-    <t>chol_grp_2</t>
-  </si>
-  <si>
-    <t>chol_grp_3</t>
-  </si>
-  <si>
-    <t>chol_grp_4</t>
-  </si>
-  <si>
     <t>{:title "Disease Group"
 :content [:&lt;&gt;
 [:p  [:b "Cystic Fibrosis (CF):"] " either ‘Cystic Fibrosis’ or ‘Bronchitectasis"]
@@ -996,6 +882,72 @@
   </si>
   <si>
     <t>:fvcreg</t>
+  </si>
+  <si>
+    <t>inhosp_1</t>
+  </si>
+  <si>
+    <t>inhosp_2</t>
+  </si>
+  <si>
+    <t>dis_CF</t>
+  </si>
+  <si>
+    <t>dis_Other</t>
+  </si>
+  <si>
+    <t>dis_PF</t>
+  </si>
+  <si>
+    <t>dis_COPD</t>
+  </si>
+  <si>
+    <t>pred_1</t>
+  </si>
+  <si>
+    <t>prev_1</t>
+  </si>
+  <si>
+    <t>prev_2</t>
+  </si>
+  <si>
+    <t>type_1</t>
+  </si>
+  <si>
+    <t>type_2</t>
+  </si>
+  <si>
+    <t>tlc_1</t>
+  </si>
+  <si>
+    <t>tlc_2</t>
+  </si>
+  <si>
+    <t>tlc_3</t>
+  </si>
+  <si>
+    <t>bili_1</t>
+  </si>
+  <si>
+    <t>bili_2</t>
+  </si>
+  <si>
+    <t>bili_3</t>
+  </si>
+  <si>
+    <t>bili_4</t>
+  </si>
+  <si>
+    <t>chol_1</t>
+  </si>
+  <si>
+    <t>chol_2</t>
+  </si>
+  <si>
+    <t>chol_3</t>
+  </si>
+  <si>
+    <t>chol_4</t>
   </si>
 </sst>
 </file>
@@ -1691,8 +1643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27012562-A5A0-B84A-8969-5006B4660465}">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="178" zoomScaleNormal="178" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1784,7 +1736,7 @@
         <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="M2" s="8"/>
     </row>
@@ -1812,7 +1764,7 @@
         <v>10</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="M3" s="8"/>
     </row>
@@ -1882,7 +1834,7 @@
         <v>10</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="M6" s="8" t="s">
         <v>75</v>
@@ -1912,7 +1864,7 @@
         <v>10</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>77</v>
@@ -1983,7 +1935,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>274</v>
+        <v>239</v>
       </c>
       <c r="M10" s="8"/>
     </row>
@@ -2007,7 +1959,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M11" s="8"/>
     </row>
@@ -2031,7 +1983,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="M12" s="8"/>
     </row>
@@ -2132,7 +2084,7 @@
         <v>122</v>
       </c>
       <c r="H17" s="47" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="I17" s="40">
         <v>20</v>
@@ -2140,7 +2092,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="M17" s="8"/>
     </row>
@@ -2164,7 +2116,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="M18" s="8"/>
     </row>
@@ -2188,7 +2140,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="M19" s="8"/>
     </row>
@@ -2212,7 +2164,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="M20" s="8"/>
     </row>
@@ -2256,7 +2208,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
       <c r="M22" s="8" t="s">
         <v>78</v>
@@ -2281,7 +2233,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
       <c r="M23" s="8"/>
     </row>
@@ -2305,7 +2257,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
       <c r="M24" s="8"/>
     </row>
@@ -2329,7 +2281,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>286</v>
+        <v>252</v>
       </c>
       <c r="M25" s="8"/>
     </row>
@@ -2353,7 +2305,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>287</v>
+        <v>253</v>
       </c>
       <c r="M26" s="8"/>
     </row>
@@ -2389,7 +2341,7 @@
         <v>122</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>304</v>
+        <v>266</v>
       </c>
       <c r="I28" s="40">
         <v>90</v>
@@ -2401,7 +2353,7 @@
         <v>10</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="M28" s="8"/>
     </row>
@@ -2430,7 +2382,7 @@
         <v>10</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="M29" s="8"/>
     </row>
@@ -2459,7 +2411,7 @@
         <v>10</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="M30" s="8"/>
     </row>
@@ -2505,7 +2457,7 @@
     </row>
     <row r="33" spans="1:13" ht="46" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>173</v>
@@ -2534,13 +2486,13 @@
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>174</v>
@@ -2557,13 +2509,13 @@
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>292</v>
+        <v>255</v>
       </c>
       <c r="M34" s="8"/>
     </row>
     <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>175</v>
@@ -2580,13 +2532,13 @@
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3" t="s">
-        <v>293</v>
+        <v>256</v>
       </c>
       <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
-        <v>305</v>
+        <v>267</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>176</v>
@@ -2603,7 +2555,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>294</v>
+        <v>257</v>
       </c>
       <c r="M36" s="8"/>
     </row>
@@ -2642,7 +2594,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="M38" s="8"/>
     </row>
@@ -2667,7 +2619,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="M39" s="8"/>
     </row>
@@ -2692,7 +2644,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="M40" s="8"/>
     </row>
@@ -2717,7 +2669,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="M41" s="8"/>
     </row>
@@ -2763,7 +2715,7 @@
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="3" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="M43" s="8"/>
     </row>
@@ -2789,7 +2741,7 @@
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="3" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="M44" s="8"/>
     </row>
@@ -2816,7 +2768,7 @@
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="M45" s="8"/>
     </row>
@@ -2843,7 +2795,7 @@
       </c>
       <c r="K46" s="3"/>
       <c r="L46" s="3" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>76</v>
@@ -28129,8 +28081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33804FB4-C3AF-0648-83D5-BC11EB7116B2}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView zoomScale="173" zoomScaleNormal="173" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -28284,13 +28236,13 @@
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="66" t="s">
-        <v>303</v>
+        <v>265</v>
       </c>
       <c r="J5" s="39">
         <v>40</v>
       </c>
       <c r="M5" s="32" t="s">
-        <v>239</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28319,7 +28271,7 @@
         <v>40</v>
       </c>
       <c r="M6" s="32" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28348,7 +28300,7 @@
         <v>40</v>
       </c>
       <c r="M7" s="32" t="s">
-        <v>241</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28377,7 +28329,7 @@
         <v>40</v>
       </c>
       <c r="M8" s="32" t="s">
-        <v>242</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28418,7 +28370,7 @@
         <v>70</v>
       </c>
       <c r="M10" s="32" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28447,7 +28399,7 @@
         <v>70</v>
       </c>
       <c r="M11" s="67" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28476,7 +28428,7 @@
         <v>70</v>
       </c>
       <c r="M12" s="32" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28518,7 +28470,7 @@
         <v>50</v>
       </c>
       <c r="M14" s="67" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28547,7 +28499,7 @@
         <v>50</v>
       </c>
       <c r="M15" s="67" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -28590,7 +28542,7 @@
         <v>60</v>
       </c>
       <c r="M17" s="32" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28619,7 +28571,7 @@
         <v>60</v>
       </c>
       <c r="M18" s="32" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28648,7 +28600,7 @@
         <v>60</v>
       </c>
       <c r="M19" s="32" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28677,7 +28629,7 @@
         <v>60</v>
       </c>
       <c r="M20" s="32" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28722,7 +28674,7 @@
       <c r="K22" s="32"/>
       <c r="L22" s="32"/>
       <c r="M22" s="32" t="s">
-        <v>252</v>
+        <v>275</v>
       </c>
       <c r="N22" s="3"/>
     </row>
@@ -28754,7 +28706,7 @@
       <c r="K23" s="32"/>
       <c r="L23" s="32"/>
       <c r="M23" s="32" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="N23" s="3"/>
     </row>
@@ -28794,7 +28746,7 @@
         <v>30</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28821,7 +28773,7 @@
         <v>30</v>
       </c>
       <c r="M26" s="32" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28848,7 +28800,7 @@
         <v>30</v>
       </c>
       <c r="M27" s="32" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28875,7 +28827,7 @@
         <v>30</v>
       </c>
       <c r="M28" s="32" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28916,7 +28868,7 @@
         <v>10</v>
       </c>
       <c r="M30" s="32" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="16" x14ac:dyDescent="0.2">
@@ -28945,7 +28897,7 @@
         <v>10</v>
       </c>
       <c r="M31" s="32" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -28976,7 +28928,7 @@
       <c r="K32" s="32"/>
       <c r="L32" s="32"/>
       <c r="M32" s="32" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -29007,7 +28959,7 @@
       <c r="K33" s="32"/>
       <c r="L33" s="32"/>
       <c r="M33" s="32" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -29036,7 +28988,7 @@
       <c r="K34" s="32"/>
       <c r="L34" s="32"/>
       <c r="M34" s="32" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -29086,7 +29038,7 @@
         <v>80</v>
       </c>
       <c r="M36" s="32" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29115,7 +29067,7 @@
         <v>80</v>
       </c>
       <c r="M37" s="32" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29144,7 +29096,7 @@
         <v>80</v>
       </c>
       <c r="M38" s="32" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29173,7 +29125,7 @@
         <v>80</v>
       </c>
       <c r="M39" s="32" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:13" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -29219,7 +29171,7 @@
         <v>90</v>
       </c>
       <c r="M41" s="32" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29245,7 +29197,7 @@
         <v>90</v>
       </c>
       <c r="M42" s="32" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="16" x14ac:dyDescent="0.2">
@@ -29271,7 +29223,7 @@
         <v>90</v>
       </c>
       <c r="M43" s="32" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="16" x14ac:dyDescent="0.2">

</xml_diff>